<commit_message>
Ajouter lien vers bulletin officiel sur nom du speaker
</commit_message>
<xml_diff>
--- a/Debats_CDF_EFK.xlsx
+++ b/Debats_CDF_EFK.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -41,25 +41,127 @@
     <t xml:space="preserve">Text</t>
   </si>
   <si>
+    <t xml:space="preserve">364841</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20251202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ständerat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hegglin Peter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M-E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Bundesrat hat uns für 2026 einen Voranschlag mit einem schuldenbremsenkonformen Budget mit einem Handlungsspielraum von 108 Millionen Franken unterbreitet. Dabei darf aber nicht übersehen werden, dass wir 2026 trotzdem ein Finanzierungsdefizit von 845 Millionen Franken haben, zumal sich der Bund dann in diesem Umfang neu verschulden muss. Dieses Ergebnis kommt aber auch nur dank umfangreichen Bereinigungsmassnahmen in den Jahren 2024 und 2025, der guten Einnahmenentwicklung und einer teilwei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Bundesrat hat uns für 2026 einen Voranschlag mit einem schuldenbremsenkonformen Budget mit einem Handlungsspielraum von 108 Millionen Franken unterbreitet. Dabei darf aber nicht übersehen werden, dass wir 2026 trotzdem ein Finanzierungsdefizit von 845 Millionen Franken haben, zumal sich der Bund dann in diesem Umfang neu verschulden muss. Dieses Ergebnis kommt aber auch nur dank umfangreichen Bereinigungsmassnahmen in den Jahren 2024 und 2025, der guten Einnahmenentwicklung und einer teilweisen Verbuchung der Ausgaben zugunsten der Schutzsuchenden aus der Ukraine im ausserordentlichen Haushalt zustande.
+Für die Jahre 2027 und 2028 werden die Vorgaben der Schuldenbremse ebenfalls eingehalten, wenn wir das Entlastungspaket 2027 so umsetzen, wie es uns der Bundesrat vorgeschlagen hat. Leider wird dem nicht so sein, denn nach den Beratungen des EP 27 in unserer Finanzkommission [PAGE 1098] dürfte der finanzielle Fehlbetrag in den Jahren 2027 und 2028 schon über 600 Millionen Franken betragen. Im Jahr 2029 würde der Bereinigungsbedarf bei 2 Milliarden Franken zu liegen kommen. Das sind beträchtliche Summen, die in den kommenden Jahren nicht einfach bei den ungebundenen Ausgaben eingespart werden dürfen. Die zusätzlichen Einnahmen aus dem Kanton Genf sind zwar erfreulich, verbessern die Ergebnisse 2025 und 2026, sind aber für die Jahre 2027 bis 2029 nicht hilfreich. Die Erträge werden dannzumal tiefer ausfallen und den Sanierungsbedarf zusätzlich erhöhen.
+Wie können wir darauf reagieren? Aus meiner Sicht gibt es mehrere Möglichkeiten. 
+1.[NB]Wir müssen schon im Voranschlag 2026 zusätzliche Einsparungen erwirken oder dürfen zumindest nicht mehr Ausgaben beschliessen, um die Lage der Ausgaben nicht zu verschlechtern.
+2.[NB]Es sind auch unkonventionelle Ideen einzubringen und zu prüfen, etwa ob öffentlich-rechtliche Körperschaften, die vor allem oder nur privatwirtschaftliche Dienstleistungen erbringen, der Steuerpflicht unterstellt werden sollen oder ob z.[NB]B. SBB Immobilien einen höheren Anteil zur Finanzierung der Bahninfrastruktur leisten soll.
+3.[NB]Es sind heute auch nicht substanziell höhere Mittel für Rüstungsgüter zu beschliessen. Davor müssten zumindest die strategischen Ziele des Bundesrates zur Sicherheitspolitik bekannt sein.
+4.[NB]Die Schuldenbremse ist nach wie vor unter allen Umständen einzuhalten. Stabile Finanzen sind ein wichtiger Pfeiler der Sicherheitspolitik. Wenn alle Massnahmen letztlich nicht reichen, müsste zumindest das Volk darüber befinden können, ob es Rüstungsbeschaffungen als notwendig erachtet oder bereit ist, dafür mehr Steuern zu bezahlen.
+Gerne gehe ich auf einzelne Aspekte näher ein. Im Budgetjahr 2026 haben wir eine Ausgabensteigerung von 5,2 Prozent. Über die ganze Finanzplanperiode sind es immer noch 3,1 Prozent, und dies erst noch unter Einhaltung des Entlastungsprogramms 2027 und gegenüber den Zahlen des Voranschlages 2025. Haupttreiber für diese Kostensteigerung sind die Bereiche Bildung und Forschung, soziale Wohlfahrt und Sicherheit. Diese haben Wachstumsraten zwischen 5 und 8 Prozent.
+Auf der Einnahmenseite sollen die Fiskalerträge für das nächste Jahr ebenfalls um 5 Prozent steigen, über die kommenden vier Jahre immer noch um 3,2 Prozent. Angesichts der wirtschaftlichen Situation in unseren Nachbarstaaten, aber auch auf den Absatzmärkten, angesichts der wirtschaftlichen Konflikte mit anderen Ländern, vor allem auch in Übersee, sind das ambitionierte Annahmen. Es wäre aber vermessen, wenn das Parlament die Schätzungen des Eidgenössischen Finanzdepartements und der Eidgenössischen Steuerverwaltung verändern würde. Ich glaube, sie haben in der Vergangenheit gezeigt, dass diese doch ziemlich genau sind. Ich gehe auch davon aus, dass die Kenngrössen, die aufgeführt sind, im nächsten Jahr erreicht werden können. Schwieriger dürfte es in den Finanzdebatten der späteren Jahre werden. Vorsorgen ist deshalb angesagt, um dann nicht bei den ungebundenen Ausgaben übermässig korrigieren zu müssen.
+Ich beziehe mich heute deshalb vor allem auch auf den Eigenbereich. Das sind vornehmlich Personal- und Sachkosten. Über das Entlastungspaket 2027 plant der Bundesrat, im Eigenbereich 300 Millionen Franken einzusparen. Das ist respektabel und verdient Unterstützung. Trotzdem soll es erlaubt sein, im Budgetprozess zusätzliche Ausgabenpositionen zu hinterfragen. Dazu gehört sicher die Anzahl der Beschäftigten bei der Verwaltung; diese steigt unaufhörlich. Im Jahr 2015 lag sie noch bei 36[NB]522. Sie soll von diesem Jahr auf das nächste Jahr um weitere 378 Vollzeitstellen auf 39[NB]453 anwachsen, allein beim VBS um 232 Stellen. Bald werden wir die vierzigtausendste Vollzeitstelle bei der Verwaltung feiern können.
+Wir sind an dieser Entwicklung nicht ganz unschuldig. Mit Beschlüssen für laufend neue Aufgaben für den Bund sind wir einerseits Treiber dieser Entwicklung, andererseits versuchen wir, durch die Digitalisierung Effizienzgewinne zu realisieren. Leider aber bleiben die Effizienzsteigerungen in einem bescheidenen Rahmen. Das Projekt Dazit ist diesbezüglich eine erwähnenswerte Ausnahme. Dieses Projekt spielte über 300 Personalstellen frei. 
+Wie können wir nun korrigierend eingreifen? Mit dem Neuen Führungsmodell des Bundes beschliessen wir nicht über Personalstellen, sondern nur über die Budgethöhe. Der Bundesrat wünscht keine Kürzungen nach der Rasenmähermethode, sondern erwartet konkrete Hinweise von uns. Die[NB]Mehrheit[NB]der[NB]Kommission schlägt solche Massnahmen vor. 
+So will sie erstens beim Bundesverwaltungsgericht das Wachstum des Funktionsaufwandes - das sind Personalstellen und Sachaufwände - auf 2 Millionen Franken begrenzen. Die Erwartung, die ich als Kommissionsmitglied auch teile, ist, dass das Bundesverwaltungsgericht seine drängenden organisatorischen Probleme löst, seine Effizienz steigert und die Abteilungen sich bei der Pendenzenlast gegenseitig unterstützen. So wurde es auch in einem anonymen Schreiben aus dieser Institution an die Kommissionsmitglieder verlangt. 
+Eine zweite Kürzung betrifft den Kommunikationsbereich. Die Massnahme soll im Verhältnis zu den Kommunikationsaufwänden umgesetzt werden. Gemäss der vorliegenden Jahresrechnung 2024 gab es in der Verwaltung allein für die Öffentlichkeitsarbeit über 420 Vollzeitstellen, was Kosten von über 100 Millionen Franken verursachte. Mit einem Absenkpfad sollen diese Stellen und die Aufwände schrittweise reduziert werden.
+Das sind kleine Versuche, das Personalstellenwachstum zu bremsen. Die Finanzkommission und auch ich sind aber bereit, bei Bedarf zusätzliche Stellen zuzulassen, so zum Beispiel beim Fedpol. Für dieses ist ein Bericht der Eidgenössischen Finanzkontrolle vorliegend, der besagt, dass dort mehr Personal notwendig sei. Dort sind 63 zusätzliche Stellen beantragt, die nicht infrage gestellt sind.
+Ein weiterer Bereich im Eigenbereich ist die Teuerung. Eingestellt sind 0,5 Prozent Teuerungsausgleich, das entspricht 34 Millionen Franken. Während der Debatte, während der Arbeit in der Kommission sank die Teuerungsrate immer mehr, auf 0,3, auf 0,2 bis auf aktuell 0,1 Prozent. Auch in Anbetracht der guten Besoldungshöhe, die verschiedene Gutachten belegen, ist es vertretbar, auf einen Teuerungsausgleich, eine generelle Lohnerhöhung, zu verzichten. Eine individuelle Lohnentwicklung ist aber unabhängig davon möglich, und diese möchte ich explizit nicht infrage stellen. Das soll nach wie vor möglich sein.
+Mit einer Anpassung der Bundespersonalverordnung hat der Bundesrat auf Anfang 2026 ein neues Lohnmodell eingeführt und dabei auch den Ortszuschlag integriert. Als Finanzkommission waren wir, abgesehen von einer Information im November 2022, nicht eingebunden. Wir haben über Umwege bei den Budgetvorbesprechungen davon erfahren. Nach den Kompetenzregelungen wäre auch die SPK unseres Rates zuständig gewesen. Wie ich aber informiert bin, liess auch sie sich nicht konsultieren, wahrscheinlich war sie über den Vorgang gar nicht informiert. Es besteht in diesem Bereich auch keine Konsultationspflicht des Bundesrates gegenüber den eidgenössischen Räten.
+Gemäss den Aussagen des Eidgenössischen Personalamtes sollen aus den neuen Personalregelungen keine höheren Kosten entstehen. Das kann ich aber schwerlich nachvollziehen: Einerseits gibt es höhere Einstiegslöhne, ein anderes Lohnband, andererseits haben uns die eidgenössischen Gerichte in den Budgetbesprechungen darauf hingewiesen, dass sie die Lohnsteigerungen, die ab Lohnklasse 33 rund 10 Prozent betragen können, ab 2027 nicht werden kompensieren können. Es braucht in diesem Bereich, ich glaube, vor allem seitens der eidgenössischen Gerichte, also noch Korrekturmassnahmen. In Zeiten des Sparprogramms hätte ich hier mehr Sensibilität oder auch einen Einbezug unserer Kommissionen gewünscht.
+Das waren jetzt zwei Schienen, auf welchen man, meine ich, korrigieren kann, sogar korrigieren soll: einerseits das Stellenwachstum - aber über das Budget, nicht über die Anzahl Stellen -, andererseits die Teuerungszulage. [PAGE 1099] 
+Nicht unerwähnt lassen möchte ich bei den Eigenausgaben noch die Spesen - diese wachsen ja auch beträchtlich. 2021 waren es noch 98 Millionen Franken, im vergangenen Jahr waren es über die gesamte Verwaltung hinweg 132 Millionen Franken. Ich meine, auch in diesem Bereich wäre es möglich, gewisse Einsparungen vorzunehmen - ohne eine konkrete Massnahme anzustossen.
+Damit komme ich zum Schluss. Ich glaube, insgesamt können wir einen guten Voranschlag beraten. Ich danke dem Bundesrat und der Verwaltung für die grosse Vorarbeit und bitte Sie, jeweils der Mehrheit Ihrer Kommission oder dem Bundesrat zu folgen und dem Voranschlag in der Gesamtabstimmung zuzustimmen.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">365062</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binder-Keller Marianne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Einschätzung, dass das Fedpol mehr Mittel braucht, ist nicht aus der Luft gegriffen. Der Bundesrat hat die Ressourcensituation selbst analysiert, dies aufgrund eines Postulates, wie das auch der Vertreter der Minderheit II erwähnt hat. Die EFK überprüfte das dann und kam zum klaren Schluss, dass das Fedpol seinen Auftrag mit den aktuellen Mitteln nicht erfüllen kann.[NB]Es[NB]wurden[NB]auch strukturelle Defizite festgestellt - auch das wurde erwähnt -, die analysiert und angegangen worden si</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Einschätzung, dass das Fedpol mehr Mittel braucht, ist nicht aus der Luft gegriffen. Der Bundesrat hat die Ressourcensituation selbst analysiert, dies aufgrund eines Postulates, wie das auch der Vertreter der Minderheit II erwähnt hat. Die EFK überprüfte das dann und kam zum klaren Schluss, dass das Fedpol seinen Auftrag mit den aktuellen Mitteln nicht erfüllen kann.[NB]Es[NB]wurden[NB]auch strukturelle Defizite festgestellt - auch das wurde erwähnt -, die analysiert und angegangen worden sind.
+Nichtsdestotrotz braucht das Fedpol mehr Mittel. Die Sicherheitslage eskaliert generell. Wir haben einen Krieg in Europa, darauf muss ich ja wohl nicht weiter eingehen. Die Eidgenössische Finanzkontrolle kam klar zum Schluss, dass die personellen Ressourcen in den Bereichen Terrorismus, organisierte Kriminalität, Wirtschaftskriminalität und Cyberkriminalität nicht ausreichen. Das führt dazu, dass Strafverfahren verzögert oder gar nicht eröffnet werden, und unter diesen Umständen verstehe ich eine Kürzung wirklich nicht. Das hat massive Auswirkungen auf die innere Sicherheit, und dass diese geschützt werden muss, steht klar in Artikel 2 der Bundesverfassung, dem Zweckartikel.
+Als Präsidentin der Subkommission Gerichte/BA habe ich mir die Problematik vom Bundesanwalt und von der Aufsichtsbehörde über die Bundesanwaltschaft eingehend schildern lassen; Kollege Zopfi hat mich darauf angesprochen. Ebenso haben wir die Probleme in der Sicherheitspolitischen Kommission analysiert.
+Ich erachte eine Erhöhung der Mittel aufgrund der allgemein eskalierenden sicherheitspolitischen Lage für mehr als gerechtfertigt. Es ist eine Zeitfrage. Die Zeit läuft uns davon, was die Finanzierung der Armee und die Verteidigungsfähigkeit betrifft, und das ist sträflich. Die Zeit läuft uns aber auch davon, was die innere Sicherheit betrifft, und diese beiden Anliegen sind miteinander verzahnt. Wir können in solch eskalierenden Zeiten nicht zu einer internationalen Drehscheibe werden.
+Deshalb werde ich die Minderheit II (Zopfi) unterstützen. [PAGE 1113] 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">365066</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zopfi Mathias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Antrag meiner Minderheit II dürfte vielen von Ihnen bekannt vorkommen. Diejenigen von Ihnen, die in der GPK sind, haben sich damit schon beschäftigt, und diejenigen von Ihnen, die in der SiK sind, haben sich auch bereits mit dieser Problematik beschäftigt. Die Minderheit II will mit ihrem Konzept, das sich dann auch im Finanzplan niederschlägt, jährlich zehn bis zwanzig Stellen beim Fedpol aufbauen, insbesondere im Bereich der Bundeskriminalpolizei. 
+Ich habe Ihnen gesagt, dass sich viele vo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Antrag meiner Minderheit II dürfte vielen von Ihnen bekannt vorkommen. Diejenigen von Ihnen, die in der GPK sind, haben sich damit schon beschäftigt, und diejenigen von Ihnen, die in der SiK sind, haben sich auch bereits mit dieser Problematik beschäftigt. Die Minderheit II will mit ihrem Konzept, das sich dann auch im Finanzplan niederschlägt, jährlich zehn bis zwanzig Stellen beim Fedpol aufbauen, insbesondere im Bereich der Bundeskriminalpolizei. 
+Ich habe Ihnen gesagt, dass sich viele von Ihnen bereits damit auseinandergesetzt haben. Ich sage nur so viel: Bei der Anhörung in der Kommission und an verschiedenen anderen Orten hörte ich immer wieder, dass wir uns in Richtung von Ländern mit sehr hoher organisierter Kriminalität bewegen. Ich nenne ein Land, das ein enormes Problem hat. Sie denken vielleicht an Italien, Sie denken vielleicht an Albanien. Nein, ich nenne Schweden als Beispiel. Schweden ist heute im Bereich der organisierten Kriminalität absolut problematisch unterwegs. Wenn ich höre, dass wir auch in der Schweiz in diese Richtung unterwegs sind und es sich um Jahre, vielleicht sogar nur um Monate handelt, bis sich solche Entwicklungen auch bei uns ergeben, dann lässt mich das aufhorchen. 
+Ich höre, dass wir vierzig Fälle nicht behandeln können, weil die Ressourcen bei der Bundeskriminalpolizei schlicht und einfach fehlen. Das lässt mich aufhorchen. Bei diesen vierzig Fällen handelt es sich nicht etwa um Bagatellfälle. Es sind Fälle organisierter Kriminalität, das müssen Sie einfach sehen. Es geht nicht um ein gestohlenes Portemonnaie oder so etwas. 
+Letztlich geht es darum, dass das Fedpol eine wichtige Aufgabe für die Sicherheit unseres Landes übernimmt, insbesondere, um unser Land vor organisierter Kriminalität zu bewahren oder möglichst gut zu schützen. Dass es dabei auch um Terrorismus und um Terrorismusfinanzierung usw. geht, wissen Sie bereits. 
+Vor Kurzem habe ich ein sehr interessantes Interview mit einem Spezialisten gelesen. Ich weiss nicht mehr, ob es in der "NZZ" oder im "Tages-Anzeiger" war. Er hat bestätigt, dass sich die organisierte Kriminalität, die wir vielleicht immer noch in Süditalien vermuten, in ganz Europa massiv ausgebreitet hat. Wir haben heute an vielen Orten Zustände, die nichts mehr mit einer heilen Welt zu tun haben oder mit Aussagen wie "Bei uns ist es ja nicht so schlimm" erklärt werden können. 
+Ich sage Ihnen das, und Sie hören mir einigermassen aufmerksam zu. Aber ich kann Ihnen sagen: Nicht nur ich sage Ihnen das. Ich habe bereits erwähnt, dass diejenigen von Ihnen, die in der GPK sind, sich damit auseinandergesetzt haben. Die GPK hat ein Schreiben an die Finanzkommission verfasst. Ich zitiere daraus nur einen Satz: "Auch die GPK kommt ebenfalls zum Schluss, dass die personellen Ressourcen der BKP rasch erhöht werden müssen." Die GPK, die sich mit der Sache auseinandergesetzt hat, ist offenbar zum Schluss gekommen, dass wir rasch etwas tun müssen. Auch in der generellen Stellungnahme der Bundesanwaltschaft steht zum Beispiel: "Der Mangel an Ermittlerressourcen bei der BKP ist eine allseits unbestrittene Erkenntnis." 
+Und was sagt die Eidgenössische Finanzkontrolle? Sie ist ihres Zeichens nicht unbedingt dafür bekannt, ausufernde Stellenbegehren gutzuheissen oder den Ausbau des Staates zu forcieren. Vielmehr nimmt sie auch für die Finanzkommission die Rolle ein, genau hinzuschauen und eher kritisch zu sein. Auch die EFK kommt in ihrem Bericht zum Schluss, dass es beim Fedpol neben Effizienzmassnahmen - die notabene vom Fedpol schon teilweise umgesetzt werden; deren Potenzial wurde bestätigt - mehr Ressourcen für die Ermittlung braucht. Die EFK sieht das also genau gleich. [PAGE 1112] 
+Zuletzt spreche ich noch diejenigen von Ihnen an, die in der SiK sitzen. Sie haben ohne Gegenstimme und mit klarer Mehrheit eine Motion beschlossen. Diese wird am 11.[NB]Dezember 2025 in diesem Rat behandelt. Die Motion fordert eigentlich nichts anderes als das, was meine Minderheit[NB]II ebenfalls fordert. Wir können schon noch zuwarten, oder wir können heute irgendwas entscheiden. Am 11.[NB]Dezember kann uns dann die Berichterstatterin - es ist die ehemalige Präsidentin der SiK, Kollegin Andrea Gmür-Schönenberger - erläutern, weshalb es wichtig ist, dass wir diese Motion wie die SiK möglichst ohne Gegenstimme annehmen. Aber dann ist es mit dem Voranschlag schon gelaufen, dann haben wir dieses Thema hier schon behandelt. Sie merken es, ich spreche die Mitglieder der SiK an, und ich habe es ihnen bereits gesagt: Die Musik spielt beim Voranschlag, die Musik spielt genau jetzt. 
+Natürlich ist es wichtig, dass wir die Finanzen im Griff behalten. Da stimme ich meinem Vorredner zu. Es ist wichtig, dass wir nicht einfach ausufernde Stellenbegehren gutheissen, nur weil ein bisschen Druck gemacht wird. Aber hier haben wir es mit einem Problem zu tun. Sie haben es von allen Seiten gehört.
+Jetzt könnten Sie, wenn Sie den Entwurf des Bundesrates und den Antrag der Minderheit I anschauen, zur Auffassung kommen, dass der Bundesrat ja bereits etwas unternimmt, denn die Minderheit I (Mühlemann) will hier kürzen. Dazu müssen Sie aber berücksichtigen: Diese 51 Stellen, die gemäss Antrag des Bundesrates geschaffen werden sollen, dienen nicht dem Aufbau der Bundeskriminalpolizei, um dieser erhöhten Bedrohungs- und Sicherheitslage Herr zu werden. Sondern 44 dieser 51 Stellen werden benötigt, um Projekte, die wir bewilligt haben - zum Beispiel die Schengen-Weiterentwicklungen, die Weiterentwicklung des automatisierten Fingerabdrucksystems usw. -, umzusetzen. Mit dem Antrag des Bundesrates setzen Sie also gerade einmal das um, was wir beschlossen haben, Sie schaffen aber keine zusätzlichen Ressourcen bei der Bundeskriminalpolizei für die Themen, die ich soeben erwähnt habe. Die übrigen 7 dieser 51 Stellen werden benötigt, um am Verwaltungszentrum Guisanplatz, wo ein neues Gebäude in Betrieb genommen worden ist, die Loge zu betreiben. Das wird dann vom VBS wieder rückerstattet und ist in dem Sinn also kostenneutral. Aber Sie werden sich auch vorstellen können, dass die 7[NB]Personen,[NB]die[NB]die[NB]Loge[NB]betreiben, nicht unbedingt der Bundeskriminalpolizei zur Bekämpfung der organisierten Kriminalität ausserhalb des Sichtradius der Loge zur Verfügung stehen. 
+Damit will ich Ihnen sagen: Die Variante Bundesrat bedeutet im Bereich der Bundeskriminalpolizei überhaupt keine Aufstockung, sondern Bewahrung des Status quo. Wenn Sie berücksichtigen wollen, was Ihnen die GPK, die SiK und alle anderen empfehlen, dann müssen Sie hier mit der Minderheit II stimmen. 
+Wenn Sie mit der Minderheit I stimmen, wovon ich Ihnen trotz klarer Sympathie natürlich wärmstens abrate, dann werden Sie die zusätzlichen Stellen, die für die Umsetzung dieser Projekte notwendig sind, beim laufenden Betrieb bei der Bundeskriminalpolizei und an anderen Orten kompensieren müssen, was dazu führt, dass im Resultat sogar weniger Ressourcen zur Verfügung stehen werden, um der genannten Herausforderungen Herr zu werden. 
+Wenn man jetzt die Zahl der Meldungen ins Spiel bringt und sagt, es werde halt zu viel gemeldet, dann kommt mir das folgendermassen vor: Es gibt eine Sicherheitslage, in der sich die Kriminalität erhöht, in der die Leute nach mehr Polizei rufen und in der das Sicherheitsgefühl sinkt. Sie sehen, dass es ein Problem gibt, aber anstatt mehr Polizei anzustellen, sagen Sie zu den Menschen: Gebt halt weniger Strafanzeigen auf, dann haben wir das Problem gelöst. So schaffen Sie einfach eine Dunkelziffer, ein Dunkelfeld. 
+Ich sage damit nicht, dass der Effekt, den Kollege Mühlemann beschrieben hat, nicht ein Stück weit eintreten kann. Aber die Tatsache ist, dass wir es hier mit organisierter Kriminalität zu tun haben, und daher ist es wichtig, dass wir nicht in die Vogel-Strauss-Politik verfallen und sagen: Gebt halt weniger Anzeigen auf, ihr macht zu viele Anzeigen; wenn wir weniger davon wissen, dann wird es weniger schlimm sein. Das wäre das Prinzip "Augen zu und durch", und dazu rate ich Ihnen im Namen unserer Sicherheit nicht.
+Ich bitte Sie deshalb, mit der Minderheit II zu stimmen und zu berücksichtigen, was bereits die GPK, die SiK und viele andere empfehlen und empfohlen haben, und hier entsprechend konsequent zu sein. Dann können Sie am 11.[NB]Dezember auch der erwähnten Motion zustimmen.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">365070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wenn man Kollege Zopfi zuhört, könnte man meinen, wir hätten in den vergangenen Jahren zu wenig oder nichts getan. Das stimmt einfach nicht. Betrachten Sie die Personalstellen beim Fedpol: Im Jahr 2019 lag der Personalbestand bei 899 Vollzeitstellen. Im Jahr 2026 soll er auf 1060 Stellen aufgestockt werden. Im Jahr 2026 sollen im Vergleich zum Vorjahr 63 Stellen hinzukommen. Die Frage ist, wo sie eingesetzt werden. Aber wir beschliessen ja über das Gesamtbudget. Der Bundesrat hat die Verantwortu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wenn man Kollege Zopfi zuhört, könnte man meinen, wir hätten in den vergangenen Jahren zu wenig oder nichts getan. Das stimmt einfach nicht. Betrachten Sie die Personalstellen beim Fedpol: Im Jahr 2019 lag der Personalbestand bei 899 Vollzeitstellen. Im Jahr 2026 soll er auf 1060 Stellen aufgestockt werden. Im Jahr 2026 sollen im Vergleich zum Vorjahr 63 Stellen hinzukommen. Die Frage ist, wo sie eingesetzt werden. Aber wir beschliessen ja über das Gesamtbudget. Der Bundesrat hat die Verantwortung und die Aufgabe, die zur Verfügung gestellten Mittel sachgerecht einzusetzen.
+Ich habe gesagt, dass 63 zusätzliche Stellen vorgesehen sind - das entspricht einem Wachstum von 6,3 Prozent. Das ist ein sehr viel stärkeres Wachstum als in der übrigen Bundesverwaltung. Über den Zeithorizont von 2019 bis 2026 lag das Personalwachstum beim Fedpol bei 2,9 Prozent im Jahr, also bei fast 3 Prozent. In der Bundesverwaltung lag es im gleichen Zeitraum bei 0,8 Prozent im Jahr. Das Fedpol wächst also im Vergleich zur übrigen Bundesverwaltung überdurchschnittlich. Von daher kommen wir den Empfehlungen der EFK nach, und wir kommen mit dem Antrag der Mehrheit Ihrer Finanzkommission auch dem Anliegen und[NB]dem[NB]Auftrag in diesem Sektor nach. Denn die Sicherheit und die Bekämpfung der kriminellen Organisationen sind wichtig.
+Ich empfehle Ihnen also, der Mehrheit Ihrer Kommission zu folgen und damit, wie gesagt, den Rahmen dafür zu schaffen, dass 63 zusätzliche Stellen geschaffen werden können.
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">365198</t>
   </si>
   <si>
-    <t xml:space="preserve">20251202</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conseil des Etats</t>
-  </si>
-  <si>
     <t xml:space="preserve">Engler Stefan</t>
   </si>
   <si>
-    <t xml:space="preserve">M-E</t>
-  </si>
-  <si>
     <t xml:space="preserve">GR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FR</t>
   </si>
   <si>
     <t xml:space="preserve">Angenommen - Adopté
@@ -585,97 +687,32 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">365062</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ständerat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Binder-Keller Marianne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Einschätzung, dass das Fedpol mehr Mittel braucht, ist nicht aus der Luft gegriffen. Der Bundesrat hat die Ressourcensituation selbst analysiert, dies aufgrund eines Postulates, wie das auch der Vertreter der Minderheit II erwähnt hat. Die EFK überprüfte das dann und kam zum klaren Schluss, dass das Fedpol seinen Auftrag mit den aktuellen Mitteln nicht erfüllen kann.[NB]Es[NB]wurden[NB]auch strukturelle Defizite festgestellt - auch das wurde erwähnt -, die analysiert und angegangen worden si</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Einschätzung, dass das Fedpol mehr Mittel braucht, ist nicht aus der Luft gegriffen. Der Bundesrat hat die Ressourcensituation selbst analysiert, dies aufgrund eines Postulates, wie das auch der Vertreter der Minderheit II erwähnt hat. Die EFK überprüfte das dann und kam zum klaren Schluss, dass das Fedpol seinen Auftrag mit den aktuellen Mitteln nicht erfüllen kann.[NB]Es[NB]wurden[NB]auch strukturelle Defizite festgestellt - auch das wurde erwähnt -, die analysiert und angegangen worden sind.
-Nichtsdestotrotz braucht das Fedpol mehr Mittel. Die Sicherheitslage eskaliert generell. Wir haben einen Krieg in Europa, darauf muss ich ja wohl nicht weiter eingehen. Die Eidgenössische Finanzkontrolle kam klar zum Schluss, dass die personellen Ressourcen in den Bereichen Terrorismus, organisierte Kriminalität, Wirtschaftskriminalität und Cyberkriminalität nicht ausreichen. Das führt dazu, dass Strafverfahren verzögert oder gar nicht eröffnet werden, und unter diesen Umständen verstehe ich eine Kürzung wirklich nicht. Das hat massive Auswirkungen auf die innere Sicherheit, und dass diese geschützt werden muss, steht klar in Artikel 2 der Bundesverfassung, dem Zweckartikel.
-Als Präsidentin der Subkommission Gerichte/BA habe ich mir die Problematik vom Bundesanwalt und von der Aufsichtsbehörde über die Bundesanwaltschaft eingehend schildern lassen; Kollege Zopfi hat mich darauf angesprochen. Ebenso haben wir die Probleme in der Sicherheitspolitischen Kommission analysiert.
-Ich erachte eine Erhöhung der Mittel aufgrund der allgemein eskalierenden sicherheitspolitischen Lage für mehr als gerechtfertigt. Es ist eine Zeitfrage. Die Zeit läuft uns davon, was die Finanzierung der Armee und die Verteidigungsfähigkeit betrifft, und das ist sträflich. Die Zeit läuft uns aber auch davon, was die innere Sicherheit betrifft, und diese beiden Anliegen sind miteinander verzahnt. Wir können in solch eskalierenden Zeiten nicht zu einer internationalen Drehscheibe werden.
-Deshalb werde ich die Minderheit II (Zopfi) unterstützen. [PAGE 1113] 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">365066</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zopfi Mathias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Der Antrag meiner Minderheit II dürfte vielen von Ihnen bekannt vorkommen. Diejenigen von Ihnen, die in der GPK sind, haben sich damit schon beschäftigt, und diejenigen von Ihnen, die in der SiK sind, haben sich auch bereits mit dieser Problematik beschäftigt. Die Minderheit II will mit ihrem Konzept, das sich dann auch im Finanzplan niederschlägt, jährlich zehn bis zwanzig Stellen beim Fedpol aufbauen, insbesondere im Bereich der Bundeskriminalpolizei. 
-Ich habe Ihnen gesagt, dass sich viele vo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Der Antrag meiner Minderheit II dürfte vielen von Ihnen bekannt vorkommen. Diejenigen von Ihnen, die in der GPK sind, haben sich damit schon beschäftigt, und diejenigen von Ihnen, die in der SiK sind, haben sich auch bereits mit dieser Problematik beschäftigt. Die Minderheit II will mit ihrem Konzept, das sich dann auch im Finanzplan niederschlägt, jährlich zehn bis zwanzig Stellen beim Fedpol aufbauen, insbesondere im Bereich der Bundeskriminalpolizei. 
-Ich habe Ihnen gesagt, dass sich viele von Ihnen bereits damit auseinandergesetzt haben. Ich sage nur so viel: Bei der Anhörung in der Kommission und an verschiedenen anderen Orten hörte ich immer wieder, dass wir uns in Richtung von Ländern mit sehr hoher organisierter Kriminalität bewegen. Ich nenne ein Land, das ein enormes Problem hat. Sie denken vielleicht an Italien, Sie denken vielleicht an Albanien. Nein, ich nenne Schweden als Beispiel. Schweden ist heute im Bereich der organisierten Kriminalität absolut problematisch unterwegs. Wenn ich höre, dass wir auch in der Schweiz in diese Richtung unterwegs sind und es sich um Jahre, vielleicht sogar nur um Monate handelt, bis sich solche Entwicklungen auch bei uns ergeben, dann lässt mich das aufhorchen. 
-Ich höre, dass wir vierzig Fälle nicht behandeln können, weil die Ressourcen bei der Bundeskriminalpolizei schlicht und einfach fehlen. Das lässt mich aufhorchen. Bei diesen vierzig Fällen handelt es sich nicht etwa um Bagatellfälle. Es sind Fälle organisierter Kriminalität, das müssen Sie einfach sehen. Es geht nicht um ein gestohlenes Portemonnaie oder so etwas. 
-Letztlich geht es darum, dass das Fedpol eine wichtige Aufgabe für die Sicherheit unseres Landes übernimmt, insbesondere, um unser Land vor organisierter Kriminalität zu bewahren oder möglichst gut zu schützen. Dass es dabei auch um Terrorismus und um Terrorismusfinanzierung usw. geht, wissen Sie bereits. 
-Vor Kurzem habe ich ein sehr interessantes Interview mit einem Spezialisten gelesen. Ich weiss nicht mehr, ob es in der "NZZ" oder im "Tages-Anzeiger" war. Er hat bestätigt, dass sich die organisierte Kriminalität, die wir vielleicht immer noch in Süditalien vermuten, in ganz Europa massiv ausgebreitet hat. Wir haben heute an vielen Orten Zustände, die nichts mehr mit einer heilen Welt zu tun haben oder mit Aussagen wie "Bei uns ist es ja nicht so schlimm" erklärt werden können. 
-Ich sage Ihnen das, und Sie hören mir einigermassen aufmerksam zu. Aber ich kann Ihnen sagen: Nicht nur ich sage Ihnen das. Ich habe bereits erwähnt, dass diejenigen von Ihnen, die in der GPK sind, sich damit auseinandergesetzt haben. Die GPK hat ein Schreiben an die Finanzkommission verfasst. Ich zitiere daraus nur einen Satz: "Auch die GPK kommt ebenfalls zum Schluss, dass die personellen Ressourcen der BKP rasch erhöht werden müssen." Die GPK, die sich mit der Sache auseinandergesetzt hat, ist offenbar zum Schluss gekommen, dass wir rasch etwas tun müssen. Auch in der generellen Stellungnahme der Bundesanwaltschaft steht zum Beispiel: "Der Mangel an Ermittlerressourcen bei der BKP ist eine allseits unbestrittene Erkenntnis." 
-Und was sagt die Eidgenössische Finanzkontrolle? Sie ist ihres Zeichens nicht unbedingt dafür bekannt, ausufernde Stellenbegehren gutzuheissen oder den Ausbau des Staates zu forcieren. Vielmehr nimmt sie auch für die Finanzkommission die Rolle ein, genau hinzuschauen und eher kritisch zu sein. Auch die EFK kommt in ihrem Bericht zum Schluss, dass es beim Fedpol neben Effizienzmassnahmen - die notabene vom Fedpol schon teilweise umgesetzt werden; deren Potenzial wurde bestätigt - mehr Ressourcen für die Ermittlung braucht. Die EFK sieht das also genau gleich. [PAGE 1112] 
-Zuletzt spreche ich noch diejenigen von Ihnen an, die in der SiK sitzen. Sie haben ohne Gegenstimme und mit klarer Mehrheit eine Motion beschlossen. Diese wird am 11.[NB]Dezember 2025 in diesem Rat behandelt. Die Motion fordert eigentlich nichts anderes als das, was meine Minderheit[NB]II ebenfalls fordert. Wir können schon noch zuwarten, oder wir können heute irgendwas entscheiden. Am 11.[NB]Dezember kann uns dann die Berichterstatterin - es ist die ehemalige Präsidentin der SiK, Kollegin Andrea Gmür-Schönenberger - erläutern, weshalb es wichtig ist, dass wir diese Motion wie die SiK möglichst ohne Gegenstimme annehmen. Aber dann ist es mit dem Voranschlag schon gelaufen, dann haben wir dieses Thema hier schon behandelt. Sie merken es, ich spreche die Mitglieder der SiK an, und ich habe es ihnen bereits gesagt: Die Musik spielt beim Voranschlag, die Musik spielt genau jetzt. 
-Natürlich ist es wichtig, dass wir die Finanzen im Griff behalten. Da stimme ich meinem Vorredner zu. Es ist wichtig, dass wir nicht einfach ausufernde Stellenbegehren gutheissen, nur weil ein bisschen Druck gemacht wird. Aber hier haben wir es mit einem Problem zu tun. Sie haben es von allen Seiten gehört.
-Jetzt könnten Sie, wenn Sie den Entwurf des Bundesrates und den Antrag der Minderheit I anschauen, zur Auffassung kommen, dass der Bundesrat ja bereits etwas unternimmt, denn die Minderheit I (Mühlemann) will hier kürzen. Dazu müssen Sie aber berücksichtigen: Diese 51 Stellen, die gemäss Antrag des Bundesrates geschaffen werden sollen, dienen nicht dem Aufbau der Bundeskriminalpolizei, um dieser erhöhten Bedrohungs- und Sicherheitslage Herr zu werden. Sondern 44 dieser 51 Stellen werden benötigt, um Projekte, die wir bewilligt haben - zum Beispiel die Schengen-Weiterentwicklungen, die Weiterentwicklung des automatisierten Fingerabdrucksystems usw. -, umzusetzen. Mit dem Antrag des Bundesrates setzen Sie also gerade einmal das um, was wir beschlossen haben, Sie schaffen aber keine zusätzlichen Ressourcen bei der Bundeskriminalpolizei für die Themen, die ich soeben erwähnt habe. Die übrigen 7 dieser 51 Stellen werden benötigt, um am Verwaltungszentrum Guisanplatz, wo ein neues Gebäude in Betrieb genommen worden ist, die Loge zu betreiben. Das wird dann vom VBS wieder rückerstattet und ist in dem Sinn also kostenneutral. Aber Sie werden sich auch vorstellen können, dass die 7[NB]Personen,[NB]die[NB]die[NB]Loge[NB]betreiben, nicht unbedingt der Bundeskriminalpolizei zur Bekämpfung der organisierten Kriminalität ausserhalb des Sichtradius der Loge zur Verfügung stehen. 
-Damit will ich Ihnen sagen: Die Variante Bundesrat bedeutet im Bereich der Bundeskriminalpolizei überhaupt keine Aufstockung, sondern Bewahrung des Status quo. Wenn Sie berücksichtigen wollen, was Ihnen die GPK, die SiK und alle anderen empfehlen, dann müssen Sie hier mit der Minderheit II stimmen. 
-Wenn Sie mit der Minderheit I stimmen, wovon ich Ihnen trotz klarer Sympathie natürlich wärmstens abrate, dann werden Sie die zusätzlichen Stellen, die für die Umsetzung dieser Projekte notwendig sind, beim laufenden Betrieb bei der Bundeskriminalpolizei und an anderen Orten kompensieren müssen, was dazu führt, dass im Resultat sogar weniger Ressourcen zur Verfügung stehen werden, um der genannten Herausforderungen Herr zu werden. 
-Wenn man jetzt die Zahl der Meldungen ins Spiel bringt und sagt, es werde halt zu viel gemeldet, dann kommt mir das folgendermassen vor: Es gibt eine Sicherheitslage, in der sich die Kriminalität erhöht, in der die Leute nach mehr Polizei rufen und in der das Sicherheitsgefühl sinkt. Sie sehen, dass es ein Problem gibt, aber anstatt mehr Polizei anzustellen, sagen Sie zu den Menschen: Gebt halt weniger Strafanzeigen auf, dann haben wir das Problem gelöst. So schaffen Sie einfach eine Dunkelziffer, ein Dunkelfeld. 
-Ich sage damit nicht, dass der Effekt, den Kollege Mühlemann beschrieben hat, nicht ein Stück weit eintreten kann. Aber die Tatsache ist, dass wir es hier mit organisierter Kriminalität zu tun haben, und daher ist es wichtig, dass wir nicht in die Vogel-Strauss-Politik verfallen und sagen: Gebt halt weniger Anzeigen auf, ihr macht zu viele Anzeigen; wenn wir weniger davon wissen, dann wird es weniger schlimm sein. Das wäre das Prinzip "Augen zu und durch", und dazu rate ich Ihnen im Namen unserer Sicherheit nicht.
-Ich bitte Sie deshalb, mit der Minderheit II zu stimmen und zu berücksichtigen, was bereits die GPK, die SiK und viele andere empfehlen und empfohlen haben, und hier entsprechend konsequent zu sein. Dann können Sie am 11.[NB]Dezember auch der erwähnten Motion zustimmen.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">365070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hegglin Peter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wenn man Kollege Zopfi zuhört, könnte man meinen, wir hätten in den vergangenen Jahren zu wenig oder nichts getan. Das stimmt einfach nicht. Betrachten Sie die Personalstellen beim Fedpol: Im Jahr 2019 lag der Personalbestand bei 899 Vollzeitstellen. Im Jahr 2026 soll er auf 1060 Stellen aufgestockt werden. Im Jahr 2026 sollen im Vergleich zum Vorjahr 63 Stellen hinzukommen. Die Frage ist, wo sie eingesetzt werden. Aber wir beschliessen ja über das Gesamtbudget. Der Bundesrat hat die Verantwortu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wenn man Kollege Zopfi zuhört, könnte man meinen, wir hätten in den vergangenen Jahren zu wenig oder nichts getan. Das stimmt einfach nicht. Betrachten Sie die Personalstellen beim Fedpol: Im Jahr 2019 lag der Personalbestand bei 899 Vollzeitstellen. Im Jahr 2026 soll er auf 1060 Stellen aufgestockt werden. Im Jahr 2026 sollen im Vergleich zum Vorjahr 63 Stellen hinzukommen. Die Frage ist, wo sie eingesetzt werden. Aber wir beschliessen ja über das Gesamtbudget. Der Bundesrat hat die Verantwortung und die Aufgabe, die zur Verfügung gestellten Mittel sachgerecht einzusetzen.
-Ich habe gesagt, dass 63 zusätzliche Stellen vorgesehen sind - das entspricht einem Wachstum von 6,3 Prozent. Das ist ein sehr viel stärkeres Wachstum als in der übrigen Bundesverwaltung. Über den Zeithorizont von 2019 bis 2026 lag das Personalwachstum beim Fedpol bei 2,9 Prozent im Jahr, also bei fast 3 Prozent. In der Bundesverwaltung lag es im gleichen Zeitraum bei 0,8 Prozent im Jahr. Das Fedpol wächst also im Vergleich zur übrigen Bundesverwaltung überdurchschnittlich. Von daher kommen wir den Empfehlungen der EFK nach, und wir kommen mit dem Antrag der Mehrheit Ihrer Finanzkommission auch dem Anliegen und[NB]dem[NB]Auftrag in diesem Sektor nach. Denn die Sicherheit und die Bekämpfung der kriminellen Organisationen sind wichtig.
-Ich empfehle Ihnen also, der Mehrheit Ihrer Kommission zu folgen und damit, wie gesagt, den Rahmen dafür zu schaffen, dass 63 zusätzliche Stellen geschaffen werden können.
+    <t xml:space="preserve">365786</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20251208</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bundesrat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keller-Sutter Karin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aufgrund eines Einstellungsfehlers in der Veranlagungssoftware konnte die kantonale Steuerverwaltung Genf für rund 60 Unternehmen, die in den vorangegangenen Steuerperioden noch nicht definitiv veranlagt worden waren, keine provisorischen Rechnungen gemäss Artikel 162 des Bundesgesetzes über die direkte Bundessteuer ausstellen. Dieser technische Fehler konnte mittlerweile behoben werden, sodass nun ordnungsgemäss provisorische Rechnungen ausgestellt werden können.
+Der Gesetzgeber hat die Finanza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aufgrund eines Einstellungsfehlers in der Veranlagungssoftware konnte die kantonale Steuerverwaltung Genf für rund 60 Unternehmen, die in den vorangegangenen Steuerperioden noch nicht definitiv veranlagt worden waren, keine provisorischen Rechnungen gemäss Artikel 162 des Bundesgesetzes über die direkte Bundessteuer ausstellen. Dieser technische Fehler konnte mittlerweile behoben werden, sodass nun ordnungsgemäss provisorische Rechnungen ausgestellt werden können.
+Der Gesetzgeber hat die Finanzaufsicht über die direkte Bundessteuer den 26 kantonalen Finanzkontrollen übertragen. Sie sind gehalten, jährlich die Ordnungs- und Rechtmässigkeit der Erhebung der direkten Bundessteuer und der Ablieferung des Bundesanteils zu prüfen und der Eidgenössischen Steuerverwaltung sowie der Eidgenössischen Finanzkontrolle darüber Bericht zu erstatten. Als Oberaufsicht hat die Eidgenössische Steuerverwaltung hierzu eine Richtlinie sowie ein verbindliches Prüfraster zuhanden der kantonalen Finanzkontrollen erlassen. Der erwähnte Softwarefehler wurde von der kantonalen Finanzkontrolle nicht festgestellt. Die Eidgenössische Steuerverwaltung ist derzeit daran, die Zusammenarbeit mit den kantonalen Finanzkontrollen zu intensivieren, und prüft übergeordnet, gemeinsam mit der Eidgenössischen Finanzverwaltung, weitergehende Massnahmen im Bereich der Rechnungsstellung für die direkte Bundessteuer. 
+Was die finanziellen Auswirkungen anbelangt, so steht der sogenannte Vergütungszins im Vordergrund. Dieser ist geschuldet, wenn Steuerpflichtige höhere Vorauszahlungen machen, als ihnen in Rechnung gestellt wurden. In welchem Ausmass dies tatsächlich erfolgte, kann erst bei der Erstellung der definitiven Veranlagung berechnet werden. Zu berücksichtigen ist jedoch, dass der Zinssatz für die Vergütungen tief ist: Für die primär betroffenen Kalenderjahre 2019 bis 2023 lag er bei 0,00 Prozent, für 2024 bei 1,25 Prozent und für 2025 bei 0,75 Prozent.
 </t>
   </si>
   <si>
     <t xml:space="preserve">366164</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20251208</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bundesrat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keller-Sutter Karin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG</t>
   </si>
   <si>
     <t xml:space="preserve">Ich äussere mich zu ausgewählten Minderheiten, da wir ja auch mit der Zeit etwas sorgsam umgehen sollten. Ich beginne beim Staatssekretariat für Migration (SEM) mit dem Ziel "Erfüllung der Qualitätsstandards im Bereich Unterbringung"; der Bundesrat ist hier einverstanden.
@@ -697,45 +734,16 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">366073</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conseil national</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nicolet Jacques</t>
+    <t xml:space="preserve">365999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nationalrat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bürgi Roman</t>
   </si>
   <si>
     <t xml:space="preserve">V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce deuxième bloc traite de la sécurité, de la justice et de la migration. Treize propositions vous sont soumises. Je vais traiter les premières et Peter Schilliger commentera les dernières.
-Concernant le DFJP, dans l'unité administrative 402, l'Office fédéral de la justice, à la position "Valeurs patrimoniales confisquées", à la page A11 du dépliant, il s'agit de valeurs qui peuvent être confisquées à des bandes criminelles organisées. Tenant compte du résultat des comptes 2024 et du fait de l'a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ce deuxième bloc traite de la sécurité, de la justice et de la migration. Treize propositions vous sont soumises. Je vais traiter les premières et Peter Schilliger commentera les dernières.
-Concernant le DFJP, dans l'unité administrative 402, l'Office fédéral de la justice, à la position "Valeurs patrimoniales confisquées", à la page A11 du dépliant, il s'agit de valeurs qui peuvent être confisquées à des bandes criminelles organisées. Tenant compte du résultat des comptes 2024 et du fait de l'augmentation des effectifs de l'Office fédéral de la police, Fedpol, la majorité de la commission propose de majorer de 12,8 millions de francs les valeurs patrimoniales confisquées afin de les porter à 100 millions. Une minorité Farinelli propose d'en rester au montant de 87 millions, comme le prévoit le Conseil fédéral, jugé plus réaliste. Cette proposition vaut également pour le plan financier 2027-2029. Par 13 voix contre 11 et 0 abstention, la Commission des finances vous demande de suivre la proposition de la majorité, à 100 millions.
-Toujours à la page A11, à la position "Subventions de construction pour la détention administrative", le Conseil des États a décidé, par 40 voix contre 2 et 1 abstention, d'une coupe de 10 millions de francs. Il s'agit d'une réduction de 10 millions pour le centre de détention administrative en vue d'expulsion de l'aéroport de Zurich. Ces contributions méritent d'être réexaminées sous l'angle de leur nécessité et de leur envergure, et, pour l'heure, en attendant des éclaircissements, par 15 voix contre 10, la commission vous demande de suivre la position du Conseil des États, soit une coupe de 10 millions. La minorité Fehlmann Rielle demande d'en rester au montant proposé par le Conseil fédéral.
-Pour l'unité administrative 403, Fedpol, à la page A11, à la position "Charges de fonctionnement", une minorité Bürgi Roman propose d'en rester au montant de 294,5 millions de francs, comme le propose le Conseil fédéral. La question du nombre de postes pour Fedpol en général, et à la police judiciaire plus particulièrement, n'est pas nouvelle. Tant l'examen des ressources de Fedpol que le rapport du Contrôle fédéral des finances l'attestent. Bien que plus de 50 postes soient prévus, 15 autres postes doivent être supprimés dans le cadre des mesures d'allégement 2027. Cette proposition vaut également pour le plan financier 2027-2029. La commission, par 16 voix contre 8 et 0 abstention, propose de majorer de 1,8 million les moyens pour Fedpol.
-Pour l'unité administrative 420, le Secrétariat d'État aux migrations (SEM), à la page A11, dans le domaine des dépenses courantes, estimant qu'il faut impérativement faire des économies dans le domaine migratoire, une minorité Sollberger propose de réduire de 600 millions de francs cette position budgétaire pour la ramener à 3,36 milliards. La commission, par 16 voix contre 8 et 0 abstention, estime qu'il n'est pas adéquat de faire une demande de coupe et propose d'en rester au montant de 3,96 milliards demandé par le Conseil fédéral.
-Toujours pour le SEM, à la page A12, dans le domaine de l'aide sociale pour les requérants admis à titre provisoire comme réfugiés, le Conseil fédéral a porté au budget un montant de 2,089 milliards de francs ainsi que de 600 millions dans la contribution aux cantons pour l'Ukraine. La majorité de notre commission propose un transfert comptable de 130 millions, qui seraient prélevés dans la contribution aux cantons pour l'Ukraine, dans les dépenses extraordinaires, pour les réaffecter aux dépenses ordinaires dans le domaine de l'aide sociale pour les requérants d'asile admis à titre provisoire. Cela permettra de soulager de 130 millions les dépenses extraordinaires. Dans le même temps, la majorité propose de diminuer de 130 millions aussi les indemnités versées aux cantons au titre de l'aide sociale dans le domaine de la migration, cela en raison des prévisions à la baisse concernant les demandes d'asile en 2026. Cette proposition a été soutenue par 14 voix contre 11. La minorité Funiciello souhaite en rester aux propositions initiales du Conseil fédéral, soit renoncer au transfert de 130 millions et maintenir 2,089 milliards en dépenses ordinaires et 600 millions en dépenses extraordinaires. Cette proposition a été refusée par 14 voix contre[NB]11.
-La minorité II (Sollberger) souhaite rapatrier les 600 millions de francs de la contribution des cantons à l'Ukraine dans l'aide sociale pour les personnes admises à titre provisoire, portant cette position à 2,69 milliards de francs, cela afin que l'ensemble des dépenses soient comptabilisées dans les dépenses ordinaires.
-Estimant qu'il y a un risque important que la Confédération doive tout de même indemniser obligatoirement les cantons, cette proposition a été rejetée, par 15 voix contre 8 et 1 abstention.
-À la page C2, s'agissant des objectifs et de la valeur-cible du Secrétariat d'État aux migrations, la commission, sans avis contraire, propose, en ce qui concerne les procédures d'asile, de porter les objectifs en matière de respect des normes de qualité dans le domaine de l'hébergement à 95 pour cent, contre 90 pour cent pour le Conseil fédéral.
-S'agissant des indicateurs relatifs aux demandes pendantes en première instance depuis plus d'un an, la minorité Kälin a été retirée.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">365999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nationalrat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bürgi Roman</t>
   </si>
   <si>
     <t xml:space="preserve">SZ</t>
@@ -758,6 +766,9 @@
   </si>
   <si>
     <t xml:space="preserve">Andrey Gerhard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR</t>
   </si>
   <si>
     <t xml:space="preserve">Ja, dieser wichtige EFK-Bericht ist der Finanzkommission natürlich bekannt. Ich würde Ihnen antworten: das eine tun, das andere nicht lassen. Ich bin mit Ihnen natürlich völlig einig, dass die Ressourcen möglichst effizient eingesetzt werden müssen. Aber wenn man genau hinschaut, auch bei den anderen Staatsebenen, sieht man, dass es sich tatsächlich um ein substanzielles Ressourcenproblem handelt. Entsprechend helfen wir da mit.
@@ -829,6 +840,9 @@
   </si>
   <si>
     <t xml:space="preserve">367062</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conseil des Etats</t>
   </si>
   <si>
     <t xml:space="preserve">Juillard Charles</t>
@@ -944,6 +958,9 @@
   </si>
   <si>
     <t xml:space="preserve">Parmelin Guy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VD</t>
   </si>
   <si>
     <t xml:space="preserve">Les temps actuels sont caractérisés par une forte incertitude et de grands défis, surtout sur le plan international, avec les tensions géopolitiques, la politique commerciale des États-Unis, des actualités comme l'imposition minimale de l'OCDE et j'en oublie. La réduction des droits de douane américains est un élément important, mais la situation va rester volatile. Avec toutes les actualités internationales, il est essentiel de ne pas perdre le focus sur notre pays, notre économie, nos travaill</t>
@@ -1006,10 +1023,42 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">367979</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20251217</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rösti Albert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ich möchte einleitend klar festhalten, dass der Bundesrat und auch ich persönlich zur Dekarbonisierung und zum Fahrplan, den unser Volk verabschiedet hat, stehen. Da besteht kein Zweifel. Ich erinnere aber gleichzeitig daran, dass wir diese Debatte - und ich danke dafür, dass wir sie führen können, es ist eine wichtige Debatte - rund einen Monat nach der Klimakonferenz in Belém abhalten. In Belém ist es nicht gelungen, international mindestens einen Fahrplan, eine Roadmap mit verbindlichen Punkt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ich möchte einleitend klar festhalten, dass der Bundesrat und auch ich persönlich zur Dekarbonisierung und zum Fahrplan, den unser Volk verabschiedet hat, stehen. Da besteht kein Zweifel. Ich erinnere aber gleichzeitig daran, dass wir diese Debatte - und ich danke dafür, dass wir sie führen können, es ist eine wichtige Debatte - rund einen Monat nach der Klimakonferenz in Belém abhalten. In Belém ist es nicht gelungen, international mindestens einen Fahrplan, eine Roadmap mit verbindlichen Punkten, wo wann was zu geschehen hat, aufzustellen; es ist nicht gelungen, auch nur zu sagen, dass sich die Länder für eine Roadmap entscheiden und eine solche aufstellen sollen. Die wichtigsten Produzenten von fossiler Energie, die grossen Mächte China, USA, Indien und Saudi-Arabien, waren nicht bereit, in diese Richtung zu gehen. Das muss man wissen. Unsere Debatte hier findet auch einen Tag nachdem die Europäische Union das Verbrennerverbot rückgängig gemacht hat, statt.
+Wir müssen einfach auch vom Umfeld sprechen. Denn eines möchte ich am Anfang in aller Klarheit sagen: Wir stehen zur Dekarbonisierung. Aber sie bringt der Schweiz nur etwas, wenn sie weltweit geschieht. Sie wissen es alle haargenau: Die Schweiz alleine wird das Klima nicht ändern, kein Jota ändern. Deshalb bin ich jetzt schon erstaunt, wenn man hier hört, dass sich der Bundesrat weigere, Verantwortung zu übernehmen.
+Ihre Initiative für den Klimaschutz, die 0,5 bis 1 Prozent des Bruttoinlandproduktes für Klimamassnahmen verwenden will, bedeutet, dass der Bund die Verantwortung alleine übernehmen und jährlich 3,5 bis über 7 Milliarden Franken für den Klimaschutz einsetzen soll. Es ist absolut legitim, das zu fordern. Aber jetzt sage ich Ihnen, was wir heute machen, auch wenn Sie es als fehlende Verantwortung quantifizieren oder darstellen: Der Bund bezahlt jährlich, das wurde von Ihnen entschieden, 2 Milliarden Franken für die Dekarbonisierung und den Klimaschutz. Dazu kommen 600 Millionen Franken für die Biodiversität und noch 800 Millionen Franken für den internationalen Klimaschutz. Das heisst, die Schweiz, die gemäss Ihren Voten und den Interpellationen offenbar nichts tut, investiert bereits heute jährlich 3,4 Milliarden Franken, dies kombiniert mit Anreizmassnahmen, mit Abbaupfaden, mit Sanktionen für die Autohersteller, mit einem Emissionshandelssystem. Es ist eine Kombination verschiedener Massnahmen. Es wird nicht einfach nur der Bund in die Verantwortung gestellt. Ich kann durchaus nachvollziehen, dass man das in der Debatte so bringt, aber ich möchte es schon klar zurückweisen, dass der Bundesrat die Verantwortung verweigert. 
+Wir haben die Interpellationen entsprechend beantwortet. Ich danke Ihnen für die entsprechenden Fragen und werde mich gesamthaft dazu äussern, weil wir nicht allzu viel Zeit haben. 
+Zur Interpellation der Fraktionen der SP und der Grünen: Die Klimaszenarien zeigen, dass die Schweiz vom Klimawandel betroffen ist, das ist unbestritten. Die Szenarien verdeutlichen die Notwendigkeit globaler - nochmals: globaler - Anstrengungen zur Verminderung der Treibhausgasemissionen und auch der Anpassung der Klimamassnahmen. Die Klimaszenarien bilden auch für den Bundesrat die Grundlage für seine Strategie zur Dekarbonisierung und zur Anpassung an den Klimawandel. 
+Der Bundesrat anerkennt den Investitionsbedarf; vorhin habe ich bereits die jährlichen Investitionen erwähnt. In den letzten Jahren haben Sie mit wichtigen Gesetzesvorlagen - dafür danke ich - klare Vorgaben gemacht. Anfang dieses Jahres haben wir vier Vorlagen unverzüglich durch Verordnungen in Kraft gesetzt: das Klima- und Innovationsgesetz, das revidierte CO2-Gesetz für die Periode 2025-2030, das Bundesgesetz über eine sichere Stromversorgung mit erneuerbaren Energien sowie das Umweltschutzgesetz zur Stärkung der Kreislaufmassnahmen. Bei Letzterem sind zwar noch einige Punkte nicht vollständig umgesetzt, doch wir sind daran, sie anzugehen. Es sind also vier Gesetze, die Sie in Kraft gesetzt haben und die der Bundesrat unverzüglich mit Verordnungen umsetzt, ebenso wie Investitionen in der Höhe von jährlich 3,4 Milliarden Franken in den Klimaschutz und die Erneuerung unseres Energiesystems. Und Sie sagen, der Bundesrat verweigere hier die Verantwortung? Mit Verlaub, das kann ich so einfach nicht stehenlassen.
+Nochmals zur Erinnerung: Heute stellt der Bund jährlich 2 Milliarden Franken für den Klimaschutz und den Umbau des Energiesystems bereit. Diese Zahl berücksichtigt bereits die Kürzungen infolge des Entlastungspaketes. Sie werden über die rund 400 Millionen Franken diskutieren und demokratisch entscheiden, die wir als Gegenpart einsparen wollen. Wenn Sie diese 400 Millionen Franken nicht einsparen, liegen wir nicht bei 3,4 Milliarden, sondern bei 3,8 Milliarden Franken. Dieser Betrag ist also bereits eingerechnet. 
+Ehrlich gesagt bin ich mir nicht sicher, ob die Schweiz ihre Klimaziele bis 2030 erreichen kann. Es braucht zusätzliche Investitionen, und diese fallen in ein finanzpolitisches Umfeld, das es uns nicht leichtmacht, angesichts der Bedürfnisse in der Armee und im Sozialbereich. Der Bundesrat wird diesbezüglich am Ball bleiben, alles analysieren und sich 2027 dazu äussern, wo wir stehen. Ich meine, heute, ein Jahr nach Inkrafttreten des revidierten CO2-Gesetzes, ist es noch zu früh, um über die Zielerreichung zu sprechen.
+Das Klima- und Innovationsgesetz verpflichtet den Bundesrat, dem Parlament rechtzeitig Vorschläge zur Weiterentwicklung der Klimapolitik vorzulegen. Das Parlament behält jederzeit die Kompetenz, hier auch zu intervenieren. Zur Weiterentwicklung der Klimapolitik hat der Bundesrat denn auch verzugslos gehandelt. Am 12.[NB]September dieses Jahres haben wir zwei Aussprachen geführt. Zum einen haben wir über die Revision des CO2-Gesetzes ab 2031 bis 2040 diskutiert und bereits Eckwerte festgehalten, die dann in eine Vernehmlassung auf Mitte nächstes Jahr einfliessen, bei der Sie Stellung nehmen können, sodass wir Ihnen 2027 auch rechtzeitig eine Botschaft werden vorlegen können. Dann werden wir sicher auch Bilanz ziehen, wo wir stehen. Zukünftig sollen gemäss diesen Eckwerten CO2-Emissionen aus Gebäuden und aus dem Verkehr respektive Brenn- und Treibstoffe in ein neues Emissionshandelssystem eingebunden werden. Dadurch können gemäss unseren Überlegungen deutlich mehr Mittel generiert werden, ohne Steuern zu erhöhen. Mehr Mittel können natürlich aus den heute bestehenden Abgaben generiert werden, indem man diese dann auch effektiv für Klimamassnahmen einsetzen kann. Der Bundesrat anerkennt das und will auf diesem Pfad weitergehen. Die Einnahmen sollen, wie gesagt, zur Dekarbonisierung in den bekannten Sektoren Gebäude, Verkehr und Industrie eingesetzt werden. Wir sind als UVEK jetzt beauftragt, für den Bundesrat bis [PAGE 2390] spätestens Sommer 2026 eine Vernehmlassungsvorlage vorzulegen.
+Ich habe vorhin die globale Situation angesprochen, und die ist wirklich schwierig und aktuell in einigen Bereichen blockiert. Deshalb bin ich dankbar, dass Frau Nationalrätin Wismer eine Interpellation zu den Anpassungsmassnahmen eingereicht hat. Es ist so: Wir brauchen zusätzliche Anpassungsmassnahmen, wir kommen nicht darum herum. Auch wenn das 1,5-Grad-Ziel erreicht wird, braucht es Anpassungsmassnahmen. Wenn es nicht erreicht wird, braucht es entsprechend mehr Anpassungsmassnahmen.
+Aber bereits heute setzen Bund, Kantone und Gemeinden jährlich 600 Millionen Franken ein. Wir stellen fest, dass diese Summe aktuell ausreicht. Mit diesen Mitteln wollen wir in Zukunft mehr erreichen, indem sie risikobasiert eingesetzt werden. Indem wir eine risikobasierte, bessere Planung machen, über die Raumplanung die Risiken auch abschwächen, wollen wir den einzelnen Franken also effizienter einsetzen. Das haben Sie letztes Jahr mit der Änderung des Wasserbaugesetzes so entschieden. Die Kantone sind zudem seit dem 1.[NB]August dieses Jahres verpflichtet, bei der Gefahrenbeurteilung und Massnahmenplanung den Klimawandel zu berücksichtigen. Gemeinsam mit dem Bund setzen die Kantone auch die nationale Strategie zur Anpassung an den Klimawandel um. Diese wird derzeit aktualisiert. 
+Zudem wurden in der Herbstsession das Postulat Wandfluh 25.3489, "Naturgefahren. Kriterien für eine differenzierte Nutzung von Gefahrengebieten", und das Postulat 25.3669 der FDP-Liberalen Fraktion, "Überprüfung und allfällige Ergänzung der gesetzlichen Grundlagen für eine rasche Katastrophenhilfe des Bundes", angenommen. Wir werden diese Postulate detailliert beantworten, dazu Bericht erstatten und daraus allfällige Schlussfolgerungen ziehen, ob es im Anpassungsbereich zusätzliche Massnahmen braucht. 
+Der Bundesrat nimmt die Erkenntnisse aus den Klimaszenarien ernst. Sie verdeutlichen den Handlungsbedarf bei der Verminderung der Treibhausgasemissionen und der Anpassung an den Klimawandel. 
+Ich möchte nun nochmals auf das Sparprogramm eingehen und erklären, weshalb die Massnahmen, die wir vorgesehen haben, für den Bundesrat und für mich verantwortbar und durchaus kohärent zum jetzt von mir Gesagten sind. Im Bericht Gaillard wurde vorgeschlagen, die 400 Millionen Franken, über die vom Volk in der Abstimmung über das Klima- und Innovationsgesetz entschieden wurde, einzusparen. Der Bundesrat hat schliesslich gesagt: Wir wollen das nicht einsparen, wir brauchen diese Mittel für den Ölheizungsersatz in Mehrparteiengebäuden, und wir brauchen sie für Innovationen. Und hier ist für mich eben die internationale Komponente sehr wichtig: dass wir mit Innovationen nicht nur in der Schweiz zur Dekarbonisierung beitragen, sondern auch international. 
+Ich war aber gezwungen, im Gegenzug zu sagen, wo wir stattdessen sparen, denn jeder Bereich musste einen Beitrag leisten. Was haben wir also genommen? Wir haben den Gebäudebereich genommen, da das Gebäudeprogramm schon sehr lange läuft und alle, die rasch ihre Heizung umstellen wollten, die Subventionen und Unterstützung längst abgeholt haben. Und bei jenen, die nicht "first movers" waren, die das noch nicht gemacht haben, kommt genau der Mitnahmeeffekt ins Spiel: Sie machen den Ersatz auch, aber erst dann, wenn ihre Heizung abgeschrieben ist; dann nehmen sie einfach die Subvention, aber das ist ohne Wirkung, weil sie die Heizung sowieso ersetzen müssen. Das ist der Mitnahmeeffekt. Wir haben in einem Bericht der Eidgenössischen Finanzkontrolle und in verschiedenen Studien gesehen, wie gross dieser Mitnahmeeffekt in etwa ist: Je nach Studie - es ist schwierig zu berechnen - sind es 40 bis 70 Prozent. Sie wollen doch nicht, dass der Bund Leuten Geld sozusagen schenkt, die es einfach nehmen, weil es der Bund anbietet, die aber ihre Heizung ohnehin umstellen würden. Das einfach zu den Sparmassnahmen. 
+Es wurden auch die 200 Millionen Franken Einsparung beim Bahninfrastrukturfonds erwähnt. Sie haben dazu bereits eine Motion angenommen, damit hier in Zukunft, ab 2029, wieder mehr Geld zur Verfügung steht. Wenn wir die Finanzierung mit dem Mehrwertsteuerpromille weiterführen, sind es 400 Millionen Franken, die jährlich dazukommen. Ich habe das ausgeführt, um einfach etwas die Relationen hier in diesem Bereich aufzuzeigen.
+Ich danke Ihnen für die Debatte und dafür, dass ich die Haltung des Bundesrates hier transparent darstellen durfte.
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">368245</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20251217</t>
   </si>
   <si>
     <t xml:space="preserve">Das ist ein bisschen ein Streit um des Kaisers Bart. Der Präsident der Finanzkommission hat es gesagt: Es geht um ein Rahmengesetz. An sich wollte der Bundesrat im Gesetz klarer festhalten, dass die Empfänger von Finanzhilfen ihre Aufgaben soweit möglich selbst finanzieren; das war auch immer ein Wunsch der Eidgenössischen Finanzkontrolle (EFK). Der Herr Präsident hat es gesagt: Es kamen dann Ängste aus dem Kultur- und dem Umweltbereich, dass durchgehend nur noch 50 Prozent Subventionen ausbezah</t>
@@ -1017,6 +1066,23 @@
   <si>
     <t xml:space="preserve">Das ist ein bisschen ein Streit um des Kaisers Bart. Der Präsident der Finanzkommission hat es gesagt: Es geht um ein Rahmengesetz. An sich wollte der Bundesrat im Gesetz klarer festhalten, dass die Empfänger von Finanzhilfen ihre Aufgaben soweit möglich selbst finanzieren; das war auch immer ein Wunsch der Eidgenössischen Finanzkontrolle (EFK). Der Herr Präsident hat es gesagt: Es kamen dann Ängste aus dem Kultur- und dem Umweltbereich, dass durchgehend nur noch 50 Prozent Subventionen ausbezahlt würden. Das wäre nicht der Fall gewesen.
 Wenn Sie das streichen, ist das nicht gravierend, weil auch das aktuelle Recht davon ausgeht, und das ist wichtig, dass Subventionsempfänger nach Kräften und ihrer wirtschaftlichen Leistungsfähigkeit mitbeteiligt werden. In der Regel, nach ständiger Praxis der Eidgenössischen Finanzverwaltung, sind das 50 Prozent, aber das muss im Einzelfall festgelegt werden. Ich verzichte hier auf eine Abstimmung, wir können mit dem geltenden Recht leben, es war der Versuch einer Präzisierung. In der Sache wird das nicht viel daran ändern, dass man immer noch darum feilschen wird, welcher Subventionssatz im Einzelfall angewendet wird.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">368193</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stark Jakob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Bundesrat beantragt, auf Finanzhilfen des Bundes im Bereich der Weiterbildung zu verzichten. Die Gründe sind folgende: Der Weiterbildungsmarkt ist weitgehend privatwirtschaftlich organisiert. Es gibt in diesem Bereich sehr namhafte Mitnahmeeffekte. Mehrfach schon gab es Kritik der Eidgenössischen Finanzkontrolle daran, wie und wofür diese Beiträge an die Organisationen der Weiterbildung gehen und wie ihre Wirkung ist. Schwergewichtig geht es hier ja um die Förderung der Grundkompetenzen, und</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Bundesrat beantragt, auf Finanzhilfen des Bundes im Bereich der Weiterbildung zu verzichten. Die Gründe sind folgende: Der Weiterbildungsmarkt ist weitgehend privatwirtschaftlich organisiert. Es gibt in diesem Bereich sehr namhafte Mitnahmeeffekte. Mehrfach schon gab es Kritik der Eidgenössischen Finanzkontrolle daran, wie und wofür diese Beiträge an die Organisationen der Weiterbildung gehen und wie ihre Wirkung ist. Schwergewichtig geht es hier ja um die Förderung der Grundkompetenzen, und dabei ist zu beachten, dass das eine ureigene Aufgabe der Kantone ist und dass sich der Bund mit Spezialgesetzen im Ausländerrecht, in der ALV und IV hier schon engagiert. Aus diesem Grund beantragt der Bundesrat, die Bestimmungen aufzuheben. Die Entlastungswirkung ist bei 19,8 Millionen Franken.
+Diese drei Anträge, die Sie hier vor sich haben, sehen alle vor, auf die Gesetzesänderung zu verzichten, mit Verweis auf die Kann-Bestimmung in Artikel 12 Absatz 1 WeBiG. Es ist also ohne Weiteres möglich, das Gesetz so zu belassen und bei der entsprechenden Position im Voranschlag den Betrag anzupassen. Die Kommissionsmehrheit möchte die volle Entlastungswirkung beibehalten, also die gut 19 Millionen Franken. Die Minderheit I (Herzog Eva) möchte die Entlastungswirkung knapp halbieren, sie möchte hier weiterhin 10[NB]Millionen[NB]Franken budgetieren. Die Minderheit II (Maillard Pierre-Yves) empfiehlt Ihnen, auf eine Kürzung ganz zu verzichten.
 </t>
   </si>
   <si>
@@ -1053,6 +1119,29 @@
 Die Ruag-Affäre ist dabei nur die Spitze des Eisbergs. Die Eidgenössische Finanzkontrolle hat gravierende Missstände aufgezeigt: fehlende Compliance, Mängel in der Governance, sogar Betrugsverdacht. Dass ein bundeseigenes Unternehmen mit Leopard-Panzern dubiose Geschäfte tätigen wollte, zeigt, dass Kontrolle und Verantwortung nicht funktionieren. Wir haben es hier nicht mit kleinen Schönheitsfehlern zu tun, sondern mit wiederkehrenden Mustern - Beschaffung ohne Reife, Kostenüberschreitungen, jahrelange Verzögerungen. Es ist immer dasselbe Muster: Verantwortung wird abgeschoben, niemand ist zuständig. 
 Ja, das Parlament hat mit GPK und FinDel starke Aufsichtsorgane. Aber sie stossen hier an ihre Grenzen. Nur eine PUK hat die vollen Rechte und ausreichend Ressourcen. Sie kann Bundesratsprotokolle einsehen, Zeugen vorladen und die ganze Führungskette unter die Lupe nehmen. Genau das braucht es, wenn wir verlorenes Vertrauen zurückgewinnen wollen. Es geht nicht darum, das VBS zu schwächen, sondern darum, es endlich zu stärken: durch Transparenz, klare Verantwortlichkeiten und eine Kultur, die Fehler nicht vertuscht, sondern aus ihnen lernt. Unser Ziel ist es, die Struktur zu verbessern, damit die Armee ihren Auftrag zuverlässig erfüllen kann, ohne dass Milliarden versickern. Die Schweiz kennt die Lehren aus der Mirage-Affäre von 1964. [PAGE 2478] Nur eine PUK kann das Vertrauen in das VBS wiederherstellen. Heute stehen wir an einem ähnlichen Punkt. Wenn wir jetzt nicht handeln, drohen neue Skandale. Die Zeche zahlen am Schluss die Steuerzahlenden und die Sicherheit unseres Landes. 
 Ich bitte Sie deshalb, diesen parlamentarischen Initiativen Folge zu geben. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">368811</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Büchel Roland Rino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Das Büro des Nationalrates hat die parlamentarischen Initiativen 25.407 und 25.414 an seiner Sitzung vom 22.[NB]August 2025 vorgeprüft. Diese waren von der Sozialdemokratischen Fraktion am 10.[NB]März 2025 bzw. von der Grünen Fraktion am[NB]21.[NB]März 2025 eingereicht worden. Sie fordern je die Einsetzung einer PUK mit dem Zweck, die Probleme bei der Rüstungsbeschaffung sowie die Führungs-, Kontroll- und Aufsichtsstrukturen innerhalb des VBS zu untersuchen. Sie haben es gehört von Herrn Bendaha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Das Büro des Nationalrates hat die parlamentarischen Initiativen 25.407 und 25.414 an seiner Sitzung vom 22.[NB]August 2025 vorgeprüft. Diese waren von der Sozialdemokratischen Fraktion am 10.[NB]März 2025 bzw. von der Grünen Fraktion am[NB]21.[NB]März 2025 eingereicht worden. Sie fordern je die Einsetzung einer PUK mit dem Zweck, die Probleme bei der Rüstungsbeschaffung sowie die Führungs-, Kontroll- und Aufsichtsstrukturen innerhalb des VBS zu untersuchen. Sie haben es gehört von Herrn Bendahan: Er denkt, dass eigentlich 15 PUK das Richtige wären - dazu gibt es aber keinen Antrag. Konkret geht es um zwei PUK, die verlangt werden.
+Das Büro des Nationalrates beantragt mit 9 zu 3 Stimmen, beiden Initiativen keine Folge zu geben. Die Minderheiten beantragen - Sie haben es gehört -, diesen Folge zu geben.
+Eine parlamentarische Untersuchungskommission einzusetzen, um die Missstände im Bereich der Ruag und Probleme bei der Rüstungsbeschaffung zu untersuchen, ist für die Minderheiten das richtige Vorgehen. Auch die Probleme bei den Führungs-, Kontroll- und Aufsichtsstrukturen innerhalb des VBS könnten von einer PUK besser untersucht werden als von der GPK und der FinDel.
+In Bezug auf die Oberaufsicht beim VBS liess sich das Büro von den GPK und der FinDel als zuständige Organe über deren laufende Arbeiten informieren. In beiden GPK gibt es je eine ständige Subkommission zur parlamentarischen Kontrolle der Geschäftsführung des VBS. Aktuelle Schwerpunktthemen sind die Inspektion zum Fixpreis des F-35A und die [PAGE 2479] Untersuchung der Governance der Ruag MRO durch den Eigner. Die beiden Berichte werden voraussichtlich im kommenden Jahr veröffentlicht.
+Mit ihrer Inspektion zum Fixpreis des F-35A will die GPK-N unter anderem klären, ob bei der Aushandlung der Verträge rückblickend Mängel in der Geschäftsführung des Bundesrates festgestellt werden können. Die GPK-S nimmt vertiefte Abklärungen zur Aufsicht und Steuerung der Ruag MRO durch den Bundesrat vor. Auslöser für diese Untersuchungen waren Unstimmigkeiten beim versuchten Verkauf - auf der anderen Seite auch beim Kauf - von 96 Leopard-1-Panzern an Deutschland im Jahr 2023, aber auch weiter zurückreichende Betrugsvorwürfe, welche von der Eidgenössischen Finanzkontrolle aufgedeckt worden waren.
+Die GPK beschäftigen sich zudem wiederkehrend und teils über Jahre hinweg mit der Mehrheit der Top-Projekte des VBS. Beispiele dafür sind das ehemalige Munitionslager Mitholz, das Aufklärungsdrohnensystem ADS 15, die Neue Digitalisierungsplattform und das Sicherheitsfunknetz Polycom. Weitere wichtige Projekte des VBS werden von den beiden GPK im Rahmen ihrer Oberaufsicht begleitet. Dabei handelt es sich unter anderem um die Planung der Rüstungsbeschaffung oder um den Schutz kritischer Infrastrukturen und um die Berechnung des Armeebestandes. An einer speziellen Sitzung befassen sich die beiden GPK jährlich mit den Berichten des Bundesrates über die Zielerreichung der Ruag MRO und der Ruag International. Dort müssen neben den Spitzen von VBS und EFD auch die beiden Unternehmungen Red und Antwort stehen.
+Aber auch die FinDel befasst sich im Rahmen ihrer Finanzoberaufsicht mit den Schlüssel- und Top-Projekten des VBS. Weil es sich beim VBS um das Departement - das wurde zu Recht erwähnt - mit den grössten finanziellen Risiken handelt und das Parlament die Rüstungsausgaben für 2025 aufgestockt hat, wird die FinDel die Finanz- und Investitionsplanung im Rüstungsbereich richtigerweise verstärkt beaufsichtigen.
+Aufgrund dieser Informationen zu den laufenden Arbeiten in den GPK und der FinDel kommt das Büro zum Schluss, dass die aufgeworfenen Problemstellungen im VBS von den entsprechenden Aufsichtsorganen des Parlamentes bereits im Detail beaufsichtigt werden.
+Für die beiden Minderheiten Widmer Céline und Glättli handelt es sich bei den aufgezählten Missständen im VBS um ein Systemversagen. Für sie kann nur eine PUK das verlorene Vertrauen in das VBS wiederherstellen; die Minderheitssprecherin hat das noch einmal unterstrichen. Für das Büro hingegen sollten die GPK und die FinDel mit ihren weitreichenden Kompetenzen und den ordentlichen Mitteln in der Lage sein, ihre Aufsichtspflicht gegenüber dem VBS wahrzunehmen. Zudem würde die Konstituierung einer PUK einen zu hohen finanziellen und zeitlichen Aufwand bedeuten, ohne einen wirklichen Mehrwert zu generieren.
+Aus diesen Gründen beantragt Ihnen das Büro, wie eingangs gesagt, den beiden Initiativen keine Folge zu geben.
+[VS]
 </t>
   </si>
 </sst>
@@ -1101,8 +1190,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:I23" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:I23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:I27" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:I27"/>
   <tableColumns count="9">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="MeetingDate"/>
@@ -1472,592 +1561,704 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
         <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
         <v>30</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I5" t="s">
         <v>31</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
       </c>
       <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
         <v>36</v>
-      </c>
-      <c r="G6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
         <v>39</v>
-      </c>
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7"/>
-      <c r="F7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" t="s">
-        <v>49</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E8"/>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G8" t="s">
         <v>15</v>
       </c>
       <c r="H8" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9"/>
+      <c r="F9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" t="s">
         <v>49</v>
-      </c>
-      <c r="F9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" t="s">
-        <v>57</v>
-      </c>
-      <c r="I9" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" t="s">
         <v>54</v>
       </c>
-      <c r="D10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>15</v>
       </c>
-      <c r="G10" t="s">
-        <v>25</v>
-      </c>
       <c r="H10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="I10" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I11" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="F12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" t="s">
         <v>65</v>
       </c>
-      <c r="G12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" t="s">
-        <v>69</v>
-      </c>
       <c r="I12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13"/>
+        <v>67</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
       <c r="F13" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G13" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H13" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="I13" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
         <v>72</v>
       </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
+      <c r="E14"/>
       <c r="F14" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G14" t="s">
         <v>15</v>
       </c>
       <c r="H14" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="I14" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="D15" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E15" t="s">
-        <v>84</v>
+        <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G15" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="H15" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I15" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="D16" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>84</v>
       </c>
       <c r="F16" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G16" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="H16" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="I16" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="E17" t="s">
         <v>13</v>
       </c>
       <c r="F17" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="G17" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I17" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>97</v>
+        <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>98</v>
+        <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>99</v>
+        <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H18" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I18" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>105</v>
-      </c>
-      <c r="E19"/>
+        <v>97</v>
+      </c>
+      <c r="E19" t="s">
+        <v>98</v>
+      </c>
       <c r="F19" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="G19" t="s">
         <v>15</v>
       </c>
       <c r="H19" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="I19" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B20" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>104</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>105</v>
       </c>
       <c r="E20"/>
       <c r="F20" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="G20" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="H20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B21" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E21"/>
       <c r="F21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G21" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I21" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22"/>
+      <c r="F22" t="s">
         <v>116</v>
       </c>
-      <c r="B22" t="s">
+      <c r="G22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" t="s">
         <v>117</v>
       </c>
-      <c r="C22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="I22" t="s">
         <v>118</v>
-      </c>
-      <c r="E22" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" t="s">
-        <v>65</v>
-      </c>
-      <c r="G22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" t="s">
-        <v>119</v>
-      </c>
-      <c r="I22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
+        <v>119</v>
+      </c>
+      <c r="B23" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23"/>
+      <c r="F23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" t="s">
+        <v>120</v>
+      </c>
+      <c r="I23" t="s">
         <v>121</v>
       </c>
-      <c r="B23" t="s">
-        <v>117</v>
-      </c>
-      <c r="C23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" t="s">
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
         <v>122</v>
       </c>
-      <c r="E23" t="s">
+      <c r="B24" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" t="s">
+        <v>124</v>
+      </c>
+      <c r="G24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" t="s">
+        <v>125</v>
+      </c>
+      <c r="I24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" t="s">
+        <v>129</v>
+      </c>
+      <c r="E25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" t="s">
+        <v>130</v>
+      </c>
+      <c r="I25" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" t="s">
+        <v>133</v>
+      </c>
+      <c r="E26" t="s">
         <v>84</v>
       </c>
-      <c r="F23" t="s">
-        <v>65</v>
-      </c>
-      <c r="G23" t="s">
-        <v>25</v>
-      </c>
-      <c r="H23" t="s">
-        <v>123</v>
-      </c>
-      <c r="I23" t="s">
-        <v>124</v>
+      <c r="F26" t="s">
+        <v>64</v>
+      </c>
+      <c r="G26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" t="s">
+        <v>134</v>
+      </c>
+      <c r="I26" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>136</v>
+      </c>
+      <c r="B27" t="s">
+        <v>128</v>
+      </c>
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" t="s">
+        <v>137</v>
+      </c>
+      <c r="E27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" t="s">
+        <v>138</v>
+      </c>
+      <c r="I27" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrections filtres débats: conseil N/S, session, layout objet
</commit_message>
<xml_diff>
--- a/Debats_CDF_EFK.xlsx
+++ b/Debats_CDF_EFK.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -20,7 +20,7 @@
     <t xml:space="preserve">MeetingDate</t>
   </si>
   <si>
-    <t xml:space="preserve">CouncilName</t>
+    <t xml:space="preserve">MeetingCouncilAbbreviation</t>
   </si>
   <si>
     <t xml:space="preserve">SpeakerFullName</t>
@@ -47,7 +47,7 @@
     <t xml:space="preserve">20251202</t>
   </si>
   <si>
-    <t xml:space="preserve">Ständerat</t>
+    <t xml:space="preserve">S</t>
   </si>
   <si>
     <t xml:space="preserve">Hegglin Peter</t>
@@ -693,7 +693,7 @@
     <t xml:space="preserve">20251208</t>
   </si>
   <si>
-    <t xml:space="preserve">Bundesrat</t>
+    <t xml:space="preserve">N</t>
   </si>
   <si>
     <t xml:space="preserve">Keller-Sutter Karin</t>
@@ -709,6 +709,83 @@
     <t xml:space="preserve">Aufgrund eines Einstellungsfehlers in der Veranlagungssoftware konnte die kantonale Steuerverwaltung Genf für rund 60 Unternehmen, die in den vorangegangenen Steuerperioden noch nicht definitiv veranlagt worden waren, keine provisorischen Rechnungen gemäss Artikel 162 des Bundesgesetzes über die direkte Bundessteuer ausstellen. Dieser technische Fehler konnte mittlerweile behoben werden, sodass nun ordnungsgemäss provisorische Rechnungen ausgestellt werden können.
 Der Gesetzgeber hat die Finanzaufsicht über die direkte Bundessteuer den 26 kantonalen Finanzkontrollen übertragen. Sie sind gehalten, jährlich die Ordnungs- und Rechtmässigkeit der Erhebung der direkten Bundessteuer und der Ablieferung des Bundesanteils zu prüfen und der Eidgenössischen Steuerverwaltung sowie der Eidgenössischen Finanzkontrolle darüber Bericht zu erstatten. Als Oberaufsicht hat die Eidgenössische Steuerverwaltung hierzu eine Richtlinie sowie ein verbindliches Prüfraster zuhanden der kantonalen Finanzkontrollen erlassen. Der erwähnte Softwarefehler wurde von der kantonalen Finanzkontrolle nicht festgestellt. Die Eidgenössische Steuerverwaltung ist derzeit daran, die Zusammenarbeit mit den kantonalen Finanzkontrollen zu intensivieren, und prüft übergeordnet, gemeinsam mit der Eidgenössischen Finanzverwaltung, weitergehende Massnahmen im Bereich der Rechnungsstellung für die direkte Bundessteuer. 
 Was die finanziellen Auswirkungen anbelangt, so steht der sogenannte Vergütungszins im Vordergrund. Dieser ist geschuldet, wenn Steuerpflichtige höhere Vorauszahlungen machen, als ihnen in Rechnung gestellt wurden. In welchem Ausmass dies tatsächlich erfolgte, kann erst bei der Erstellung der definitiven Veranlagung berechnet werden. Zu berücksichtigen ist jedoch, dass der Zinssatz für die Vergütungen tief ist: Für die primär betroffenen Kalenderjahre 2019 bis 2023 lag er bei 0,00 Prozent, für 2024 bei 1,25 Prozent und für 2025 bei 0,75 Prozent.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">365999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bürgi Roman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ich begründe meinen Minderheitsantrag zum Funktionsaufwand des Bundesamts für Polizei. Der Bundesrat beantragt ein Globalbudget von 294 Millionen Franken. Die Mehrheit der Kommission möchte diesen Betrag nun um weitere 1,8 Millionen Franken erhöhen. Die SVP-Fraktion lehnt diese Aufstockung ab und beantragt, dem Bundesrat zu folgen. 
+Aus Sicht der SVP-Fraktion ist unbestritten, dass die Bundeskriminalpolizei zusätzliche Manpower an der Front benötigt. Das steht aber nicht zur Diskussion. Die Frag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ich begründe meinen Minderheitsantrag zum Funktionsaufwand des Bundesamts für Polizei. Der Bundesrat beantragt ein Globalbudget von 294 Millionen Franken. Die Mehrheit der Kommission möchte diesen Betrag nun um weitere 1,8 Millionen Franken erhöhen. Die SVP-Fraktion lehnt diese Aufstockung ab und beantragt, dem Bundesrat zu folgen. 
+Aus Sicht der SVP-Fraktion ist unbestritten, dass die Bundeskriminalpolizei zusätzliche Manpower an der Front benötigt. Das steht aber nicht zur Diskussion. Die Frage ist vielmehr, ob wir eine strukturelle Budgeterhöhung sprechen sollen, bevor klar ist, wo und wie das Fedpol die zusätzlichen Stellen tatsächlich einsetzt. 
+Die Beratungen haben deutlich gezeigt, dass das Fedpol in der Vergangenheit primär hinsichtlich der Verwaltung und in der Kommunikation und nicht bei der operativen Kriminalpolizei ausgebaut wurde. Das Fedpol hat in den letzten Jahren Ressourcen erhalten, aber eben nicht für die Bereiche, in denen der eigentliche Bedarf besteht. Auch der EFK-Bericht bestätigt, dass intern bereits Effizienzsteigerungen im Gang und Kompensationen vorgenommen worden sind. Gleichzeitig aber bleibt unklar, weshalb genau jetzt externe Mittel über zusätzliche Stellen gesprochen werden müssen, bevor das Fedpol intern das vorhandene Potenzial ausgeschöpft hat. 
+Die Bundeskriminalpolizei verfügt heute über rund 700 Stellen, und der Bundesrat plant bereits 51 neue Stellen im Jahr 2026. Doch gemäss den Unterlagen entfallen davon nur sehr wenige auf die Ermittlungsarbeit, während der Rest für neue Projekte, für die IT-Weiterentwicklung und für die Bewirtschaftung des Verwaltungszentrums vorgesehen ist. Das hat mit der eigentlichen Kriminalbekämpfung wenig zu tun. 
+Bevor wir also zusätzliche Mittel bewilligen, erwarten wir zwei Dinge: Erstens muss das Fedpol intern jene Stellenprozente kompensieren, die es gemäss eigenen Aussagen einsparen kann, und zweitens braucht es ein klares Konzept, das detailliert aufzeigt, wo die zusätzlichen Ermittlungsstellen tatsächlich eingesetzt werden sollen. Wir fragten zu Recht, weshalb das Fedpol im ordentlichen Voranschlag nicht selbst mehr Ermittlungsstellen beantragte und weshalb im Entwicklungsrahmen zwar mehr Stellen gefordert wurden, diese dann aber nicht priorisiert wurden. Solange diese Fragen nicht beantwortet sind, ist eine Erhöhung des Budgets um 1,8 Millionen Franken nicht nachvollziehbar. Ich möchte betonen: Es geht nicht darum, die Sicherheit zu schwächen oder die Bedrohungslage zu verharmlosen. Es geht darum, dass wir zuerst sicherstellen müssen, dass die Bundesverwaltung ihre Mittel richtig einsetzt. Wenn das Fedpol erklärt, dass es intern noch Kompensationspotenzial hat, und gleichzeitig bestimmte Stellenpriorisierungen nicht vorgenommen wurden, ist es nicht sachgerecht, jetzt zusätzliches Geld zu sprechen. [PAGE 2100] 
+Der Bundesrat hat diese Abwägung gemacht und ist zum Schluss gekommen, dass 294 Millionen Franken ausreichend sind. Die SVP-Fraktion folgt dieser Einschätzung.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">366005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrey Gerhard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ja, dieser wichtige EFK-Bericht ist der Finanzkommission natürlich bekannt. Ich würde Ihnen antworten: das eine tun, das andere nicht lassen. Ich bin mit Ihnen natürlich völlig einig, dass die Ressourcen möglichst effizient eingesetzt werden müssen. Aber wenn man genau hinschaut, auch bei den anderen Staatsebenen, sieht man, dass es sich tatsächlich um ein substanzielles Ressourcenproblem handelt. Entsprechend helfen wir da mit.
+Es ist eine spezielle Situation, dass Ihre Fraktion, die Law-and-Or</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ja, dieser wichtige EFK-Bericht ist der Finanzkommission natürlich bekannt. Ich würde Ihnen antworten: das eine tun, das andere nicht lassen. Ich bin mit Ihnen natürlich völlig einig, dass die Ressourcen möglichst effizient eingesetzt werden müssen. Aber wenn man genau hinschaut, auch bei den anderen Staatsebenen, sieht man, dass es sich tatsächlich um ein substanzielles Ressourcenproblem handelt. Entsprechend helfen wir da mit.
+Es ist eine spezielle Situation, dass Ihre Fraktion, die Law-and-Order-Fraktion, hier kritisch ist, wo es um mehr Polizei geht, und wir mit der Kommissionsmehrheit dafür sind. Das ist eine interessante Ausgangslage. Aber ich würde auf jeden Fall meinen: das eine tun, das andere nicht lassen.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">366006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fischer Benjamin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geschätzter Kollege Andrey, ist Ihnen der EFK-Prüfbericht zur Ressourcensituation des Fedpol bekannt? Darin stellt die Eidgenössische Finanzkontrolle Mängel fest und hält auch klar fest, dass es ein Ressourcenproblem, aber auch ein grosses Potenzial gebe und[NB]man[NB]zuerst[NB]intern diese Ressourcen freispielen müsse, bevor das Parlament für das Fedpol wieder zusätzliche Gelder spricht. [PAGE 2103] 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">366067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bürgin Yvonne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ich spreche für die Mitte-Fraktion. Die Mitte. EVP zu Block 2, "Justiz, Sicherheit und Migration". Dieser Block betrifft zentrale Aufgaben unseres Staates, den Schutz des Rechtsstaats, die innere Sicherheit, die Cyberresilienz und die Steuerung der Migration. Unsere Haltung ist klar und ziemlich einfach. Wir unterstützen alle Mehrheitsanträge der Finanzkommission und lehnen alle Minderheitsanträge ab.
+Ein Punkt ist uns besonders wichtig. Neue Stellen betrachten wir grundsätzlich kritisch. Die Ve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ich spreche für die Mitte-Fraktion. Die Mitte. EVP zu Block 2, "Justiz, Sicherheit und Migration". Dieser Block betrifft zentrale Aufgaben unseres Staates, den Schutz des Rechtsstaats, die innere Sicherheit, die Cyberresilienz und die Steuerung der Migration. Unsere Haltung ist klar und ziemlich einfach. Wir unterstützen alle Mehrheitsanträge der Finanzkommission und lehnen alle Minderheitsanträge ab.
+Ein Punkt ist uns besonders wichtig. Neue Stellen betrachten wir grundsätzlich kritisch. Die Verwaltung wächst seit Jahren. Es braucht Prioritäten und Effizienz, nicht reflexartige Aufstockungen. Gleichzeitig gilt: Wo Sicherheit und Funktionsfähigkeit des Staates gefährdet sind, müssen wir handeln. Das betrifft insbesondere das Fedpol und das Bundesamt für Cybersicherheit (BACS). Dort unterstützen wir zusätzliche Stellen ausdrücklich. Und ich möchte auch noch eine Antwort auf die Frage von vorhin von Herrn Fischer an Herrn Andrey geben: Ja, intern wurde schon sehr viel gemacht, aber das Fedpol braucht mehr Stellen.
+Beim Budget müssen aber auch die Einnahmen betrachtet werden. Wir unterstützen eine Erhöhung, und zwar mithilfe der eingezogenen Vermögenswerte beim Bundesamt für Justiz. Die realisierten Werte lagen in den letzten Jahren regelmässig über dem Budget. Mit diesem Durchschnittswert der Vergangenheit ist eine realistische Planung möglich.
+Beim Staatssekretariat für Migration sehen wir die bekannten Dynamiken. Die Sozialhilfekosten im Asylbereich hängen direkt von den Zugangszahlen ab. Bei den Beiträgen an die Kantone bezüglich der Ukraine-Flüchtlinge sind die Zahlen stabil, aber ein Teil der Kosten wird immer noch ausserordentlich verbucht. Wir unterstützen den Ansatz, dass diese Finanzierung schrittweise ins ordentliche Budget zu überführen ist. Gleich auf null zu gehen, geht uns zu weit. Wir möchten den Antrag unterstützen, dies entsprechend dem Beschluss des Ständerates schneller zu tun, d.[NB]h., nur 470 Millionen statt 600 Millionen Franken ausserordentlich zu verbuchen. Die dadurch ordentlich verbuchten 130 Millionen Franken kompensieren wir beim Kredit "Sozialhilfe Asylsuchende, vorläufig Aufgenommene, Flüchtlinge"; dies ist aufgrund der Erwartung tieferer Zugangszahlen möglich.
+Kern dieses Blocks ist die Sicherheit. Beim Fedpol zeigt sich klar: Wir wollen nicht einfach kürzen, wir wollen dort stärken, wo es nötig ist. Der Personalbestand, besonders bei der Bundeskriminalpolizei, ist zu tief. Das belegen der EFK-Bericht, die Antwort auf das Postulat der Finanzkommission und weitere Unterlagen eindeutig. Die Bekämpfung der Schwerstkriminalität ist gefährdet. Operativ ist eine Aufstockung schon 2026 möglich. Der Bundesrat plant sie erst ab 2027. Wir, die Mitte-Fraktion. Die Mitte. EVP, unterstützen die Erhöhung um 1,8 Millionen Franken für 10 zusätzliche Ermittlerstellen bereits ab nächstem Jahr sowie einen gestaffelten Ausbau ab 2027 zur Stärkung der inneren Sicherheit. Ein Zuwarten wäre fahrlässig. 
+Ähnlich ist es beim BACS. Die Cyberbedrohungslage verschärft sich massiv, und zentrale Wirtschaftssektoren benötigen Unterstützung. Auch hier zeigt ein Zusatzbericht klar Handlungsbedarf. Wir unterstützen auch hier eine Aufstockung um zusätzliche 10 Millionen Franken im Funktionsaufwand zur Stärkung der Cyberresilienz.
+Bei der Verteidigung geht es um die Umsetzung des parlamentarischen Auftrags des letzten Jahres: mehr Rüstungsinvestitionen und tiefere Betriebsausgaben durch Effizienzmassnahmen. Wir unterstützen den Antrag, bei der Position "Rüstungsaufwand und -investitionen" 50 Millionen Franken mehr zu sprechen und 25 Millionen Franken bei der Position "Funktionsaufwand (Globalbudget)" zu kompensieren oder zu sparen. Der Ständerat möchte weiter gehen. Er möchte 70 Millionen Franken zusätzlich investieren. Hier liegt nun auch der Einzelantrag Nause vor. Angesichts der sicherheitspolitischen Lage und Bedrohung - Stichwort Drohnen über Belgien, Deutschland, Dänemark und sogar auch über der Schweiz, über dem Flugplatz Meiringen - müssen wir bei den Investitionen tatsächlich einen Zacken zulegen. Wir unterstützen den Einzelantrag Nause, zusätzliche 70 Millionen Franken bereits in diesem Budget einzustellen. Der Pfad, 1 Prozent des BIP bis 2032 für die Armee aufzuwenden, bleibt unverändert.
+Die Mitte-Fraktion steht für eine verantwortungsvolle Finanzpolitik. Wir sparen dort, wo es möglich ist, und investieren dort, wo es für Sicherheit und Stabilität notwendig ist.
 </t>
   </si>
   <si>
@@ -734,157 +811,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">365999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nationalrat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bürgi Roman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ich begründe meinen Minderheitsantrag zum Funktionsaufwand des Bundesamts für Polizei. Der Bundesrat beantragt ein Globalbudget von 294 Millionen Franken. Die Mehrheit der Kommission möchte diesen Betrag nun um weitere 1,8 Millionen Franken erhöhen. Die SVP-Fraktion lehnt diese Aufstockung ab und beantragt, dem Bundesrat zu folgen. 
-Aus Sicht der SVP-Fraktion ist unbestritten, dass die Bundeskriminalpolizei zusätzliche Manpower an der Front benötigt. Das steht aber nicht zur Diskussion. Die Frag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ich begründe meinen Minderheitsantrag zum Funktionsaufwand des Bundesamts für Polizei. Der Bundesrat beantragt ein Globalbudget von 294 Millionen Franken. Die Mehrheit der Kommission möchte diesen Betrag nun um weitere 1,8 Millionen Franken erhöhen. Die SVP-Fraktion lehnt diese Aufstockung ab und beantragt, dem Bundesrat zu folgen. 
-Aus Sicht der SVP-Fraktion ist unbestritten, dass die Bundeskriminalpolizei zusätzliche Manpower an der Front benötigt. Das steht aber nicht zur Diskussion. Die Frage ist vielmehr, ob wir eine strukturelle Budgeterhöhung sprechen sollen, bevor klar ist, wo und wie das Fedpol die zusätzlichen Stellen tatsächlich einsetzt. 
-Die Beratungen haben deutlich gezeigt, dass das Fedpol in der Vergangenheit primär hinsichtlich der Verwaltung und in der Kommunikation und nicht bei der operativen Kriminalpolizei ausgebaut wurde. Das Fedpol hat in den letzten Jahren Ressourcen erhalten, aber eben nicht für die Bereiche, in denen der eigentliche Bedarf besteht. Auch der EFK-Bericht bestätigt, dass intern bereits Effizienzsteigerungen im Gang und Kompensationen vorgenommen worden sind. Gleichzeitig aber bleibt unklar, weshalb genau jetzt externe Mittel über zusätzliche Stellen gesprochen werden müssen, bevor das Fedpol intern das vorhandene Potenzial ausgeschöpft hat. 
-Die Bundeskriminalpolizei verfügt heute über rund 700 Stellen, und der Bundesrat plant bereits 51 neue Stellen im Jahr 2026. Doch gemäss den Unterlagen entfallen davon nur sehr wenige auf die Ermittlungsarbeit, während der Rest für neue Projekte, für die IT-Weiterentwicklung und für die Bewirtschaftung des Verwaltungszentrums vorgesehen ist. Das hat mit der eigentlichen Kriminalbekämpfung wenig zu tun. 
-Bevor wir also zusätzliche Mittel bewilligen, erwarten wir zwei Dinge: Erstens muss das Fedpol intern jene Stellenprozente kompensieren, die es gemäss eigenen Aussagen einsparen kann, und zweitens braucht es ein klares Konzept, das detailliert aufzeigt, wo die zusätzlichen Ermittlungsstellen tatsächlich eingesetzt werden sollen. Wir fragten zu Recht, weshalb das Fedpol im ordentlichen Voranschlag nicht selbst mehr Ermittlungsstellen beantragte und weshalb im Entwicklungsrahmen zwar mehr Stellen gefordert wurden, diese dann aber nicht priorisiert wurden. Solange diese Fragen nicht beantwortet sind, ist eine Erhöhung des Budgets um 1,8 Millionen Franken nicht nachvollziehbar. Ich möchte betonen: Es geht nicht darum, die Sicherheit zu schwächen oder die Bedrohungslage zu verharmlosen. Es geht darum, dass wir zuerst sicherstellen müssen, dass die Bundesverwaltung ihre Mittel richtig einsetzt. Wenn das Fedpol erklärt, dass es intern noch Kompensationspotenzial hat, und gleichzeitig bestimmte Stellenpriorisierungen nicht vorgenommen wurden, ist es nicht sachgerecht, jetzt zusätzliches Geld zu sprechen. [PAGE 2100] 
-Der Bundesrat hat diese Abwägung gemacht und ist zum Schluss gekommen, dass 294 Millionen Franken ausreichend sind. Die SVP-Fraktion folgt dieser Einschätzung.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">366005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andrey Gerhard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ja, dieser wichtige EFK-Bericht ist der Finanzkommission natürlich bekannt. Ich würde Ihnen antworten: das eine tun, das andere nicht lassen. Ich bin mit Ihnen natürlich völlig einig, dass die Ressourcen möglichst effizient eingesetzt werden müssen. Aber wenn man genau hinschaut, auch bei den anderen Staatsebenen, sieht man, dass es sich tatsächlich um ein substanzielles Ressourcenproblem handelt. Entsprechend helfen wir da mit.
-Es ist eine spezielle Situation, dass Ihre Fraktion, die Law-and-Or</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ja, dieser wichtige EFK-Bericht ist der Finanzkommission natürlich bekannt. Ich würde Ihnen antworten: das eine tun, das andere nicht lassen. Ich bin mit Ihnen natürlich völlig einig, dass die Ressourcen möglichst effizient eingesetzt werden müssen. Aber wenn man genau hinschaut, auch bei den anderen Staatsebenen, sieht man, dass es sich tatsächlich um ein substanzielles Ressourcenproblem handelt. Entsprechend helfen wir da mit.
-Es ist eine spezielle Situation, dass Ihre Fraktion, die Law-and-Order-Fraktion, hier kritisch ist, wo es um mehr Polizei geht, und wir mit der Kommissionsmehrheit dafür sind. Das ist eine interessante Ausgangslage. Aber ich würde auf jeden Fall meinen: das eine tun, das andere nicht lassen.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">366006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fischer Benjamin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geschätzter Kollege Andrey, ist Ihnen der EFK-Prüfbericht zur Ressourcensituation des Fedpol bekannt? Darin stellt die Eidgenössische Finanzkontrolle Mängel fest und hält auch klar fest, dass es ein Ressourcenproblem, aber auch ein grosses Potenzial gebe und[NB]man[NB]zuerst[NB]intern diese Ressourcen freispielen müsse, bevor das Parlament für das Fedpol wieder zusätzliche Gelder spricht. [PAGE 2103] 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">366067</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bürgin Yvonne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ich spreche für die Mitte-Fraktion. Die Mitte. EVP zu Block 2, "Justiz, Sicherheit und Migration". Dieser Block betrifft zentrale Aufgaben unseres Staates, den Schutz des Rechtsstaats, die innere Sicherheit, die Cyberresilienz und die Steuerung der Migration. Unsere Haltung ist klar und ziemlich einfach. Wir unterstützen alle Mehrheitsanträge der Finanzkommission und lehnen alle Minderheitsanträge ab.
-Ein Punkt ist uns besonders wichtig. Neue Stellen betrachten wir grundsätzlich kritisch. Die Ve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ich spreche für die Mitte-Fraktion. Die Mitte. EVP zu Block 2, "Justiz, Sicherheit und Migration". Dieser Block betrifft zentrale Aufgaben unseres Staates, den Schutz des Rechtsstaats, die innere Sicherheit, die Cyberresilienz und die Steuerung der Migration. Unsere Haltung ist klar und ziemlich einfach. Wir unterstützen alle Mehrheitsanträge der Finanzkommission und lehnen alle Minderheitsanträge ab.
-Ein Punkt ist uns besonders wichtig. Neue Stellen betrachten wir grundsätzlich kritisch. Die Verwaltung wächst seit Jahren. Es braucht Prioritäten und Effizienz, nicht reflexartige Aufstockungen. Gleichzeitig gilt: Wo Sicherheit und Funktionsfähigkeit des Staates gefährdet sind, müssen wir handeln. Das betrifft insbesondere das Fedpol und das Bundesamt für Cybersicherheit (BACS). Dort unterstützen wir zusätzliche Stellen ausdrücklich. Und ich möchte auch noch eine Antwort auf die Frage von vorhin von Herrn Fischer an Herrn Andrey geben: Ja, intern wurde schon sehr viel gemacht, aber das Fedpol braucht mehr Stellen.
-Beim Budget müssen aber auch die Einnahmen betrachtet werden. Wir unterstützen eine Erhöhung, und zwar mithilfe der eingezogenen Vermögenswerte beim Bundesamt für Justiz. Die realisierten Werte lagen in den letzten Jahren regelmässig über dem Budget. Mit diesem Durchschnittswert der Vergangenheit ist eine realistische Planung möglich.
-Beim Staatssekretariat für Migration sehen wir die bekannten Dynamiken. Die Sozialhilfekosten im Asylbereich hängen direkt von den Zugangszahlen ab. Bei den Beiträgen an die Kantone bezüglich der Ukraine-Flüchtlinge sind die Zahlen stabil, aber ein Teil der Kosten wird immer noch ausserordentlich verbucht. Wir unterstützen den Ansatz, dass diese Finanzierung schrittweise ins ordentliche Budget zu überführen ist. Gleich auf null zu gehen, geht uns zu weit. Wir möchten den Antrag unterstützen, dies entsprechend dem Beschluss des Ständerates schneller zu tun, d.[NB]h., nur 470 Millionen statt 600 Millionen Franken ausserordentlich zu verbuchen. Die dadurch ordentlich verbuchten 130 Millionen Franken kompensieren wir beim Kredit "Sozialhilfe Asylsuchende, vorläufig Aufgenommene, Flüchtlinge"; dies ist aufgrund der Erwartung tieferer Zugangszahlen möglich.
-Kern dieses Blocks ist die Sicherheit. Beim Fedpol zeigt sich klar: Wir wollen nicht einfach kürzen, wir wollen dort stärken, wo es nötig ist. Der Personalbestand, besonders bei der Bundeskriminalpolizei, ist zu tief. Das belegen der EFK-Bericht, die Antwort auf das Postulat der Finanzkommission und weitere Unterlagen eindeutig. Die Bekämpfung der Schwerstkriminalität ist gefährdet. Operativ ist eine Aufstockung schon 2026 möglich. Der Bundesrat plant sie erst ab 2027. Wir, die Mitte-Fraktion. Die Mitte. EVP, unterstützen die Erhöhung um 1,8 Millionen Franken für 10 zusätzliche Ermittlerstellen bereits ab nächstem Jahr sowie einen gestaffelten Ausbau ab 2027 zur Stärkung der inneren Sicherheit. Ein Zuwarten wäre fahrlässig. 
-Ähnlich ist es beim BACS. Die Cyberbedrohungslage verschärft sich massiv, und zentrale Wirtschaftssektoren benötigen Unterstützung. Auch hier zeigt ein Zusatzbericht klar Handlungsbedarf. Wir unterstützen auch hier eine Aufstockung um zusätzliche 10 Millionen Franken im Funktionsaufwand zur Stärkung der Cyberresilienz.
-Bei der Verteidigung geht es um die Umsetzung des parlamentarischen Auftrags des letzten Jahres: mehr Rüstungsinvestitionen und tiefere Betriebsausgaben durch Effizienzmassnahmen. Wir unterstützen den Antrag, bei der Position "Rüstungsaufwand und -investitionen" 50 Millionen Franken mehr zu sprechen und 25 Millionen Franken bei der Position "Funktionsaufwand (Globalbudget)" zu kompensieren oder zu sparen. Der Ständerat möchte weiter gehen. Er möchte 70 Millionen Franken zusätzlich investieren. Hier liegt nun auch der Einzelantrag Nause vor. Angesichts der sicherheitspolitischen Lage und Bedrohung - Stichwort Drohnen über Belgien, Deutschland, Dänemark und sogar auch über der Schweiz, über dem Flugplatz Meiringen - müssen wir bei den Investitionen tatsächlich einen Zacken zulegen. Wir unterstützen den Einzelantrag Nause, zusätzliche 70 Millionen Franken bereits in diesem Budget einzustellen. Der Pfad, 1 Prozent des BIP bis 2032 für die Armee aufzuwenden, bleibt unverändert.
-Die Mitte-Fraktion steht für eine verantwortungsvolle Finanzpolitik. Wir sparen dort, wo es möglich ist, und investieren dort, wo es für Sicherheit und Stabilität notwendig ist.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">367087</t>
+    <t xml:space="preserve">367075</t>
   </si>
   <si>
     <t xml:space="preserve">20251211</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jans Beat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mit dieser Motion ist ja vorgesehen, dass die Bundeskriminalpolizei (BKP) personell etappenweise verstärkt wird. Aus unserer Sicht ist das zwingend nötig. Sie und der Nationalrat sehen das erfreulicherweise gleich. Sie haben an der diesjährigen Budgetberatung in beiden Räten beschlossen, dass das Fedpol für das Jahr 2026 vorbehältlich der Schlussabstimmung 1,8 Millionen Franken mehr personelle Mittel bekommt; das entspricht zehn Ermittlerinnen und Ermittlern für die BKP. Das ist ein wichtiger Sc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mit dieser Motion ist ja vorgesehen, dass die Bundeskriminalpolizei (BKP) personell etappenweise verstärkt wird. Aus unserer Sicht ist das zwingend nötig. Sie und der Nationalrat sehen das erfreulicherweise gleich. Sie haben an der diesjährigen Budgetberatung in beiden Räten beschlossen, dass das Fedpol für das Jahr 2026 vorbehältlich der Schlussabstimmung 1,8 Millionen Franken mehr personelle Mittel bekommt; das entspricht zehn Ermittlerinnen und Ermittlern für die BKP. Das ist ein wichtiger Schritt hin zu einer wirksameren Bekämpfung der Schwerkriminalität. 
-Der Bundesrat will für den Aufbau der Bundeskriminalpolizei aber eben die ordentlichen Prozesse nutzen. Das heisst, eine solche personelle Verstärkung müssen wir als EJPD in den ordentlichen Budgetprozess eingeben und eine Genehmigung beantragen. Deshalb empfiehlt der Bundesrat die vorliegende Motion zur Ablehnung. Das heisst aber auch, Herr Salzmann, dass der Bundesrat dann Anfang 2026 über Prioritäten entscheiden muss; denn es ist jetzt schon klar, dass die verfügbaren Ressourcen bei Weitem nicht genügen, um alle Stellenanträge der Departemente zu erfüllen. Sollte der Bundesrat eine Erhöhung der Stellen bei der BKP genehmigen, wie wir das als EJPD beantragen - auch aufgrund der verschiedenen Berichte, die uns zugrunde liegen -, so würden die entsprechenden Mittel aber in jedem Fall frühestens 2027 zur Verfügung stehen. Mit zusätzlichen Ressourcen für das Fedpol und namentlich für die BKP, gestaffelt über die nächsten Jahre, können gezielt Stellen geschaffen werden - dort, wo die Not am grössten ist und wo sie den grössten Beitrag zur Sicherheit leisten. Mir als Departementsvorsteher ist es ein wichtiges Anliegen, dass wir klar darlegen können, wofür genau es diese Stellen braucht, welchen Nutzen sie haben und wie wir die Prioritäten entsprechend setzen. Wir sind gemeinsam auf diesem Weg, die innere Sicherheit dort, wo es ihrer bedarf, zu stärken. 
-Ich möchte mich aber gegen die Vorwürfe, dass strategisches oder konzeptionelles Vorgehen fehlt, doch ein bisschen wehren, Herr Hegglin. Der EFK-Bericht war für mich zwingend. Bevor ich überhaupt Stellen beantrage, wollte ich diesen Bericht hören und sehen. Ich gehöre nicht zu den Departementsvorstehern, die in den letzten Jahren einfach gesagt haben: "Wir brauchen, wir brauchen, und wir stellen ein", sondern ich habe gesagt, dass wir das anders machen müssen, dass wir das abstützen müssen, dass wir das strategisch korrekt machen müssen. Da haben wir eben von der EFK klar - und das gibt es selten - den Hinweis erhalten, dass die BKP zusätzliche Mittel braucht, um in der aktuellen Situation die Aufgaben zu erfüllen; das ist klar. Sie sagt aber auch, dass wir eine Reorganisation machen müssen, dass wir auch Stellen im Bereich Kopf wegnehmen müssen und in den Bereich der Ermittler bringen. Auch das gehen wir an, die neue Fedpol-Leitung ist an diesem Vorhaben dran. Das sind nicht einfache Entscheide, das wissen Sie auch; man kann Leute nicht einfach von einem Tag auf den anderen zu Spezialisten machen. Das sind anstrengende, wichtige Prozesse, die wir sehr ernst nehmen. Also wir sind da unterwegs. 
-Aber was ich wirklich wichtig finde, ist, dass wir das alle sehen, auch Sie bitte, Herr Rieder: Der Bedarf ist da, und das ist nicht nur mit diesen neuesten Statistiken zu erfassen. Wir haben heute ein ganz anderes Lagebild, das sagt uns Europol in all ihren Untersuchungen. Wir haben verschiedene Länder, die es verpasst haben, rechtzeitig gegen die organisierte Kriminalität vorzugehen. Diese haben auch Unterlassungen gemacht und sind in ihren Strafverfahren zu wenig [PAGE 1322] streng gewesen. Das hat dazu geführt, dass sie heute zum Teil - ich rede jetzt von Holland, ich rede von Dänemark und von Schweden - offene Bandenkriminalität in ihren Städten bekämpfen müssen.
-Wenn Sie damit zu spät anfangen oder spät anfangen, kann es sein, dass Sie dann zu spät sind. Das ist das, was mir die EU-Innenminister letzte Woche alle gesagt haben. Da müssen wir rechtzeitig sein, und da müssen wir genau hinschauen. Die Schweiz ist als Finanzplatz für die organisierte Kriminalität exponiert. Wir werden mit dieser Strategie kommen, und zwar schon sehr bald: erstens mit der Sicherheitsstrategie und darin eingebettet mit der Strategie für organisierte Kriminalität. Wir werden zweitens - das ist Teil dieser Strategie - Gesetzesänderungen vorschlagen, um den Strafverfolgungsbehörden auch bessere Instrumente an die Hand zu geben, nicht nur mehr Personal. Das ist etwas, das wir feststellen: Die Fälle insbesondere zur Bekämpfung der organisierten Kriminalität sind auch sehr viel komplizierter geworden.
-Der Bundesanwalt, mit dem ich heute Morgen noch telefonieren konnte, begrüsst es sehr, dass es für Fälle, die er zum Teil heute einfach nicht bewältigen kann, mehr Ermittler geben soll, Fälle, bei denen er zum Teil bis zu 20 oder sogar mehr Ermittler braucht - das für einen einzigen Fall. Sie stellen sich wahrscheinlich immer vor, ein Fall, ein Ermittler. Das ist leider nicht so. Die Fälle sind unglaublich kompliziert, und gerade die Netzwerke der organisierten Kriminalität nehmen ihre Verteidigungsrechte, die sie mit der Strafprozessordnung neu erhalten haben, sehr exzessiv wahr. Die machen mit einem Heer von besten Anwälten alles, um die Prozesse zu verlängern und komplizierter zu machen, um weitere Berichte und Untersuchungen einzufordern. Das ist die Realität, der wir uns stellen müssen. Diese wurde noch durch die Tatsache verschärft - das ist ganz wichtig, was Frau Gmür-Schönenberger gesagt hat -, dass die organisierte Kriminalität im Internet stattfindet. Dort müssen wir besser werden. Es ist enorm kompliziert und aufwendig, die grenzüberschreitend im virtuellen Bereich tätigen Banden zu knacken. Aber es ist wegen des Risikos für die Sicherheit unserer Bevölkerung, aber auch wegen des Image unseres Landes, wegen der Reputation, die auf der Kippe steht, unglaublich wichtig. 
-Deshalb ist es wichtig, dass wir hier vorangehen und dass wir schrittweise vorgehen. Der Bundesrat braucht diese Motion nicht dafür, wir werden diese Entscheide schrittweise im Rahmen der ordentlichen Budgetprozesse fällen, aber es ist wichtig, das möchte ich doch noch sagen, dass Sie den Handlungsbedarf wirklich erkennen.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">367062</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conseil des Etats</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juillard Charles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Je vais m'exprimer en tant que membre de la Commission de la politique de sécurité, mais aussi en tant que membre et ancien président de la Commission de gestion, puisque nous avons abordé la question des effectifs de Fedpol à plusieurs reprises lors des séances de la Commission de gestion, et que nous sommes arrivés à la conclusion qu'il y avait un vrai problème d'effectifs concernant les enquêteurs de Fedpol. C'est aussi dans cet esprit que nous avons écrit au Conseil fédéral pour qu'il envisa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Je vais m'exprimer en tant que membre de la Commission de la politique de sécurité, mais aussi en tant que membre et ancien président de la Commission de gestion, puisque nous avons abordé la question des effectifs de Fedpol à plusieurs reprises lors des séances de la Commission de gestion, et que nous sommes arrivés à la conclusion qu'il y avait un vrai problème d'effectifs concernant les enquêteurs de Fedpol. C'est aussi dans cet esprit que nous avons écrit au Conseil fédéral pour qu'il envisage l'augmentation des effectifs, ce qui va dans le même sens que cette motion. Je dois cependant vous dire que nous n'avons pas examiné dans le détail si ces postes supplémentaires, - ces postes d'enquêteurs, parce que c'est surtout là qu'il y a un problème -, pouvaient être en tout ou partie compensés par une réorganisation de Fedpol - qui s'impose, selon le Contrôle fédéral des finances -, et s'il serait possible de diminuer les postes dans le domaine administratif pour les concentrer sur le terrain, là où les besoins se font particulièrement sentir, si l'on écoute aussi le Ministère public de la Confédération. Je voulais vous donner ces informations.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">367096</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sommaruga Carlo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Je prends la parole en tant que président de la sous-commission de la Commission de gestion qui s'occupe du DFJP et de la Chancellerie fédérale. Ce sujet, nous l'avons traité à plusieurs reprises et le faisons depuis fort longtemps. Nous avons entendu le procureur général de la Confédération, nous avons entendu l'ancienne et la nouvelle directrice de Fedpol et différentes autres personnes. Sur cette base-là, nous avons pu constater de manière claire que les personnes entendues relevaient qu'il y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Je prends la parole en tant que président de la sous-commission de la Commission de gestion qui s'occupe du DFJP et de la Chancellerie fédérale. Ce sujet, nous l'avons traité à plusieurs reprises et le faisons depuis fort longtemps. Nous avons entendu le procureur général de la Confédération, nous avons entendu l'ancienne et la nouvelle directrice de Fedpol et différentes autres personnes. Sur cette base-là, nous avons pu constater de manière claire que les personnes entendues relevaient qu'il y a aujourd'hui un déficit de personnel pour assurer la sécurité de la Suisse au niveau des infractions qui sont de la compétence fédérale et donc de la compétence du DFJP.
-J'entends bien les chiffres de notre collègue Rieder, mais ces chiffres ne reflètent pas la réalité qui nous est décrite par le procureur général de la Confédération et dont les termes ont été rappelés par notre collègue Dittli, à savoir que, aujourd'hui, il y a des procédures pénales concernant surtout la criminalité organisée internationale qui ne peuvent pas être ouvertes parce qu'il n'y a pas assez de personnel spécialisé. Je pense que cet élément doit être pris en compte.
-Si cette motion est aujourd'hui sur la table, c'est parce qu'il y a non seulement le rapport du Contrôle fédéral des finances, mais également des rapports de la Commission de gestion. Ce sont des éléments essentiels, et j'avoue que je suis surpris que l'on conteste les travaux faits par la Commission de gestion, et au Conseil national et au Conseil des États, sur la situation au niveau du procureur général et au niveau de Fedpol.
-J'aimerais juste dire que l'élément central qui a été évoqué par notre collègue, ce n'est pas la stabilité des plaintes ou des procédures qui ont été ouvertes de manière générale, c'est la criminalité organisée. Il a confirmé qu'il y avait une augmentation de 8 pour cent des affaires. Or, ce ne sont pas seulement les chiffres qu'il faut regarder, mais aussi la complexité des procédures qui sont ouvertes. Aujourd'hui, elles sont de plus en plus complexes dans le cadre de la poursuite pénale.
-J'aimerais juste relever que ce ne sont pas seulement des gigabits ou des mégabits qu'il faut examiner dans le cadre de toutes ces saisies de données faites en rapport avec la criminalité organisée, mais aussi les boîtes mail et les téléphones cryptés, et que cela nécessite des spécialistes. Aujourd'hui, le problème est immédiat. Il n'y a pas lieu d'attendre ou de compter sur le fait que des personnes vont partir à la retraite, même dans d'autres domaines, pour pouvoir engager du personnel.
-Je prends juste un exemple[NB]: il n'y a pas très longtemps, Fedpol a dû s'occuper d'un cas très particulier, celui des bombes qui avaient été placées pour faire chanter Patek Philippe. Pour rappel, cela s'est passé à Genève. Des bombes artisanales ont été mises dans des boîtes aux lettres et il y a eu des blessés. Il a fallu déployer des moyens extrêmement importants, non seulement à Genève, mais également au niveau de Fedpol qui disposait de spécialiste, pour enfin trouver la personne responsable de ces actes. J'aimerais relever que ce sont aussi des procédures qui, en général, demandent beaucoup, beaucoup de ressources humaines, et des ressources humaines spécialisées.
-Dès lors, je veux simplement vous dire que si l'on veut avoir une sécurité de la Suisse non seulement extérieure mais aussi intérieure, je crois qu'il faut entendre le message qui nous est donné par Fedpol, par le procureur général et par la Commission de gestion.
-Je vous invite donc à accepter cette motion, comme le propose la majorité de la commission.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">367075</t>
   </si>
   <si>
     <t xml:space="preserve">Gmür-Schönenberger Andrea</t>
@@ -925,6 +855,28 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">367087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jans Beat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mit dieser Motion ist ja vorgesehen, dass die Bundeskriminalpolizei (BKP) personell etappenweise verstärkt wird. Aus unserer Sicht ist das zwingend nötig. Sie und der Nationalrat sehen das erfreulicherweise gleich. Sie haben an der diesjährigen Budgetberatung in beiden Räten beschlossen, dass das Fedpol für das Jahr 2026 vorbehältlich der Schlussabstimmung 1,8 Millionen Franken mehr personelle Mittel bekommt; das entspricht zehn Ermittlerinnen und Ermittlern für die BKP. Das ist ein wichtiger Sc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mit dieser Motion ist ja vorgesehen, dass die Bundeskriminalpolizei (BKP) personell etappenweise verstärkt wird. Aus unserer Sicht ist das zwingend nötig. Sie und der Nationalrat sehen das erfreulicherweise gleich. Sie haben an der diesjährigen Budgetberatung in beiden Räten beschlossen, dass das Fedpol für das Jahr 2026 vorbehältlich der Schlussabstimmung 1,8 Millionen Franken mehr personelle Mittel bekommt; das entspricht zehn Ermittlerinnen und Ermittlern für die BKP. Das ist ein wichtiger Schritt hin zu einer wirksameren Bekämpfung der Schwerkriminalität. 
+Der Bundesrat will für den Aufbau der Bundeskriminalpolizei aber eben die ordentlichen Prozesse nutzen. Das heisst, eine solche personelle Verstärkung müssen wir als EJPD in den ordentlichen Budgetprozess eingeben und eine Genehmigung beantragen. Deshalb empfiehlt der Bundesrat die vorliegende Motion zur Ablehnung. Das heisst aber auch, Herr Salzmann, dass der Bundesrat dann Anfang 2026 über Prioritäten entscheiden muss; denn es ist jetzt schon klar, dass die verfügbaren Ressourcen bei Weitem nicht genügen, um alle Stellenanträge der Departemente zu erfüllen. Sollte der Bundesrat eine Erhöhung der Stellen bei der BKP genehmigen, wie wir das als EJPD beantragen - auch aufgrund der verschiedenen Berichte, die uns zugrunde liegen -, so würden die entsprechenden Mittel aber in jedem Fall frühestens 2027 zur Verfügung stehen. Mit zusätzlichen Ressourcen für das Fedpol und namentlich für die BKP, gestaffelt über die nächsten Jahre, können gezielt Stellen geschaffen werden - dort, wo die Not am grössten ist und wo sie den grössten Beitrag zur Sicherheit leisten. Mir als Departementsvorsteher ist es ein wichtiges Anliegen, dass wir klar darlegen können, wofür genau es diese Stellen braucht, welchen Nutzen sie haben und wie wir die Prioritäten entsprechend setzen. Wir sind gemeinsam auf diesem Weg, die innere Sicherheit dort, wo es ihrer bedarf, zu stärken. 
+Ich möchte mich aber gegen die Vorwürfe, dass strategisches oder konzeptionelles Vorgehen fehlt, doch ein bisschen wehren, Herr Hegglin. Der EFK-Bericht war für mich zwingend. Bevor ich überhaupt Stellen beantrage, wollte ich diesen Bericht hören und sehen. Ich gehöre nicht zu den Departementsvorstehern, die in den letzten Jahren einfach gesagt haben: "Wir brauchen, wir brauchen, und wir stellen ein", sondern ich habe gesagt, dass wir das anders machen müssen, dass wir das abstützen müssen, dass wir das strategisch korrekt machen müssen. Da haben wir eben von der EFK klar - und das gibt es selten - den Hinweis erhalten, dass die BKP zusätzliche Mittel braucht, um in der aktuellen Situation die Aufgaben zu erfüllen; das ist klar. Sie sagt aber auch, dass wir eine Reorganisation machen müssen, dass wir auch Stellen im Bereich Kopf wegnehmen müssen und in den Bereich der Ermittler bringen. Auch das gehen wir an, die neue Fedpol-Leitung ist an diesem Vorhaben dran. Das sind nicht einfache Entscheide, das wissen Sie auch; man kann Leute nicht einfach von einem Tag auf den anderen zu Spezialisten machen. Das sind anstrengende, wichtige Prozesse, die wir sehr ernst nehmen. Also wir sind da unterwegs. 
+Aber was ich wirklich wichtig finde, ist, dass wir das alle sehen, auch Sie bitte, Herr Rieder: Der Bedarf ist da, und das ist nicht nur mit diesen neuesten Statistiken zu erfassen. Wir haben heute ein ganz anderes Lagebild, das sagt uns Europol in all ihren Untersuchungen. Wir haben verschiedene Länder, die es verpasst haben, rechtzeitig gegen die organisierte Kriminalität vorzugehen. Diese haben auch Unterlassungen gemacht und sind in ihren Strafverfahren zu wenig [PAGE 1322] streng gewesen. Das hat dazu geführt, dass sie heute zum Teil - ich rede jetzt von Holland, ich rede von Dänemark und von Schweden - offene Bandenkriminalität in ihren Städten bekämpfen müssen.
+Wenn Sie damit zu spät anfangen oder spät anfangen, kann es sein, dass Sie dann zu spät sind. Das ist das, was mir die EU-Innenminister letzte Woche alle gesagt haben. Da müssen wir rechtzeitig sein, und da müssen wir genau hinschauen. Die Schweiz ist als Finanzplatz für die organisierte Kriminalität exponiert. Wir werden mit dieser Strategie kommen, und zwar schon sehr bald: erstens mit der Sicherheitsstrategie und darin eingebettet mit der Strategie für organisierte Kriminalität. Wir werden zweitens - das ist Teil dieser Strategie - Gesetzesänderungen vorschlagen, um den Strafverfolgungsbehörden auch bessere Instrumente an die Hand zu geben, nicht nur mehr Personal. Das ist etwas, das wir feststellen: Die Fälle insbesondere zur Bekämpfung der organisierten Kriminalität sind auch sehr viel komplizierter geworden.
+Der Bundesanwalt, mit dem ich heute Morgen noch telefonieren konnte, begrüsst es sehr, dass es für Fälle, die er zum Teil heute einfach nicht bewältigen kann, mehr Ermittler geben soll, Fälle, bei denen er zum Teil bis zu 20 oder sogar mehr Ermittler braucht - das für einen einzigen Fall. Sie stellen sich wahrscheinlich immer vor, ein Fall, ein Ermittler. Das ist leider nicht so. Die Fälle sind unglaublich kompliziert, und gerade die Netzwerke der organisierten Kriminalität nehmen ihre Verteidigungsrechte, die sie mit der Strafprozessordnung neu erhalten haben, sehr exzessiv wahr. Die machen mit einem Heer von besten Anwälten alles, um die Prozesse zu verlängern und komplizierter zu machen, um weitere Berichte und Untersuchungen einzufordern. Das ist die Realität, der wir uns stellen müssen. Diese wurde noch durch die Tatsache verschärft - das ist ganz wichtig, was Frau Gmür-Schönenberger gesagt hat -, dass die organisierte Kriminalität im Internet stattfindet. Dort müssen wir besser werden. Es ist enorm kompliziert und aufwendig, die grenzüberschreitend im virtuellen Bereich tätigen Banden zu knacken. Aber es ist wegen des Risikos für die Sicherheit unserer Bevölkerung, aber auch wegen des Image unseres Landes, wegen der Reputation, die auf der Kippe steht, unglaublich wichtig. 
+Deshalb ist es wichtig, dass wir hier vorangehen und dass wir schrittweise vorgehen. Der Bundesrat braucht diese Motion nicht dafür, wir werden diese Entscheide schrittweise im Rahmen der ordentlichen Budgetprozesse fällen, aber es ist wichtig, das möchte ich doch noch sagen, dass Sie den Handlungsbedarf wirklich erkennen.
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">367106</t>
   </si>
   <si>
@@ -948,13 +900,49 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">367062</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juillard Charles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je vais m'exprimer en tant que membre de la Commission de la politique de sécurité, mais aussi en tant que membre et ancien président de la Commission de gestion, puisque nous avons abordé la question des effectifs de Fedpol à plusieurs reprises lors des séances de la Commission de gestion, et que nous sommes arrivés à la conclusion qu'il y avait un vrai problème d'effectifs concernant les enquêteurs de Fedpol. C'est aussi dans cet esprit que nous avons écrit au Conseil fédéral pour qu'il envisa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je vais m'exprimer en tant que membre de la Commission de la politique de sécurité, mais aussi en tant que membre et ancien président de la Commission de gestion, puisque nous avons abordé la question des effectifs de Fedpol à plusieurs reprises lors des séances de la Commission de gestion, et que nous sommes arrivés à la conclusion qu'il y avait un vrai problème d'effectifs concernant les enquêteurs de Fedpol. C'est aussi dans cet esprit que nous avons écrit au Conseil fédéral pour qu'il envisage l'augmentation des effectifs, ce qui va dans le même sens que cette motion. Je dois cependant vous dire que nous n'avons pas examiné dans le détail si ces postes supplémentaires, - ces postes d'enquêteurs, parce que c'est surtout là qu'il y a un problème -, pouvaient être en tout ou partie compensés par une réorganisation de Fedpol - qui s'impose, selon le Contrôle fédéral des finances -, et s'il serait possible de diminuer les postes dans le domaine administratif pour les concentrer sur le terrain, là où les besoins se font particulièrement sentir, si l'on écoute aussi le Ministère public de la Confédération. Je voulais vous donner ces informations.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">367096</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sommaruga Carlo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je prends la parole en tant que président de la sous-commission de la Commission de gestion qui s'occupe du DFJP et de la Chancellerie fédérale. Ce sujet, nous l'avons traité à plusieurs reprises et le faisons depuis fort longtemps. Nous avons entendu le procureur général de la Confédération, nous avons entendu l'ancienne et la nouvelle directrice de Fedpol et différentes autres personnes. Sur cette base-là, nous avons pu constater de manière claire que les personnes entendues relevaient qu'il y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je prends la parole en tant que président de la sous-commission de la Commission de gestion qui s'occupe du DFJP et de la Chancellerie fédérale. Ce sujet, nous l'avons traité à plusieurs reprises et le faisons depuis fort longtemps. Nous avons entendu le procureur général de la Confédération, nous avons entendu l'ancienne et la nouvelle directrice de Fedpol et différentes autres personnes. Sur cette base-là, nous avons pu constater de manière claire que les personnes entendues relevaient qu'il y a aujourd'hui un déficit de personnel pour assurer la sécurité de la Suisse au niveau des infractions qui sont de la compétence fédérale et donc de la compétence du DFJP.
+J'entends bien les chiffres de notre collègue Rieder, mais ces chiffres ne reflètent pas la réalité qui nous est décrite par le procureur général de la Confédération et dont les termes ont été rappelés par notre collègue Dittli, à savoir que, aujourd'hui, il y a des procédures pénales concernant surtout la criminalité organisée internationale qui ne peuvent pas être ouvertes parce qu'il n'y a pas assez de personnel spécialisé. Je pense que cet élément doit être pris en compte.
+Si cette motion est aujourd'hui sur la table, c'est parce qu'il y a non seulement le rapport du Contrôle fédéral des finances, mais également des rapports de la Commission de gestion. Ce sont des éléments essentiels, et j'avoue que je suis surpris que l'on conteste les travaux faits par la Commission de gestion, et au Conseil national et au Conseil des États, sur la situation au niveau du procureur général et au niveau de Fedpol.
+J'aimerais juste dire que l'élément central qui a été évoqué par notre collègue, ce n'est pas la stabilité des plaintes ou des procédures qui ont été ouvertes de manière générale, c'est la criminalité organisée. Il a confirmé qu'il y avait une augmentation de 8 pour cent des affaires. Or, ce ne sont pas seulement les chiffres qu'il faut regarder, mais aussi la complexité des procédures qui sont ouvertes. Aujourd'hui, elles sont de plus en plus complexes dans le cadre de la poursuite pénale.
+J'aimerais juste relever que ce ne sont pas seulement des gigabits ou des mégabits qu'il faut examiner dans le cadre de toutes ces saisies de données faites en rapport avec la criminalité organisée, mais aussi les boîtes mail et les téléphones cryptés, et que cela nécessite des spécialistes. Aujourd'hui, le problème est immédiat. Il n'y a pas lieu d'attendre ou de compter sur le fait que des personnes vont partir à la retraite, même dans d'autres domaines, pour pouvoir engager du personnel.
+Je prends juste un exemple[NB]: il n'y a pas très longtemps, Fedpol a dû s'occuper d'un cas très particulier, celui des bombes qui avaient été placées pour faire chanter Patek Philippe. Pour rappel, cela s'est passé à Genève. Des bombes artisanales ont été mises dans des boîtes aux lettres et il y a eu des blessés. Il a fallu déployer des moyens extrêmement importants, non seulement à Genève, mais également au niveau de Fedpol qui disposait de spécialiste, pour enfin trouver la personne responsable de ces actes. J'aimerais relever que ce sont aussi des procédures qui, en général, demandent beaucoup, beaucoup de ressources humaines, et des ressources humaines spécialisées.
+Dès lors, je veux simplement vous dire que si l'on veut avoir une sécurité de la Suisse non seulement extérieure mais aussi intérieure, je crois qu'il faut entendre le message qui nous est donné par Fedpol, par le procureur général et par la Commission de gestion.
+Je vous invite donc à accepter cette motion, comme le propose la majorité de la commission.
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">367621</t>
   </si>
   <si>
     <t xml:space="preserve">20251215</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conseil fédéral</t>
   </si>
   <si>
     <t xml:space="preserve">Parmelin Guy</t>
@@ -1058,6 +1046,23 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">368193</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stark Jakob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Bundesrat beantragt, auf Finanzhilfen des Bundes im Bereich der Weiterbildung zu verzichten. Die Gründe sind folgende: Der Weiterbildungsmarkt ist weitgehend privatwirtschaftlich organisiert. Es gibt in diesem Bereich sehr namhafte Mitnahmeeffekte. Mehrfach schon gab es Kritik der Eidgenössischen Finanzkontrolle daran, wie und wofür diese Beiträge an die Organisationen der Weiterbildung gehen und wie ihre Wirkung ist. Schwergewichtig geht es hier ja um die Förderung der Grundkompetenzen, und</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Bundesrat beantragt, auf Finanzhilfen des Bundes im Bereich der Weiterbildung zu verzichten. Die Gründe sind folgende: Der Weiterbildungsmarkt ist weitgehend privatwirtschaftlich organisiert. Es gibt in diesem Bereich sehr namhafte Mitnahmeeffekte. Mehrfach schon gab es Kritik der Eidgenössischen Finanzkontrolle daran, wie und wofür diese Beiträge an die Organisationen der Weiterbildung gehen und wie ihre Wirkung ist. Schwergewichtig geht es hier ja um die Förderung der Grundkompetenzen, und dabei ist zu beachten, dass das eine ureigene Aufgabe der Kantone ist und dass sich der Bund mit Spezialgesetzen im Ausländerrecht, in der ALV und IV hier schon engagiert. Aus diesem Grund beantragt der Bundesrat, die Bestimmungen aufzuheben. Die Entlastungswirkung ist bei 19,8 Millionen Franken.
+Diese drei Anträge, die Sie hier vor sich haben, sehen alle vor, auf die Gesetzesänderung zu verzichten, mit Verweis auf die Kann-Bestimmung in Artikel 12 Absatz 1 WeBiG. Es ist also ohne Weiteres möglich, das Gesetz so zu belassen und bei der entsprechenden Position im Voranschlag den Betrag anzupassen. Die Kommissionsmehrheit möchte die volle Entlastungswirkung beibehalten, also die gut 19 Millionen Franken. Die Minderheit I (Herzog Eva) möchte die Entlastungswirkung knapp halbieren, sie möchte hier weiterhin 10[NB]Millionen[NB]Franken budgetieren. Die Minderheit II (Maillard Pierre-Yves) empfiehlt Ihnen, auf eine Kürzung ganz zu verzichten.
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">368245</t>
   </si>
   <si>
@@ -1066,23 +1071,6 @@
   <si>
     <t xml:space="preserve">Das ist ein bisschen ein Streit um des Kaisers Bart. Der Präsident der Finanzkommission hat es gesagt: Es geht um ein Rahmengesetz. An sich wollte der Bundesrat im Gesetz klarer festhalten, dass die Empfänger von Finanzhilfen ihre Aufgaben soweit möglich selbst finanzieren; das war auch immer ein Wunsch der Eidgenössischen Finanzkontrolle (EFK). Der Herr Präsident hat es gesagt: Es kamen dann Ängste aus dem Kultur- und dem Umweltbereich, dass durchgehend nur noch 50 Prozent Subventionen ausbezahlt würden. Das wäre nicht der Fall gewesen.
 Wenn Sie das streichen, ist das nicht gravierend, weil auch das aktuelle Recht davon ausgeht, und das ist wichtig, dass Subventionsempfänger nach Kräften und ihrer wirtschaftlichen Leistungsfähigkeit mitbeteiligt werden. In der Regel, nach ständiger Praxis der Eidgenössischen Finanzverwaltung, sind das 50 Prozent, aber das muss im Einzelfall festgelegt werden. Ich verzichte hier auf eine Abstimmung, wir können mit dem geltenden Recht leben, es war der Versuch einer Präzisierung. In der Sache wird das nicht viel daran ändern, dass man immer noch darum feilschen wird, welcher Subventionssatz im Einzelfall angewendet wird.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">368193</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stark Jakob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Der Bundesrat beantragt, auf Finanzhilfen des Bundes im Bereich der Weiterbildung zu verzichten. Die Gründe sind folgende: Der Weiterbildungsmarkt ist weitgehend privatwirtschaftlich organisiert. Es gibt in diesem Bereich sehr namhafte Mitnahmeeffekte. Mehrfach schon gab es Kritik der Eidgenössischen Finanzkontrolle daran, wie und wofür diese Beiträge an die Organisationen der Weiterbildung gehen und wie ihre Wirkung ist. Schwergewichtig geht es hier ja um die Förderung der Grundkompetenzen, und</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Der Bundesrat beantragt, auf Finanzhilfen des Bundes im Bereich der Weiterbildung zu verzichten. Die Gründe sind folgende: Der Weiterbildungsmarkt ist weitgehend privatwirtschaftlich organisiert. Es gibt in diesem Bereich sehr namhafte Mitnahmeeffekte. Mehrfach schon gab es Kritik der Eidgenössischen Finanzkontrolle daran, wie und wofür diese Beiträge an die Organisationen der Weiterbildung gehen und wie ihre Wirkung ist. Schwergewichtig geht es hier ja um die Förderung der Grundkompetenzen, und dabei ist zu beachten, dass das eine ureigene Aufgabe der Kantone ist und dass sich der Bund mit Spezialgesetzen im Ausländerrecht, in der ALV und IV hier schon engagiert. Aus diesem Grund beantragt der Bundesrat, die Bestimmungen aufzuheben. Die Entlastungswirkung ist bei 19,8 Millionen Franken.
-Diese drei Anträge, die Sie hier vor sich haben, sehen alle vor, auf die Gesetzesänderung zu verzichten, mit Verweis auf die Kann-Bestimmung in Artikel 12 Absatz 1 WeBiG. Es ist also ohne Weiteres möglich, das Gesetz so zu belassen und bei der entsprechenden Position im Voranschlag den Betrag anzupassen. Die Kommissionsmehrheit möchte die volle Entlastungswirkung beibehalten, also die gut 19 Millionen Franken. Die Minderheit I (Herzog Eva) möchte die Entlastungswirkung knapp halbieren, sie möchte hier weiterhin 10[NB]Millionen[NB]Franken budgetieren. Die Minderheit II (Maillard Pierre-Yves) empfiehlt Ihnen, auf eine Kürzung ganz zu verzichten.
 </t>
   </si>
   <si>
@@ -1195,7 +1183,7 @@
   <tableColumns count="9">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="MeetingDate"/>
-    <tableColumn id="3" name="CouncilName"/>
+    <tableColumn id="3" name="MeetingCouncilAbbreviation"/>
     <tableColumn id="4" name="SpeakerFullName"/>
     <tableColumn id="5" name="ParlGroupAbbreviation"/>
     <tableColumn id="6" name="CantonAbbreviation"/>
@@ -1733,75 +1721,77 @@
         <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9"/>
+        <v>48</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
       <c r="F9" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="G9" t="s">
         <v>15</v>
       </c>
       <c r="H9" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="I9" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
         <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G10" t="s">
         <v>15</v>
       </c>
       <c r="H10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G11" t="s">
         <v>15</v>
       </c>
       <c r="H11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I11" t="s">
         <v>61</v>
@@ -1815,22 +1805,22 @@
         <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
         <v>63</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G12" t="s">
         <v>15</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I12" t="s">
         <v>65</v>
@@ -1844,235 +1834,233 @@
         <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E13"/>
       <c r="F13" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="G13" t="s">
         <v>15</v>
       </c>
       <c r="H13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" t="s">
         <v>68</v>
-      </c>
-      <c r="I13" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
         <v>70</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
         <v>71</v>
       </c>
-      <c r="C14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
         <v>72</v>
-      </c>
-      <c r="E14"/>
-      <c r="F14" t="s">
-        <v>73</v>
       </c>
       <c r="G14" t="s">
         <v>15</v>
       </c>
       <c r="H14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" t="s">
         <v>74</v>
-      </c>
-      <c r="I14" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="H15" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16"/>
+      <c r="F16" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" t="s">
+        <v>81</v>
+      </c>
+      <c r="I16" t="s">
         <v>82</v>
-      </c>
-      <c r="B16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E16" t="s">
-        <v>84</v>
-      </c>
-      <c r="F16" t="s">
-        <v>85</v>
-      </c>
-      <c r="G16" t="s">
-        <v>59</v>
-      </c>
-      <c r="H16" t="s">
-        <v>86</v>
-      </c>
-      <c r="I16" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="F17" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G17" t="s">
         <v>15</v>
       </c>
       <c r="H17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I17" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>90</v>
       </c>
       <c r="E18" t="s">
         <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>14</v>
+        <v>91</v>
       </c>
       <c r="G18" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="H18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
       </c>
       <c r="D19" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G19" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" t="s">
         <v>97</v>
       </c>
-      <c r="E19" t="s">
+      <c r="I19" t="s">
         <v>98</v>
-      </c>
-      <c r="F19" t="s">
-        <v>99</v>
-      </c>
-      <c r="G19" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" t="s">
-        <v>100</v>
-      </c>
-      <c r="I19" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="D20" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E20"/>
       <c r="F20" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G20" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H20" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I20" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="D21" t="s">
         <v>43</v>
@@ -2085,168 +2073,168 @@
         <v>15</v>
       </c>
       <c r="H21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I21" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B22" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C22" t="s">
         <v>42</v>
       </c>
       <c r="D22" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E22"/>
       <c r="F22" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G22" t="s">
         <v>15</v>
       </c>
       <c r="H22" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I22" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B23" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23"/>
+        <v>116</v>
+      </c>
+      <c r="E23" t="s">
+        <v>49</v>
+      </c>
       <c r="F23" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="G23" t="s">
         <v>15</v>
       </c>
       <c r="H23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I23" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B24" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
       </c>
       <c r="D24" t="s">
-        <v>123</v>
-      </c>
-      <c r="E24" t="s">
-        <v>53</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E24"/>
       <c r="F24" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="G24" t="s">
         <v>15</v>
       </c>
       <c r="H24" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I24" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B25" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D25" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E25" t="s">
         <v>25</v>
       </c>
       <c r="F25" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G25" t="s">
         <v>15</v>
       </c>
       <c r="H25" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="I25" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B26" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D26" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E26" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="F26" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G26" t="s">
         <v>15</v>
       </c>
       <c r="H26" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="I26" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B27" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D27" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E27" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F27" t="s">
         <v>44</v>
@@ -2255,10 +2243,10 @@
         <v>15</v>
       </c>
       <c r="H27" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I27" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Régénération JSON avec recherche italien: 163 débats (+3)
</commit_message>
<xml_diff>
--- a/Debats_CDF_EFK.xlsx
+++ b/Debats_CDF_EFK.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="672">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -904,6 +904,45 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">338578</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giacometti Anna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il 27 marzo 2024 il Consiglio federale ha adottato il messaggio concernente il consuntivo della Confederazione svizzera per il 2023 a mano del Parlamento. La Commissione delle finanze ha esaminato il consuntivo nelle sue quattro sottocommissioni e nelle riunioni plenarie.
+La Commissione delle finanze ha preso atto del rapporto del Controllo federale delle finanze che raccomanda di approvare i conti annuali della Confederazione e dei due fondi FIF e Fostra.
+La modifica della legge federale sulle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il 27 marzo 2024 il Consiglio federale ha adottato il messaggio concernente il consuntivo della Confederazione svizzera per il 2023 a mano del Parlamento. La Commissione delle finanze ha esaminato il consuntivo nelle sue quattro sottocommissioni e nelle riunioni plenarie.
+La Commissione delle finanze ha preso atto del rapporto del Controllo federale delle finanze che raccomanda di approvare i conti annuali della Confederazione e dei due fondi FIF e Fostra.
+La modifica della legge federale sulle finanze della Confederazione (LFC) che semplifica e ottimizza la gestione delle finanze pubbliche, è entrata in vigore il 1° gennaio 2022 ed è stata applicata per la prima volta nel preventivo 2023. Il consuntivo 2023 è quindi la prima chiusura dei conti secondo la nuova legislazione. Le novità principali riguardano la soppressione del conto di finanziamento come conto autonomo, una gestione delle finanze pubbliche improntata al principio della conformità temporale - la costituzione e lo scioglimento di accantonamenti e delimitazioni sottostanno ora al freno all'indebitamento - e una nuova definizione del debito netto. La modifica della LFC ha richiesto un [PAGE 821] adeguamento una tantum del conto di compensazione e del conto di ammortamento.
+Per la seconda volta consecutiva e per la terza volta dal 2005, la Confederazione registra un deficit strutturale nel suo bilancio ordinario. Il consuntivo 2023 chiude con un deficit di finanziamento pari a 1,4 miliardi di franchi; questo significa che le entrate non sono bastate per finanziare le uscite e gli investimenti netti. 
+Circa la metà del deficit proviene dal bilancio ordinario e il resto da quello straordinario.
+Il freno all'indebitamento limita le uscite ordinarie al livello delle entrate ordinarie, tenendo conto della situazione economica. Per il 2023 il freno all'indebitamento avrebbe consentito alle uscite di superare le entrate di 238 milioni di franchi, pari allo 0,3 per cento delle entrate ordinarie. Il deficit ordinario di finanziamento per il 2023 ammonta però a 672 milioni di franchi. I rimanenti 434 milioni di deficit sono pertanto di natura strutturale e vengono addebitati al conto di compensazione. Il saldo al 31 dicembre 2023 è di 20,043 miliardi di franchi.
+Sul conto di ammortamento vengono addebitate le uscite e accreditate le entrate supplementari. A causa delle uscite legate alla pandemia di Covid-19, il conto di ammortamento presenta un saldo fortemente negativo. Il disavanzo del conto di ammortamento al 31 dicembre 2023 ammonta a 27,216 miliardi di franchi.
+L'economia svizzera è cresciuta dell'1,3 per cento in termini reali e del 2,3 per cento in termini nominali registrando, in entrambi i casi, un andamento meno dinamico di quello ipotizzato nel preventivo. Il calo degli investimenti e la crescita negativa a livello mondiale hanno neutralizzato gli impulsi positivi generati dai consumi privati. Per contro, l'indice nazionale dei prezzi al consumo è aumentato più del previsto, attestandosi al 2,1 per cento.
+Il debito netto è dato dal capitale di terzi al netto dei beni patrimoniali. Nel 2023 l'indebitamento netto è aumentato di 2,7 miliardi di franchi, attestandosi a 142 miliardi; questo è dovuto al deficit di finanziamento e a transazioni imputate direttamente al capitale proprio.
+Nel 2023 sono state contabilizzate entrate pari a 79,6 miliardi di franchi, il che corrisponde a una progressione del 5,2 per cento rispetto all'esercizio 2022. Le entrate della Confederazione sono aumentate sensibilmente, nonostante la mancata distribuzione degli utili della Banca nazionale svizzera. L'incremento è riconducibile principalmente alle maggiori entrate dall'imposta federale diretta e dall'imposta preventiva. Il reddito fiscale dell'imposta sul valore aggiunto è aumentato di 0,6 miliardi di franchi. Nell'ambito dell'imposta federale diretta è aumentato soprattutto il gettito dell'imposta sull'utile delle persone giuridiche, più 2,2 miliardi di franchi. Per[NB]quanto[NB]riguarda[NB]l'imposta preventiva, il forte aumento è riconducibile alla correzione di alcune stime riguardanti gli anni precedenti.
+Le entrate straordinarie ammontano a 310 milioni di franchi. La vendita di alcune unità operative di Ruag International Holding SA ha generato entrate straordinarie pari a 200 milioni di franchi. Altre entrate straordinarie derivano dai premi di rischio versati da Credit Suisse per i mutui a sostegno della liquidità, coperti da una garanzia della Confederazione.
+Le uscite complessive della Confederazione nel 2023 ammontano a 81 miliardi di franchi, rimanendo quindi stabili rispetto all'anno precedente. Già per il quarto anno consecutivo è stato necessario far valere un fabbisogno finanziario eccezionale. Rispetto agli esercizi precedenti, caratterizzati dalle uscite legate alla pandemia, esso è però sensibilmente inferiore.
+Le uscite ordinarie sono cresciute di 2,2 miliardi di franchi, dunque in maniera più marcata rispetto al PIL nominale pari al 2,3 per cento. Il contributo della Confederazione a favore della previdenza per la vecchiaia è aumentato di 459 milioni rispetto all'anno precedente, e quello destinato all'assicurazione per l'invalidità di 90 milioni di franchi. Sono aumentate anche le uscite per le riduzioni dei premi nell'assicurazione malattie e per le prestazioni complementari. Si osservano maggiori uscite per il settore della migrazione sebbene le uscite a favore delle persone provenienti dall'Ucraina siano state contabilizzate a titolo straordinario. 
+Le uscite legate alle finanze e alle imposte sono cresciute del 10 per cento, questo a causa dell'aumento dei tassi d'interesse e della partecipazione dei cantoni alle entrate dell'imposta federale diretta e dell'imposta preventiva. Infine, rispetto al 2022, la Confederazione ha speso 310 milioni di franchi in più per il Settore educazione e ricerca. Le uscite per le relazioni con l'estero e la cooperazione internazionale sono aumentate di 208 milioni di franchi, pari al 5,4 per cento.
+Per quanto concerne le uscite straordinarie, i contributi ai cantoni per le persone in cerca di protezione provenienti dall'Ucraina ammontano a 1,1 miliardi di franchi. Il piano di salvataggio per il Settore energia elettrica di 4 miliardi di franchi è rimasto inutilizzato e ha quindi potuto essere revocato.
+La vostra Commissione delle finanze propone, con 16 voti contro 8, di approvare il consuntivo 2023 e, all'unanimità, di approvare i conti speciali "Fondo per l'infrastruttura ferroviaria" e "Fondo per le strade nazionali e il traffico d'agglomerato". In tal modo segue la raccomandazione del Controllo federale delle finanze che, nel suo ruolo di revisore, si era espresso a favore dell'approvazione del conto annuale 2023 della Confederazione, dei sorpassi di credito per 2,25 miliardi di franchi e della costituzione di nuove riserve per 174 milioni di franchi.
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">339510</t>
   </si>
   <si>
@@ -1010,9 +1049,6 @@
   </si>
   <si>
     <t xml:space="preserve">Wehrli Laurent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RL</t>
   </si>
   <si>
     <t xml:space="preserve">Dans sa séance plénière de mai 2024, en présence du président et du secrétaire général du Tribunal fédéral, votre Commission de gestion a pris connaissance et étudié le rapport de gestion du Tribunal fédéral pour l'année 2023. Votre sous-commission de gestion, en charge notamment du suivi des tribunaux fédéraux et du Ministère public de la Confédération, l'avait précédemment fait lors de sa séance, qui a eu lieu à Lausanne le 8 mai 2024, en présence du président et de divers autres responsables.</t>
@@ -1105,9 +1141,6 @@
     <t xml:space="preserve">Engler Stefan</t>
   </si>
   <si>
-    <t xml:space="preserve">GR</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bei der Beratung dieses Geschäfts können wir uns kurzhalten. Ihre Staatspolitische Kommission hat die Motion Farinelli 23.3592, "Alle Berichte sollen zumindest eine Zusammenfassung in den drei Amtssprachen enthalten", vorgeprüft und ist zum Schluss gekommen, Ihnen die Annahme dieser Motion zu beantragen. Dasselbe hat der Nationalrat getan, und dasselbe will auch der Bundesrat tun, allerdings mit der Einschränkung, dass es sich um Berichte des Bundesrates und der Bundesverwaltung handeln müsse, d</t>
   </si>
   <si>
@@ -1118,6 +1151,27 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">341085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regazzi Fabio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visto che parliamo di un tema legato al multilinguismo permettetemi di rivolgermi a voi in italiano per qualche breve riflessione.
+Come ticinese so bene quanto sia importante sentirsi parte del tessuto nazionale svizzero a pieno titolo. Per questo sostengo con convinzione la mozione Farinelli, e ho sentito con piacere che anche la commissione competente la sostiene. L'autore della mozione chiede che tutti i rapporti presentati dall'amministrazione e dal Consiglio federale includano un breve rias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visto che parliamo di un tema legato al multilinguismo permettetemi di rivolgermi a voi in italiano per qualche breve riflessione.
+Come ticinese so bene quanto sia importante sentirsi parte del tessuto nazionale svizzero a pieno titolo. Per questo sostengo con convinzione la mozione Farinelli, e ho sentito con piacere che anche la commissione competente la sostiene. L'autore della mozione chiede che tutti i rapporti presentati dall'amministrazione e dal Consiglio federale includano un breve riassunto nelle tre lingue ufficiali della Svizzera. Questa proposta, che mi sembra ragionevole, è un buon compromesso. Non solo promuove la diversità linguistica del nostro paese, ma rafforza anche la trasparenza e l'accessibilità delle informazioni. Attualmente i riassunti dei rapporti, come l'ha ricordato il relatore, sono spesso disponibili solo in una o due lingue ufficiali, escludendo quindi una parte significativa della popolazione. Ricordo che quando si parla di Svizzera italiana non si deve pensare solo al canton Ticino o al Grigioni italiano, ma a quasi 700[NB]000 persone che in tutta la Svizzera parlano la lingua di Dante.
+Il modello adottato dal Controllo federale delle finanze, che include sempre una versione riassuntiva nelle lingue ufficiali, ha dimostrato l'efficacia di questa pratica. Estendere questo approccio a tutti i rapporti dell'amministrazione e del Consiglio federale standardizzerebbe e migliorerebbe ulteriormente la comunicazione istituzionale.
+In sintesi, sostenere questa mozione significa promuovere multilinguismo, trasparenza ed efficienza comunicativa. È un impegno concreto per una maggiore accessibilità delle informazioni governative e rappresenta una misura equa e rispettosa della diversità linguistica della Svizzera.
+Per questo motivo vi invito ad approvare la presente mozione.
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">341480</t>
   </si>
   <si>
@@ -1140,9 +1194,6 @@
   </si>
   <si>
     <t xml:space="preserve">Chiesa Marco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TI</t>
   </si>
   <si>
     <t xml:space="preserve">Künftig darf der medizinisch-technische Fortschritt nicht nur Berücksichtigung finden, wenn es zu teuer wird. Wie auch sonst im Markt müssen die Effizienzgewinne der Kundschaft bzw. den Kostenträgern, den Prämienzahlern und der öffentlichen Hand, weitergegeben werden. Die Tarifpartner müssen diesbezüglich aktiv werden und Lösungen finden, auch wenn dies nicht allen Beteiligten passt. Der Bundesrat muss subsidiär, regelmässig und zeitnah eingreifen, wenn die Tarifpartner den präzisierten gesetzli</t>
@@ -1402,9 +1453,6 @@
   </si>
   <si>
     <t xml:space="preserve">20240924</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regazzi Fabio</t>
   </si>
   <si>
     <t xml:space="preserve">Ich danke dem Bundesrat für die Stellungnahme zu meiner Interpellation. Ich bin damit aber nicht zufrieden, daher möchte ich den Bundesrat um eine Klarstellung bitten. Es hat nämlich den Anschein, als ob der Kostenrahmen nur scheinbar eingehalten wird. Die Stellungnahme vermittelt den Eindruck, dass das Projekt inhaltlich und finanziell im Rahmen liegt, nur weil bisher nicht das gesamte Budget aufgewendet wurde. Der Verweis darauf, dass 71,8 Prozent der veranlagten Kosten verwendet wurden, sagt </t>
@@ -2859,6 +2907,29 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">356868</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farinelli Alex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A nome della Commissione delle finanze vi presento le considerazioni emerse durante l'esame del consuntivo 2024. Non ripeterò tutte le cifre già citate dalla collega. Vi posso dire che l'esame si è svolto in diverse sedute e ha incluso l'audizione del Consiglio federale, dei vari uffici federali rispettivamente del Controllo federale delle finanze e delle autorità della Confederazione. 
+Nel 2024, il consuntivo chiude con un disavanzo di finanziamento contenuto pari a 80 milioni di franchi. È il </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A nome della Commissione delle finanze vi presento le considerazioni emerse durante l'esame del consuntivo 2024. Non ripeterò tutte le cifre già citate dalla collega. Vi posso dire che l'esame si è svolto in diverse sedute e ha incluso l'audizione del Consiglio federale, dei vari uffici federali rispettivamente del Controllo federale delle finanze e delle autorità della Confederazione. 
+Nel 2024, il consuntivo chiude con un disavanzo di finanziamento contenuto pari a 80 milioni di franchi. È il miglior risultato dal 2019 con un'eccedenza strutturale di 1,3 miliardi di franchi nel bilancio ordinario. Le entrate hanno superato le previsioni soprattutto grazie ad un forte incremento del gettito dell'imposta federale diretta e dell'IVA - questo è dovuto sia a fattori straordinari che strutturali -, mentre le spese sono rimaste sotto controllo. 
+La commissione prende atto con soddisfazione che i principi della legge sul freno all'indebitamento sono stati rispettati. Tuttavia desidera richiamare l'attenzione su alcuni elementi critici messi in evidenza dal Controllo federale delle finanze nei suoi rapporti di revisione. 
+Primo: il fondo dell'infrastruttura ferroviaria mostra segnali di squilibrio a medio termine. Le uscite previste supereranno le entrate già nel 2027. In assenza di misure correttive, le riserve minime legali non potranno più essere rispettate entro il 2028. Anche se non è oggetto diretto dalla revisione, la commissione sostiene la raccomandazione del Controllo federale delle finanze di monitorare attentamente l'evoluzione per garantire la sostenibilità finanziaria del fondo. 
+Secondo: persistono incertezze nella contabilizzazione delle entrate, in particolare riguardante la tassa sul traffico pesante commisurata alle prestazioni e l'e-vignetta, dove la mancanza di giustificativi completi limita la tracciabilità. Il Controllo federale delle finanze ha riconosciuto gli sforzi dell'amministrazione per contenere i rischi, ma ritiene necessaria una soluzione strutturale entro la fine di quest'anno. 
+Terzo: continuano ad essere presenti poste di bilancio segnate da un'elevata incertezza delle stime, come le riserve per i test Covid, i crediti Covid alle imprese o i costi di bonifica del deposito di munizioni di Mitholz. In tutti questi casi le stime sono state confermate come plausibili, ma devono essere sempre oggetto di un riesame continuo. 
+La commissione riconosce inoltre l'importanza della gestione prudente delle spese straordinarie legate al conflitto in Ucraina. Tale spese, ammesse nel bilancio straordinario per il 2024, dovranno progressivamente rientrare nel bilancio ordinario. A partire dal 2027, dovranno essere completamente assorbite da quest'ultimo. Si condivide quindi l'osservazione del Controllo federale delle finanze, che la classificazione delle spese straordinarie deve rimanere eccezionale e rigorosa, per non compromettere la credibilità del freno all'indebitamento e la stabilità delle finanze federali.
+Nel complesso, la commissione ritiene che il conto di Stato della Confederazione 2024 presenti un'immagine conforme alla legge. Pertanto, sostiene la raccomandazione del Controllo federale delle finanze di approvare la contabilità dello Stato. Propone a questo consiglio, con 17 voti favorevoli, 0 contrari e 8 astensioni, di approvare il consuntivo 2024. 
+Per quanto riguarda invece i fondi infrastrutturali legati all'infrastruttura ferroviaria e a quella stradale, ossia il FIF e il Fostra, essi sono stati approvati all'unanimità dei 25 consiglieri presenti in sala.
+In conclusione, mi permetto di ringraziare anch'io il Consiglio federale e la presidente della Confederazione per l'ottima collaborazione e il lavoro svolto, l'amministrazione federale delle finanze per averci supportato, il segretariato commissionale che è sempre a disposizione e il Controllo federale delle finanze che ci supporta in tutto quello che riguarda il controllo dei conti della Confederazione. 
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">357753</t>
   </si>
   <si>
@@ -4286,8 +4357,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:I161" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:I161"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:I164" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:I164"/>
   <tableColumns count="9">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="MeetingDate"/>
@@ -5646,42 +5717,42 @@
         <v>177</v>
       </c>
       <c r="B38" t="s">
+        <v>167</v>
+      </c>
+      <c r="C38" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" t="s">
         <v>178</v>
       </c>
-      <c r="C38" t="s">
-        <v>19</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>179</v>
       </c>
-      <c r="E38" t="s">
-        <v>28</v>
-      </c>
       <c r="F38" t="s">
-        <v>117</v>
+        <v>180</v>
       </c>
       <c r="G38" t="s">
-        <v>22</v>
+        <v>181</v>
       </c>
       <c r="H38" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="I38" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B39" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="C39" t="s">
         <v>19</v>
       </c>
       <c r="D39" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E39" t="s">
         <v>28</v>
@@ -5693,147 +5764,147 @@
         <v>22</v>
       </c>
       <c r="H39" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="I39" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B40" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="C40" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D40" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E40" t="s">
         <v>28</v>
       </c>
       <c r="F40" t="s">
-        <v>188</v>
+        <v>117</v>
       </c>
       <c r="G40" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H40" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="I40" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B41" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C41" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D41" t="s">
-        <v>20</v>
-      </c>
-      <c r="E41"/>
+        <v>194</v>
+      </c>
+      <c r="E41" t="s">
+        <v>28</v>
+      </c>
       <c r="F41" t="s">
-        <v>21</v>
+        <v>195</v>
       </c>
       <c r="G41" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H41" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="I41" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B42" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C42" t="s">
         <v>19</v>
       </c>
       <c r="D42" t="s">
-        <v>122</v>
-      </c>
-      <c r="E42" t="s">
-        <v>37</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E42"/>
       <c r="F42" t="s">
-        <v>98</v>
+        <v>21</v>
       </c>
       <c r="G42" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H42" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="I42" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B43" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C43" t="s">
         <v>19</v>
       </c>
       <c r="D43" t="s">
-        <v>200</v>
+        <v>122</v>
       </c>
       <c r="E43" t="s">
-        <v>201</v>
+        <v>37</v>
       </c>
       <c r="F43" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="G43" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H43" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="I43" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B44" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D44" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E44" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="F44" t="s">
-        <v>207</v>
+        <v>117</v>
       </c>
       <c r="G44" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H44" t="s">
         <v>208</v>
@@ -5856,39 +5927,39 @@
         <v>212</v>
       </c>
       <c r="E45" t="s">
-        <v>78</v>
+        <v>179</v>
       </c>
       <c r="F45" t="s">
-        <v>73</v>
+        <v>213</v>
       </c>
       <c r="G45" t="s">
         <v>14</v>
       </c>
       <c r="H45" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="I45" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B46" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C46" t="s">
         <v>11</v>
       </c>
       <c r="D46" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E46" t="s">
         <v>78</v>
       </c>
       <c r="F46" t="s">
-        <v>218</v>
+        <v>73</v>
       </c>
       <c r="G46" t="s">
         <v>14</v>
@@ -5908,33 +5979,33 @@
         <v>222</v>
       </c>
       <c r="C47" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D47" t="s">
-        <v>60</v>
+        <v>223</v>
       </c>
       <c r="E47" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="F47" t="s">
-        <v>48</v>
+        <v>180</v>
       </c>
       <c r="G47" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H47" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I47" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B48" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C48" t="s">
         <v>11</v>
@@ -5943,13 +6014,13 @@
         <v>227</v>
       </c>
       <c r="E48" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="F48" t="s">
         <v>228</v>
       </c>
       <c r="G48" t="s">
-        <v>14</v>
+        <v>181</v>
       </c>
       <c r="H48" t="s">
         <v>229</v>
@@ -5963,36 +6034,36 @@
         <v>231</v>
       </c>
       <c r="B49" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="C49" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D49" t="s">
-        <v>232</v>
+        <v>60</v>
       </c>
       <c r="E49" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="F49" t="s">
+        <v>48</v>
+      </c>
+      <c r="G49" t="s">
+        <v>22</v>
+      </c>
+      <c r="H49" t="s">
         <v>233</v>
       </c>
-      <c r="G49" t="s">
-        <v>14</v>
-      </c>
-      <c r="H49" t="s">
+      <c r="I49" t="s">
         <v>234</v>
-      </c>
-      <c r="I49" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
+        <v>235</v>
+      </c>
+      <c r="B50" t="s">
         <v>236</v>
-      </c>
-      <c r="B50" t="s">
-        <v>226</v>
       </c>
       <c r="C50" t="s">
         <v>11</v>
@@ -6001,13 +6072,13 @@
         <v>237</v>
       </c>
       <c r="E50" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F50" t="s">
-        <v>117</v>
+        <v>228</v>
       </c>
       <c r="G50" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H50" t="s">
         <v>238</v>
@@ -6021,19 +6092,19 @@
         <v>240</v>
       </c>
       <c r="B51" t="s">
+        <v>236</v>
+      </c>
+      <c r="C51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" t="s">
         <v>241</v>
       </c>
-      <c r="C51" t="s">
-        <v>19</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
+        <v>78</v>
+      </c>
+      <c r="F51" t="s">
         <v>242</v>
-      </c>
-      <c r="E51" t="s">
-        <v>201</v>
-      </c>
-      <c r="F51" t="s">
-        <v>43</v>
       </c>
       <c r="G51" t="s">
         <v>14</v>
@@ -6050,46 +6121,48 @@
         <v>245</v>
       </c>
       <c r="B52" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C52" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D52" t="s">
-        <v>20</v>
-      </c>
-      <c r="E52"/>
+        <v>246</v>
+      </c>
+      <c r="E52" t="s">
+        <v>11</v>
+      </c>
       <c r="F52" t="s">
-        <v>21</v>
+        <v>117</v>
       </c>
       <c r="G52" t="s">
         <v>22</v>
       </c>
       <c r="H52" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="I52" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B53" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C53" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D53" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E53" t="s">
-        <v>28</v>
+        <v>179</v>
       </c>
       <c r="F53" t="s">
-        <v>251</v>
+        <v>43</v>
       </c>
       <c r="G53" t="s">
         <v>14</v>
@@ -6106,10 +6179,10 @@
         <v>254</v>
       </c>
       <c r="B54" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C54" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D54" t="s">
         <v>20</v>
@@ -6142,24 +6215,24 @@
         <v>259</v>
       </c>
       <c r="E55" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F55" t="s">
-        <v>79</v>
+        <v>260</v>
       </c>
       <c r="G55" t="s">
         <v>14</v>
       </c>
       <c r="H55" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I55" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B56" t="s">
         <v>258</v>
@@ -6168,36 +6241,34 @@
         <v>11</v>
       </c>
       <c r="D56" t="s">
-        <v>259</v>
-      </c>
-      <c r="E56" t="s">
-        <v>11</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E56"/>
       <c r="F56" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="G56" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H56" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="I56" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B57" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="C57" t="s">
         <v>11</v>
       </c>
       <c r="D57" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="E57" t="s">
         <v>11</v>
@@ -6209,99 +6280,103 @@
         <v>14</v>
       </c>
       <c r="H57" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="I57" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B58" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="C58" t="s">
         <v>11</v>
       </c>
       <c r="D58" t="s">
-        <v>154</v>
-      </c>
-      <c r="E58"/>
+        <v>268</v>
+      </c>
+      <c r="E58" t="s">
+        <v>11</v>
+      </c>
       <c r="F58" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="G58" t="s">
         <v>14</v>
       </c>
       <c r="H58" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="I58" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B59" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C59" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D59" t="s">
-        <v>20</v>
-      </c>
-      <c r="E59"/>
+        <v>268</v>
+      </c>
+      <c r="E59" t="s">
+        <v>11</v>
+      </c>
       <c r="F59" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="G59" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H59" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="I59" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B60" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C60" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D60" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="E60"/>
       <c r="F60" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="G60" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H60" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="I60" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B61" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C61" t="s">
         <v>19</v>
@@ -6314,36 +6389,34 @@
         <v>21</v>
       </c>
       <c r="G61" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H61" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="I61" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B62" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C62" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D62" t="s">
-        <v>284</v>
-      </c>
-      <c r="E62" t="s">
-        <v>78</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E62"/>
       <c r="F62" t="s">
-        <v>228</v>
+        <v>21</v>
       </c>
       <c r="G62" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H62" t="s">
         <v>285</v>
@@ -6357,77 +6430,75 @@
         <v>287</v>
       </c>
       <c r="B63" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="C63" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D63" t="s">
-        <v>217</v>
-      </c>
-      <c r="E63" t="s">
-        <v>78</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E63"/>
       <c r="F63" t="s">
-        <v>218</v>
+        <v>21</v>
       </c>
       <c r="G63" t="s">
         <v>14</v>
       </c>
       <c r="H63" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="I63" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B64" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="C64" t="s">
         <v>11</v>
       </c>
       <c r="D64" t="s">
-        <v>291</v>
+        <v>227</v>
       </c>
       <c r="E64" t="s">
         <v>78</v>
       </c>
       <c r="F64" t="s">
-        <v>163</v>
+        <v>228</v>
       </c>
       <c r="G64" t="s">
         <v>14</v>
       </c>
       <c r="H64" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="I64" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B65" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="C65" t="s">
         <v>11</v>
       </c>
       <c r="D65" t="s">
-        <v>295</v>
+        <v>223</v>
       </c>
       <c r="E65" t="s">
         <v>78</v>
       </c>
       <c r="F65" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="G65" t="s">
         <v>14</v>
@@ -6444,7 +6515,7 @@
         <v>298</v>
       </c>
       <c r="B66" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="C66" t="s">
         <v>11</v>
@@ -6453,10 +6524,10 @@
         <v>299</v>
       </c>
       <c r="E66" t="s">
-        <v>201</v>
+        <v>78</v>
       </c>
       <c r="F66" t="s">
-        <v>73</v>
+        <v>163</v>
       </c>
       <c r="G66" t="s">
         <v>14</v>
@@ -6473,7 +6544,7 @@
         <v>302</v>
       </c>
       <c r="B67" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="C67" t="s">
         <v>11</v>
@@ -6485,7 +6556,7 @@
         <v>78</v>
       </c>
       <c r="F67" t="s">
-        <v>98</v>
+        <v>195</v>
       </c>
       <c r="G67" t="s">
         <v>14</v>
@@ -6502,7 +6573,7 @@
         <v>306</v>
       </c>
       <c r="B68" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="C68" t="s">
         <v>11</v>
@@ -6511,39 +6582,39 @@
         <v>307</v>
       </c>
       <c r="E68" t="s">
-        <v>28</v>
+        <v>179</v>
       </c>
       <c r="F68" t="s">
+        <v>73</v>
+      </c>
+      <c r="G68" t="s">
+        <v>14</v>
+      </c>
+      <c r="H68" t="s">
         <v>308</v>
       </c>
-      <c r="G68" t="s">
-        <v>14</v>
-      </c>
-      <c r="H68" t="s">
+      <c r="I68" t="s">
         <v>309</v>
-      </c>
-      <c r="I68" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B69" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="C69" t="s">
         <v>11</v>
       </c>
       <c r="D69" t="s">
-        <v>217</v>
+        <v>311</v>
       </c>
       <c r="E69" t="s">
         <v>78</v>
       </c>
       <c r="F69" t="s">
-        <v>218</v>
+        <v>98</v>
       </c>
       <c r="G69" t="s">
         <v>14</v>
@@ -6560,48 +6631,48 @@
         <v>314</v>
       </c>
       <c r="B70" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="C70" t="s">
         <v>11</v>
       </c>
       <c r="D70" t="s">
-        <v>284</v>
+        <v>315</v>
       </c>
       <c r="E70" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="F70" t="s">
-        <v>228</v>
+        <v>316</v>
       </c>
       <c r="G70" t="s">
         <v>14</v>
       </c>
       <c r="H70" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="I70" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B71" t="s">
-        <v>318</v>
+        <v>292</v>
       </c>
       <c r="C71" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D71" t="s">
-        <v>319</v>
+        <v>223</v>
       </c>
       <c r="E71" t="s">
         <v>78</v>
       </c>
       <c r="F71" t="s">
-        <v>73</v>
+        <v>180</v>
       </c>
       <c r="G71" t="s">
         <v>14</v>
@@ -6618,36 +6689,36 @@
         <v>322</v>
       </c>
       <c r="B72" t="s">
-        <v>318</v>
+        <v>292</v>
       </c>
       <c r="C72" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D72" t="s">
+        <v>227</v>
+      </c>
+      <c r="E72" t="s">
+        <v>78</v>
+      </c>
+      <c r="F72" t="s">
+        <v>228</v>
+      </c>
+      <c r="G72" t="s">
+        <v>14</v>
+      </c>
+      <c r="H72" t="s">
         <v>323</v>
       </c>
-      <c r="E72" t="s">
-        <v>28</v>
-      </c>
-      <c r="F72" t="s">
-        <v>218</v>
-      </c>
-      <c r="G72" t="s">
-        <v>14</v>
-      </c>
-      <c r="H72" t="s">
+      <c r="I72" t="s">
         <v>324</v>
-      </c>
-      <c r="I72" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
+        <v>325</v>
+      </c>
+      <c r="B73" t="s">
         <v>326</v>
-      </c>
-      <c r="B73" t="s">
-        <v>318</v>
       </c>
       <c r="C73" t="s">
         <v>19</v>
@@ -6656,10 +6727,10 @@
         <v>327</v>
       </c>
       <c r="E73" t="s">
-        <v>201</v>
+        <v>78</v>
       </c>
       <c r="F73" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="G73" t="s">
         <v>14</v>
@@ -6676,7 +6747,7 @@
         <v>330</v>
       </c>
       <c r="B74" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="C74" t="s">
         <v>19</v>
@@ -6685,10 +6756,10 @@
         <v>331</v>
       </c>
       <c r="E74" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F74" t="s">
-        <v>73</v>
+        <v>180</v>
       </c>
       <c r="G74" t="s">
         <v>14</v>
@@ -6705,7 +6776,7 @@
         <v>334</v>
       </c>
       <c r="B75" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="C75" t="s">
         <v>19</v>
@@ -6714,154 +6785,156 @@
         <v>335</v>
       </c>
       <c r="E75" t="s">
-        <v>78</v>
+        <v>179</v>
       </c>
       <c r="F75" t="s">
+        <v>43</v>
+      </c>
+      <c r="G75" t="s">
+        <v>14</v>
+      </c>
+      <c r="H75" t="s">
         <v>336</v>
       </c>
-      <c r="G75" t="s">
-        <v>14</v>
-      </c>
-      <c r="H75" t="s">
+      <c r="I75" t="s">
         <v>337</v>
-      </c>
-      <c r="I75" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
+        <v>338</v>
+      </c>
+      <c r="B76" t="s">
+        <v>326</v>
+      </c>
+      <c r="C76" t="s">
+        <v>19</v>
+      </c>
+      <c r="D76" t="s">
         <v>339</v>
       </c>
-      <c r="B76" t="s">
-        <v>318</v>
-      </c>
-      <c r="C76" t="s">
-        <v>19</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
+        <v>11</v>
+      </c>
+      <c r="F76" t="s">
+        <v>73</v>
+      </c>
+      <c r="G76" t="s">
+        <v>14</v>
+      </c>
+      <c r="H76" t="s">
         <v>340</v>
       </c>
-      <c r="E76" t="s">
+      <c r="I76" t="s">
         <v>341</v>
-      </c>
-      <c r="F76" t="s">
-        <v>13</v>
-      </c>
-      <c r="G76" t="s">
-        <v>14</v>
-      </c>
-      <c r="H76" t="s">
-        <v>342</v>
-      </c>
-      <c r="I76" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
+        <v>342</v>
+      </c>
+      <c r="B77" t="s">
+        <v>326</v>
+      </c>
+      <c r="C77" t="s">
+        <v>19</v>
+      </c>
+      <c r="D77" t="s">
+        <v>343</v>
+      </c>
+      <c r="E77" t="s">
+        <v>78</v>
+      </c>
+      <c r="F77" t="s">
         <v>344</v>
       </c>
-      <c r="B77" t="s">
-        <v>318</v>
-      </c>
-      <c r="C77" t="s">
-        <v>19</v>
-      </c>
-      <c r="D77" t="s">
+      <c r="G77" t="s">
+        <v>14</v>
+      </c>
+      <c r="H77" t="s">
         <v>345</v>
       </c>
-      <c r="E77"/>
-      <c r="F77" t="s">
-        <v>29</v>
-      </c>
-      <c r="G77" t="s">
-        <v>14</v>
-      </c>
-      <c r="H77" t="s">
+      <c r="I77" t="s">
         <v>346</v>
-      </c>
-      <c r="I77" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
+        <v>347</v>
+      </c>
+      <c r="B78" t="s">
+        <v>326</v>
+      </c>
+      <c r="C78" t="s">
+        <v>19</v>
+      </c>
+      <c r="D78" t="s">
         <v>348</v>
       </c>
-      <c r="B78" t="s">
-        <v>318</v>
-      </c>
-      <c r="C78" t="s">
-        <v>19</v>
-      </c>
-      <c r="D78" t="s">
-        <v>55</v>
-      </c>
       <c r="E78" t="s">
-        <v>37</v>
+        <v>349</v>
       </c>
       <c r="F78" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="G78" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H78" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="I78" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B79" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="C79" t="s">
         <v>19</v>
       </c>
       <c r="D79" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E79"/>
       <c r="F79" t="s">
-        <v>117</v>
+        <v>29</v>
       </c>
       <c r="G79" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H79" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="I79" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B80" t="s">
-        <v>356</v>
+        <v>326</v>
       </c>
       <c r="C80" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D80" t="s">
-        <v>303</v>
+        <v>55</v>
       </c>
       <c r="E80" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="F80" t="s">
-        <v>98</v>
+        <v>56</v>
       </c>
       <c r="G80" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H80" t="s">
         <v>357</v>
@@ -6875,48 +6948,46 @@
         <v>359</v>
       </c>
       <c r="B81" t="s">
+        <v>326</v>
+      </c>
+      <c r="C81" t="s">
+        <v>19</v>
+      </c>
+      <c r="D81" t="s">
         <v>360</v>
       </c>
-      <c r="C81" t="s">
-        <v>19</v>
-      </c>
-      <c r="D81" t="s">
+      <c r="E81"/>
+      <c r="F81" t="s">
+        <v>117</v>
+      </c>
+      <c r="G81" t="s">
+        <v>22</v>
+      </c>
+      <c r="H81" t="s">
         <v>361</v>
       </c>
-      <c r="E81" t="s">
-        <v>201</v>
-      </c>
-      <c r="F81" t="s">
-        <v>73</v>
-      </c>
-      <c r="G81" t="s">
-        <v>14</v>
-      </c>
-      <c r="H81" t="s">
+      <c r="I81" t="s">
         <v>362</v>
-      </c>
-      <c r="I81" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
+        <v>363</v>
+      </c>
+      <c r="B82" t="s">
         <v>364</v>
       </c>
-      <c r="B82" t="s">
-        <v>360</v>
-      </c>
       <c r="C82" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D82" t="s">
-        <v>36</v>
+        <v>311</v>
       </c>
       <c r="E82" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="F82" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
       <c r="G82" t="s">
         <v>14</v>
@@ -6942,10 +7013,10 @@
         <v>369</v>
       </c>
       <c r="E83" t="s">
-        <v>28</v>
+        <v>179</v>
       </c>
       <c r="F83" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="G83" t="s">
         <v>14</v>
@@ -6965,16 +7036,16 @@
         <v>368</v>
       </c>
       <c r="C84" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D84" t="s">
-        <v>217</v>
+        <v>36</v>
       </c>
       <c r="E84" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="F84" t="s">
-        <v>218</v>
+        <v>22</v>
       </c>
       <c r="G84" t="s">
         <v>14</v>
@@ -6991,48 +7062,48 @@
         <v>375</v>
       </c>
       <c r="B85" t="s">
-        <v>368</v>
+        <v>376</v>
       </c>
       <c r="C85" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D85" t="s">
-        <v>187</v>
+        <v>377</v>
       </c>
       <c r="E85" t="s">
         <v>28</v>
       </c>
       <c r="F85" t="s">
-        <v>188</v>
+        <v>98</v>
       </c>
       <c r="G85" t="s">
         <v>14</v>
       </c>
       <c r="H85" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="I85" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B86" t="s">
-        <v>368</v>
+        <v>376</v>
       </c>
       <c r="C86" t="s">
         <v>11</v>
       </c>
       <c r="D86" t="s">
-        <v>379</v>
+        <v>223</v>
       </c>
       <c r="E86" t="s">
-        <v>201</v>
+        <v>78</v>
       </c>
       <c r="F86" t="s">
-        <v>380</v>
+        <v>180</v>
       </c>
       <c r="G86" t="s">
         <v>14</v>
@@ -7049,46 +7120,48 @@
         <v>383</v>
       </c>
       <c r="B87" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="C87" t="s">
         <v>11</v>
       </c>
       <c r="D87" t="s">
-        <v>103</v>
-      </c>
-      <c r="E87"/>
+        <v>194</v>
+      </c>
+      <c r="E87" t="s">
+        <v>28</v>
+      </c>
       <c r="F87" t="s">
-        <v>104</v>
+        <v>195</v>
       </c>
       <c r="G87" t="s">
         <v>14</v>
       </c>
       <c r="H87" t="s">
+        <v>384</v>
+      </c>
+      <c r="I87" t="s">
         <v>385</v>
-      </c>
-      <c r="I87" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B88" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="C88" t="s">
         <v>11</v>
       </c>
       <c r="D88" t="s">
+        <v>387</v>
+      </c>
+      <c r="E88" t="s">
+        <v>179</v>
+      </c>
+      <c r="F88" t="s">
         <v>388</v>
-      </c>
-      <c r="E88" t="s">
-        <v>201</v>
-      </c>
-      <c r="F88" t="s">
-        <v>341</v>
       </c>
       <c r="G88" t="s">
         <v>14</v>
@@ -7105,133 +7178,133 @@
         <v>391</v>
       </c>
       <c r="B89" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
       <c r="C89" t="s">
         <v>11</v>
       </c>
       <c r="D89" t="s">
-        <v>187</v>
-      </c>
-      <c r="E89" t="s">
-        <v>28</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="E89"/>
       <c r="F89" t="s">
-        <v>188</v>
+        <v>104</v>
       </c>
       <c r="G89" t="s">
         <v>14</v>
       </c>
       <c r="H89" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="I89" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B90" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
       <c r="C90" t="s">
         <v>11</v>
       </c>
       <c r="D90" t="s">
-        <v>303</v>
+        <v>396</v>
       </c>
       <c r="E90" t="s">
-        <v>78</v>
+        <v>179</v>
       </c>
       <c r="F90" t="s">
-        <v>98</v>
+        <v>349</v>
       </c>
       <c r="G90" t="s">
         <v>14</v>
       </c>
       <c r="H90" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="I90" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B91" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
       <c r="C91" t="s">
         <v>11</v>
       </c>
       <c r="D91" t="s">
-        <v>126</v>
+        <v>194</v>
       </c>
       <c r="E91" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="F91" t="s">
-        <v>21</v>
+        <v>195</v>
       </c>
       <c r="G91" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H91" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="I91" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B92" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
       <c r="C92" t="s">
         <v>11</v>
       </c>
       <c r="D92" t="s">
-        <v>401</v>
+        <v>311</v>
       </c>
       <c r="E92" t="s">
-        <v>201</v>
+        <v>78</v>
       </c>
       <c r="F92" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="G92" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H92" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="I92" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B93" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
       <c r="C93" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D93" t="s">
-        <v>345</v>
-      </c>
-      <c r="E93"/>
+        <v>126</v>
+      </c>
+      <c r="E93" t="s">
+        <v>78</v>
+      </c>
       <c r="F93" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G93" t="s">
         <v>22</v>
@@ -7248,16 +7321,16 @@
         <v>408</v>
       </c>
       <c r="B94" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
       <c r="C94" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D94" t="s">
+        <v>409</v>
+      </c>
+      <c r="E94" t="s">
         <v>179</v>
-      </c>
-      <c r="E94" t="s">
-        <v>28</v>
       </c>
       <c r="F94" t="s">
         <v>117</v>
@@ -7266,60 +7339,60 @@
         <v>22</v>
       </c>
       <c r="H94" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="I94" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B95" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C95" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D95" t="s">
-        <v>103</v>
+        <v>353</v>
       </c>
       <c r="E95"/>
       <c r="F95" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
       <c r="G95" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H95" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="I95" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B96" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C96" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D96" t="s">
-        <v>134</v>
+        <v>186</v>
       </c>
       <c r="E96" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="F96" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="G96" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H96" t="s">
         <v>417</v>
@@ -7339,16 +7412,14 @@
         <v>11</v>
       </c>
       <c r="D97" t="s">
-        <v>126</v>
-      </c>
-      <c r="E97" t="s">
-        <v>78</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="E97"/>
       <c r="F97" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="G97" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H97" t="s">
         <v>421</v>
@@ -7365,14 +7436,16 @@
         <v>424</v>
       </c>
       <c r="C98" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D98" t="s">
-        <v>84</v>
-      </c>
-      <c r="E98"/>
+        <v>134</v>
+      </c>
+      <c r="E98" t="s">
+        <v>78</v>
+      </c>
       <c r="F98" t="s">
-        <v>13</v>
+        <v>104</v>
       </c>
       <c r="G98" t="s">
         <v>14</v>
@@ -7389,48 +7462,46 @@
         <v>427</v>
       </c>
       <c r="B99" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="C99" t="s">
         <v>11</v>
       </c>
       <c r="D99" t="s">
-        <v>401</v>
+        <v>126</v>
       </c>
       <c r="E99" t="s">
-        <v>201</v>
+        <v>78</v>
       </c>
       <c r="F99" t="s">
-        <v>117</v>
+        <v>21</v>
       </c>
       <c r="G99" t="s">
         <v>22</v>
       </c>
       <c r="H99" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I99" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B100" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C100" t="s">
         <v>19</v>
       </c>
       <c r="D100" t="s">
-        <v>432</v>
-      </c>
-      <c r="E100" t="s">
-        <v>341</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="E100"/>
       <c r="F100" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="G100" t="s">
         <v>14</v>
@@ -7447,49 +7518,51 @@
         <v>435</v>
       </c>
       <c r="B101" t="s">
+        <v>432</v>
+      </c>
+      <c r="C101" t="s">
+        <v>11</v>
+      </c>
+      <c r="D101" t="s">
+        <v>409</v>
+      </c>
+      <c r="E101" t="s">
+        <v>179</v>
+      </c>
+      <c r="F101" t="s">
+        <v>117</v>
+      </c>
+      <c r="G101" t="s">
+        <v>22</v>
+      </c>
+      <c r="H101" t="s">
         <v>436</v>
       </c>
-      <c r="C101" t="s">
-        <v>19</v>
-      </c>
-      <c r="D101" t="s">
+      <c r="I101" t="s">
         <v>437</v>
-      </c>
-      <c r="E101" t="s">
-        <v>341</v>
-      </c>
-      <c r="F101" t="s">
-        <v>29</v>
-      </c>
-      <c r="G101" t="s">
-        <v>14</v>
-      </c>
-      <c r="H101" t="s">
-        <v>438</v>
-      </c>
-      <c r="I101" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
+        <v>438</v>
+      </c>
+      <c r="B102" t="s">
+        <v>439</v>
+      </c>
+      <c r="C102" t="s">
+        <v>19</v>
+      </c>
+      <c r="D102" t="s">
         <v>440</v>
       </c>
-      <c r="B102" t="s">
-        <v>436</v>
-      </c>
-      <c r="C102" t="s">
-        <v>19</v>
-      </c>
-      <c r="D102" t="s">
-        <v>20</v>
-      </c>
-      <c r="E102"/>
+      <c r="E102" t="s">
+        <v>349</v>
+      </c>
       <c r="F102" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="G102" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H102" t="s">
         <v>441</v>
@@ -7503,76 +7576,76 @@
         <v>443</v>
       </c>
       <c r="B103" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
       <c r="C103" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D103" t="s">
-        <v>84</v>
-      </c>
-      <c r="E103"/>
+        <v>445</v>
+      </c>
+      <c r="E103" t="s">
+        <v>349</v>
+      </c>
       <c r="F103" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="G103" t="s">
         <v>14</v>
       </c>
       <c r="H103" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="I103" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B104" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C104" t="s">
         <v>19</v>
       </c>
       <c r="D104" t="s">
-        <v>345</v>
+        <v>20</v>
       </c>
       <c r="E104"/>
       <c r="F104" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G104" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H104" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="I104" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B105" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="C105" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D105" t="s">
-        <v>55</v>
-      </c>
-      <c r="E105" t="s">
-        <v>37</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="E105"/>
       <c r="F105" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="G105" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H105" t="s">
         <v>452</v>
@@ -7586,75 +7659,75 @@
         <v>454</v>
       </c>
       <c r="B106" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="C106" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D106" t="s">
-        <v>295</v>
-      </c>
-      <c r="E106" t="s">
-        <v>78</v>
-      </c>
+        <v>353</v>
+      </c>
+      <c r="E106"/>
       <c r="F106" t="s">
-        <v>188</v>
+        <v>29</v>
       </c>
       <c r="G106" t="s">
         <v>14</v>
       </c>
       <c r="H106" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="I106" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B107" t="s">
-        <v>451</v>
+        <v>459</v>
       </c>
       <c r="C107" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D107" t="s">
-        <v>20</v>
-      </c>
-      <c r="E107"/>
+        <v>55</v>
+      </c>
+      <c r="E107" t="s">
+        <v>37</v>
+      </c>
       <c r="F107" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G107" t="s">
         <v>22</v>
       </c>
       <c r="H107" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="I107" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="B108" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C108" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D108" t="s">
-        <v>462</v>
+        <v>303</v>
       </c>
       <c r="E108" t="s">
-        <v>341</v>
+        <v>78</v>
       </c>
       <c r="F108" t="s">
-        <v>43</v>
+        <v>195</v>
       </c>
       <c r="G108" t="s">
         <v>14</v>
@@ -7671,225 +7744,223 @@
         <v>465</v>
       </c>
       <c r="B109" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="C109" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D109" t="s">
-        <v>467</v>
-      </c>
-      <c r="E109" t="s">
-        <v>201</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E109"/>
       <c r="F109" t="s">
-        <v>468</v>
+        <v>21</v>
       </c>
       <c r="G109" t="s">
         <v>22</v>
       </c>
       <c r="H109" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="I109" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
+        <v>468</v>
+      </c>
+      <c r="B110" t="s">
+        <v>469</v>
+      </c>
+      <c r="C110" t="s">
+        <v>19</v>
+      </c>
+      <c r="D110" t="s">
+        <v>470</v>
+      </c>
+      <c r="E110" t="s">
+        <v>349</v>
+      </c>
+      <c r="F110" t="s">
+        <v>43</v>
+      </c>
+      <c r="G110" t="s">
+        <v>14</v>
+      </c>
+      <c r="H110" t="s">
         <v>471</v>
       </c>
-      <c r="B110" t="s">
+      <c r="I110" t="s">
         <v>472</v>
-      </c>
-      <c r="C110" t="s">
-        <v>11</v>
-      </c>
-      <c r="D110" t="s">
-        <v>187</v>
-      </c>
-      <c r="E110" t="s">
-        <v>28</v>
-      </c>
-      <c r="F110" t="s">
-        <v>188</v>
-      </c>
-      <c r="G110" t="s">
-        <v>14</v>
-      </c>
-      <c r="H110" t="s">
-        <v>473</v>
-      </c>
-      <c r="I110" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
+        <v>473</v>
+      </c>
+      <c r="B111" t="s">
+        <v>474</v>
+      </c>
+      <c r="C111" t="s">
+        <v>19</v>
+      </c>
+      <c r="D111" t="s">
         <v>475</v>
       </c>
-      <c r="B111" t="s">
+      <c r="E111" t="s">
+        <v>179</v>
+      </c>
+      <c r="F111" t="s">
         <v>476</v>
       </c>
-      <c r="C111" t="s">
-        <v>19</v>
-      </c>
-      <c r="D111" t="s">
+      <c r="G111" t="s">
+        <v>22</v>
+      </c>
+      <c r="H111" t="s">
         <v>477</v>
       </c>
-      <c r="E111" t="s">
-        <v>11</v>
-      </c>
-      <c r="F111" t="s">
-        <v>29</v>
-      </c>
-      <c r="G111" t="s">
-        <v>14</v>
-      </c>
-      <c r="H111" t="s">
+      <c r="I111" t="s">
         <v>478</v>
-      </c>
-      <c r="I111" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
+        <v>479</v>
+      </c>
+      <c r="B112" t="s">
         <v>480</v>
       </c>
-      <c r="B112" t="s">
-        <v>476</v>
-      </c>
       <c r="C112" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D112" t="s">
+        <v>194</v>
+      </c>
+      <c r="E112" t="s">
+        <v>28</v>
+      </c>
+      <c r="F112" t="s">
+        <v>195</v>
+      </c>
+      <c r="G112" t="s">
+        <v>14</v>
+      </c>
+      <c r="H112" t="s">
         <v>481</v>
       </c>
-      <c r="E112" t="s">
-        <v>201</v>
-      </c>
-      <c r="F112" t="s">
-        <v>163</v>
-      </c>
-      <c r="G112" t="s">
-        <v>14</v>
-      </c>
-      <c r="H112" t="s">
+      <c r="I112" t="s">
         <v>482</v>
-      </c>
-      <c r="I112" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
+        <v>483</v>
+      </c>
+      <c r="B113" t="s">
         <v>484</v>
       </c>
-      <c r="B113" t="s">
-        <v>476</v>
-      </c>
       <c r="C113" t="s">
         <v>19</v>
       </c>
       <c r="D113" t="s">
-        <v>168</v>
+        <v>485</v>
       </c>
       <c r="E113" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="F113" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="G113" t="s">
         <v>14</v>
       </c>
       <c r="H113" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="I113" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B114" t="s">
-        <v>476</v>
+        <v>484</v>
       </c>
       <c r="C114" t="s">
         <v>19</v>
       </c>
       <c r="D114" t="s">
-        <v>477</v>
+        <v>489</v>
       </c>
       <c r="E114" t="s">
-        <v>11</v>
+        <v>179</v>
       </c>
       <c r="F114" t="s">
-        <v>29</v>
+        <v>163</v>
       </c>
       <c r="G114" t="s">
         <v>14</v>
       </c>
       <c r="H114" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="I114" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="B115" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="C115" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D115" t="s">
-        <v>206</v>
+        <v>168</v>
       </c>
       <c r="E115" t="s">
-        <v>201</v>
+        <v>37</v>
       </c>
       <c r="F115" t="s">
-        <v>207</v>
+        <v>79</v>
       </c>
       <c r="G115" t="s">
         <v>14</v>
       </c>
       <c r="H115" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="I115" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B116" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="C116" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D116" t="s">
-        <v>495</v>
+        <v>485</v>
       </c>
       <c r="E116" t="s">
         <v>11</v>
       </c>
       <c r="F116" t="s">
-        <v>468</v>
+        <v>29</v>
       </c>
       <c r="G116" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H116" t="s">
         <v>496</v>
@@ -7903,20 +7974,22 @@
         <v>498</v>
       </c>
       <c r="B117" t="s">
+        <v>484</v>
+      </c>
+      <c r="C117" t="s">
+        <v>19</v>
+      </c>
+      <c r="D117" t="s">
         <v>499</v>
       </c>
-      <c r="C117" t="s">
-        <v>19</v>
-      </c>
-      <c r="D117" t="s">
-        <v>154</v>
-      </c>
-      <c r="E117"/>
+      <c r="E117" t="s">
+        <v>179</v>
+      </c>
       <c r="F117" t="s">
-        <v>29</v>
+        <v>228</v>
       </c>
       <c r="G117" t="s">
-        <v>14</v>
+        <v>181</v>
       </c>
       <c r="H117" t="s">
         <v>500</v>
@@ -7930,104 +8003,102 @@
         <v>502</v>
       </c>
       <c r="B118" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="C118" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D118" t="s">
-        <v>154</v>
-      </c>
-      <c r="E118"/>
+        <v>212</v>
+      </c>
+      <c r="E118" t="s">
+        <v>179</v>
+      </c>
       <c r="F118" t="s">
-        <v>29</v>
+        <v>213</v>
       </c>
       <c r="G118" t="s">
         <v>14</v>
       </c>
       <c r="H118" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="I118" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B119" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="C119" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D119" t="s">
-        <v>200</v>
+        <v>507</v>
       </c>
       <c r="E119" t="s">
-        <v>201</v>
+        <v>11</v>
       </c>
       <c r="F119" t="s">
-        <v>117</v>
+        <v>476</v>
       </c>
       <c r="G119" t="s">
         <v>22</v>
       </c>
       <c r="H119" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="I119" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B120" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="C120" t="s">
         <v>19</v>
       </c>
       <c r="D120" t="s">
-        <v>510</v>
-      </c>
-      <c r="E120" t="s">
-        <v>37</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="E120"/>
       <c r="F120" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
       <c r="G120" t="s">
         <v>14</v>
       </c>
       <c r="H120" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="I120" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B121" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="C121" t="s">
         <v>19</v>
       </c>
       <c r="D121" t="s">
-        <v>514</v>
-      </c>
-      <c r="E121" t="s">
-        <v>28</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="E121"/>
       <c r="F121" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="G121" t="s">
         <v>14</v>
@@ -8044,36 +8115,36 @@
         <v>517</v>
       </c>
       <c r="B122" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="C122" t="s">
         <v>19</v>
       </c>
       <c r="D122" t="s">
+        <v>207</v>
+      </c>
+      <c r="E122" t="s">
+        <v>179</v>
+      </c>
+      <c r="F122" t="s">
+        <v>117</v>
+      </c>
+      <c r="G122" t="s">
+        <v>22</v>
+      </c>
+      <c r="H122" t="s">
         <v>518</v>
       </c>
-      <c r="E122" t="s">
-        <v>11</v>
-      </c>
-      <c r="F122" t="s">
-        <v>73</v>
-      </c>
-      <c r="G122" t="s">
-        <v>14</v>
-      </c>
-      <c r="H122" t="s">
+      <c r="I122" t="s">
         <v>519</v>
-      </c>
-      <c r="I122" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
+        <v>520</v>
+      </c>
+      <c r="B123" t="s">
         <v>521</v>
-      </c>
-      <c r="B123" t="s">
-        <v>509</v>
       </c>
       <c r="C123" t="s">
         <v>19</v>
@@ -8082,13 +8153,13 @@
         <v>522</v>
       </c>
       <c r="E123" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="F123" t="s">
-        <v>48</v>
+        <v>104</v>
       </c>
       <c r="G123" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H123" t="s">
         <v>523</v>
@@ -8102,440 +8173,440 @@
         <v>525</v>
       </c>
       <c r="B124" t="s">
+        <v>521</v>
+      </c>
+      <c r="C124" t="s">
+        <v>19</v>
+      </c>
+      <c r="D124" t="s">
         <v>526</v>
       </c>
-      <c r="C124" t="s">
-        <v>19</v>
-      </c>
-      <c r="D124" t="s">
+      <c r="E124" t="s">
+        <v>28</v>
+      </c>
+      <c r="F124" t="s">
+        <v>73</v>
+      </c>
+      <c r="G124" t="s">
+        <v>14</v>
+      </c>
+      <c r="H124" t="s">
         <v>527</v>
       </c>
-      <c r="E124" t="s">
-        <v>37</v>
-      </c>
-      <c r="F124" t="s">
-        <v>43</v>
-      </c>
-      <c r="G124" t="s">
-        <v>14</v>
-      </c>
-      <c r="H124" t="s">
+      <c r="I124" t="s">
         <v>528</v>
-      </c>
-      <c r="I124" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
+        <v>529</v>
+      </c>
+      <c r="B125" t="s">
+        <v>521</v>
+      </c>
+      <c r="C125" t="s">
+        <v>19</v>
+      </c>
+      <c r="D125" t="s">
         <v>530</v>
-      </c>
-      <c r="B125" t="s">
-        <v>531</v>
-      </c>
-      <c r="C125" t="s">
-        <v>19</v>
-      </c>
-      <c r="D125" t="s">
-        <v>532</v>
       </c>
       <c r="E125" t="s">
         <v>11</v>
       </c>
       <c r="F125" t="s">
-        <v>468</v>
+        <v>73</v>
       </c>
       <c r="G125" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H125" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="I125" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B126" t="s">
-        <v>536</v>
+        <v>521</v>
       </c>
       <c r="C126" t="s">
         <v>19</v>
       </c>
       <c r="D126" t="s">
-        <v>345</v>
-      </c>
-      <c r="E126"/>
+        <v>534</v>
+      </c>
+      <c r="E126" t="s">
+        <v>11</v>
+      </c>
       <c r="F126" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="G126" t="s">
         <v>22</v>
       </c>
       <c r="H126" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="I126" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
+        <v>537</v>
+      </c>
+      <c r="B127" t="s">
+        <v>538</v>
+      </c>
+      <c r="C127" t="s">
+        <v>19</v>
+      </c>
+      <c r="D127" t="s">
         <v>539</v>
       </c>
-      <c r="B127" t="s">
+      <c r="E127" t="s">
+        <v>37</v>
+      </c>
+      <c r="F127" t="s">
+        <v>43</v>
+      </c>
+      <c r="G127" t="s">
+        <v>14</v>
+      </c>
+      <c r="H127" t="s">
         <v>540</v>
       </c>
-      <c r="C127" t="s">
-        <v>19</v>
-      </c>
-      <c r="D127" t="s">
-        <v>84</v>
-      </c>
-      <c r="E127"/>
-      <c r="F127" t="s">
-        <v>13</v>
-      </c>
-      <c r="G127" t="s">
-        <v>14</v>
-      </c>
-      <c r="H127" t="s">
+      <c r="I127" t="s">
         <v>541</v>
-      </c>
-      <c r="I127" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
+        <v>542</v>
+      </c>
+      <c r="B128" t="s">
         <v>543</v>
       </c>
-      <c r="B128" t="s">
-        <v>540</v>
-      </c>
       <c r="C128" t="s">
         <v>19</v>
       </c>
       <c r="D128" t="s">
-        <v>84</v>
-      </c>
-      <c r="E128"/>
+        <v>544</v>
+      </c>
+      <c r="E128" t="s">
+        <v>11</v>
+      </c>
       <c r="F128" t="s">
-        <v>13</v>
+        <v>476</v>
       </c>
       <c r="G128" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H128" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I128" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B129" t="s">
-        <v>540</v>
+        <v>548</v>
       </c>
       <c r="C129" t="s">
         <v>19</v>
       </c>
       <c r="D129" t="s">
-        <v>547</v>
-      </c>
-      <c r="E129" t="s">
-        <v>28</v>
-      </c>
+        <v>353</v>
+      </c>
+      <c r="E129"/>
       <c r="F129" t="s">
-        <v>308</v>
+        <v>29</v>
       </c>
       <c r="G129" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H129" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="I129" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="B130" t="s">
-        <v>540</v>
+        <v>552</v>
       </c>
       <c r="C130" t="s">
         <v>19</v>
       </c>
       <c r="D130" t="s">
-        <v>550</v>
-      </c>
-      <c r="E130" t="s">
-        <v>11</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="E130"/>
       <c r="F130" t="s">
-        <v>308</v>
+        <v>13</v>
       </c>
       <c r="G130" t="s">
         <v>14</v>
       </c>
       <c r="H130" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="I130" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="B131" t="s">
-        <v>540</v>
+        <v>552</v>
       </c>
       <c r="C131" t="s">
         <v>19</v>
       </c>
       <c r="D131" t="s">
-        <v>547</v>
-      </c>
-      <c r="E131" t="s">
-        <v>28</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="E131"/>
       <c r="F131" t="s">
-        <v>308</v>
+        <v>13</v>
       </c>
       <c r="G131" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H131" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="I131" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="B132" t="s">
-        <v>540</v>
+        <v>552</v>
       </c>
       <c r="C132" t="s">
         <v>19</v>
       </c>
       <c r="D132" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="E132" t="s">
         <v>28</v>
       </c>
       <c r="F132" t="s">
-        <v>117</v>
+        <v>316</v>
       </c>
       <c r="G132" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H132" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="I132" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="B133" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="C133" t="s">
+        <v>19</v>
+      </c>
+      <c r="D133" t="s">
+        <v>562</v>
+      </c>
+      <c r="E133" t="s">
         <v>11</v>
       </c>
-      <c r="D133" t="s">
-        <v>217</v>
-      </c>
-      <c r="E133" t="s">
-        <v>78</v>
-      </c>
       <c r="F133" t="s">
-        <v>218</v>
+        <v>316</v>
       </c>
       <c r="G133" t="s">
         <v>14</v>
       </c>
       <c r="H133" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="I133" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="B134" t="s">
+        <v>552</v>
+      </c>
+      <c r="C134" t="s">
+        <v>19</v>
+      </c>
+      <c r="D134" t="s">
         <v>559</v>
       </c>
-      <c r="C134" t="s">
-        <v>11</v>
-      </c>
-      <c r="D134" t="s">
-        <v>20</v>
-      </c>
-      <c r="E134"/>
+      <c r="E134" t="s">
+        <v>28</v>
+      </c>
       <c r="F134" t="s">
-        <v>21</v>
+        <v>316</v>
       </c>
       <c r="G134" t="s">
         <v>22</v>
       </c>
       <c r="H134" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="I134" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="B135" t="s">
-        <v>566</v>
+        <v>552</v>
       </c>
       <c r="C135" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D135" t="s">
-        <v>495</v>
+        <v>568</v>
       </c>
       <c r="E135" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F135" t="s">
-        <v>468</v>
+        <v>117</v>
       </c>
       <c r="G135" t="s">
         <v>22</v>
       </c>
       <c r="H135" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="I135" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B136" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C136" t="s">
         <v>11</v>
       </c>
       <c r="D136" t="s">
-        <v>303</v>
+        <v>223</v>
       </c>
       <c r="E136" t="s">
         <v>78</v>
       </c>
       <c r="F136" t="s">
-        <v>98</v>
+        <v>180</v>
       </c>
       <c r="G136" t="s">
         <v>14</v>
       </c>
       <c r="H136" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="I136" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B137" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C137" t="s">
         <v>11</v>
       </c>
       <c r="D137" t="s">
-        <v>212</v>
-      </c>
-      <c r="E137" t="s">
-        <v>78</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E137"/>
       <c r="F137" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="G137" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H137" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="I137" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B138" t="s">
-        <v>570</v>
+        <v>578</v>
       </c>
       <c r="C138" t="s">
         <v>11</v>
       </c>
       <c r="D138" t="s">
-        <v>577</v>
+        <v>507</v>
       </c>
       <c r="E138" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="F138" t="s">
-        <v>341</v>
+        <v>476</v>
       </c>
       <c r="G138" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H138" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="I138" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B139" t="s">
-        <v>570</v>
+        <v>582</v>
       </c>
       <c r="C139" t="s">
         <v>11</v>
       </c>
       <c r="D139" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="E139" t="s">
         <v>78</v>
@@ -8547,485 +8618,491 @@
         <v>14</v>
       </c>
       <c r="H139" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="I139" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="B140" t="s">
-        <v>570</v>
+        <v>582</v>
       </c>
       <c r="C140" t="s">
         <v>11</v>
       </c>
       <c r="D140" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E140" t="s">
         <v>78</v>
       </c>
       <c r="F140" t="s">
-        <v>218</v>
+        <v>73</v>
       </c>
       <c r="G140" t="s">
         <v>14</v>
       </c>
       <c r="H140" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="I140" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="B141" t="s">
-        <v>570</v>
+        <v>582</v>
       </c>
       <c r="C141" t="s">
         <v>11</v>
       </c>
       <c r="D141" t="s">
-        <v>217</v>
+        <v>589</v>
       </c>
       <c r="E141" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="F141" t="s">
-        <v>218</v>
+        <v>349</v>
       </c>
       <c r="G141" t="s">
         <v>14</v>
       </c>
       <c r="H141" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="I141" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="B142" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="C142" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D142" t="s">
-        <v>103</v>
-      </c>
-      <c r="E142"/>
+        <v>311</v>
+      </c>
+      <c r="E142" t="s">
+        <v>78</v>
+      </c>
       <c r="F142" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G142" t="s">
         <v>14</v>
       </c>
       <c r="H142" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="I142" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="B143" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="C143" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D143" t="s">
-        <v>594</v>
+        <v>223</v>
       </c>
       <c r="E143" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="F143" t="s">
-        <v>251</v>
+        <v>180</v>
       </c>
       <c r="G143" t="s">
         <v>14</v>
       </c>
       <c r="H143" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="I143" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B144" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="C144" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D144" t="s">
-        <v>36</v>
+        <v>223</v>
       </c>
       <c r="E144" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="F144" t="s">
-        <v>22</v>
+        <v>180</v>
       </c>
       <c r="G144" t="s">
         <v>14</v>
       </c>
       <c r="H144" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="I144" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="B145" t="s">
-        <v>590</v>
+        <v>602</v>
       </c>
       <c r="C145" t="s">
         <v>19</v>
       </c>
       <c r="D145" t="s">
-        <v>601</v>
-      </c>
-      <c r="E145" t="s">
-        <v>28</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="E145"/>
       <c r="F145" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
       <c r="G145" t="s">
         <v>14</v>
       </c>
       <c r="H145" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="I145" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="B146" t="s">
-        <v>590</v>
+        <v>602</v>
       </c>
       <c r="C146" t="s">
         <v>19</v>
       </c>
       <c r="D146" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="E146" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="F146" t="s">
-        <v>43</v>
+        <v>260</v>
       </c>
       <c r="G146" t="s">
         <v>14</v>
       </c>
       <c r="H146" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="I146" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="B147" t="s">
-        <v>590</v>
+        <v>602</v>
       </c>
       <c r="C147" t="s">
         <v>19</v>
       </c>
       <c r="D147" t="s">
-        <v>103</v>
-      </c>
-      <c r="E147"/>
+        <v>36</v>
+      </c>
+      <c r="E147" t="s">
+        <v>37</v>
+      </c>
       <c r="F147" t="s">
-        <v>104</v>
+        <v>22</v>
       </c>
       <c r="G147" t="s">
         <v>14</v>
       </c>
       <c r="H147" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="I147" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="B148" t="s">
-        <v>611</v>
+        <v>602</v>
       </c>
       <c r="C148" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D148" t="s">
-        <v>291</v>
+        <v>613</v>
       </c>
       <c r="E148" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="F148" t="s">
-        <v>163</v>
+        <v>43</v>
       </c>
       <c r="G148" t="s">
         <v>14</v>
       </c>
       <c r="H148" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="I148" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B149" t="s">
-        <v>611</v>
+        <v>602</v>
       </c>
       <c r="C149" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D149" t="s">
-        <v>303</v>
+        <v>616</v>
       </c>
       <c r="E149" t="s">
         <v>78</v>
       </c>
       <c r="F149" t="s">
-        <v>98</v>
+        <v>43</v>
       </c>
       <c r="G149" t="s">
         <v>14</v>
       </c>
       <c r="H149" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="I149" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="B150" t="s">
-        <v>611</v>
+        <v>602</v>
       </c>
       <c r="C150" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D150" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="E150"/>
       <c r="F150" t="s">
-        <v>13</v>
+        <v>104</v>
       </c>
       <c r="G150" t="s">
         <v>14</v>
       </c>
       <c r="H150" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="I150" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="B151" t="s">
-        <v>611</v>
+        <v>623</v>
       </c>
       <c r="C151" t="s">
         <v>11</v>
       </c>
       <c r="D151" t="s">
-        <v>206</v>
+        <v>299</v>
       </c>
       <c r="E151" t="s">
-        <v>201</v>
+        <v>78</v>
       </c>
       <c r="F151" t="s">
-        <v>207</v>
+        <v>163</v>
       </c>
       <c r="G151" t="s">
         <v>14</v>
       </c>
       <c r="H151" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="I151" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="s">
+        <v>626</v>
+      </c>
+      <c r="B152" t="s">
         <v>623</v>
-      </c>
-      <c r="B152" t="s">
-        <v>611</v>
       </c>
       <c r="C152" t="s">
         <v>11</v>
       </c>
       <c r="D152" t="s">
-        <v>126</v>
+        <v>311</v>
       </c>
       <c r="E152" t="s">
         <v>78</v>
       </c>
       <c r="F152" t="s">
-        <v>21</v>
+        <v>98</v>
       </c>
       <c r="G152" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H152" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="I152" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="B153" t="s">
-        <v>611</v>
+        <v>623</v>
       </c>
       <c r="C153" t="s">
         <v>11</v>
       </c>
       <c r="D153" t="s">
-        <v>495</v>
-      </c>
-      <c r="E153" t="s">
-        <v>11</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="E153"/>
       <c r="F153" t="s">
-        <v>468</v>
+        <v>13</v>
       </c>
       <c r="G153" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H153" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="I153" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="B154" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
       <c r="C154" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D154" t="s">
-        <v>352</v>
-      </c>
-      <c r="E154"/>
+        <v>212</v>
+      </c>
+      <c r="E154" t="s">
+        <v>179</v>
+      </c>
       <c r="F154" t="s">
-        <v>117</v>
+        <v>213</v>
       </c>
       <c r="G154" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H154" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="I154" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="B155" t="s">
-        <v>634</v>
+        <v>623</v>
       </c>
       <c r="C155" t="s">
         <v>11</v>
       </c>
       <c r="D155" t="s">
-        <v>103</v>
-      </c>
-      <c r="E155"/>
+        <v>126</v>
+      </c>
+      <c r="E155" t="s">
+        <v>78</v>
+      </c>
       <c r="F155" t="s">
-        <v>104</v>
+        <v>21</v>
       </c>
       <c r="G155" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H155" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="I155" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B156" t="s">
-        <v>638</v>
+        <v>623</v>
       </c>
       <c r="C156" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D156" t="s">
-        <v>345</v>
-      </c>
-      <c r="E156"/>
+        <v>507</v>
+      </c>
+      <c r="E156" t="s">
+        <v>11</v>
+      </c>
       <c r="F156" t="s">
-        <v>29</v>
+        <v>476</v>
       </c>
       <c r="G156" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H156" t="s">
         <v>639</v>
@@ -9039,36 +9116,34 @@
         <v>641</v>
       </c>
       <c r="B157" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="C157" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D157" t="s">
-        <v>187</v>
-      </c>
-      <c r="E157" t="s">
-        <v>28</v>
-      </c>
+        <v>360</v>
+      </c>
+      <c r="E157"/>
       <c r="F157" t="s">
-        <v>188</v>
+        <v>117</v>
       </c>
       <c r="G157" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H157" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="I157" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B158" t="s">
-        <v>638</v>
+        <v>646</v>
       </c>
       <c r="C158" t="s">
         <v>11</v>
@@ -9084,59 +9159,57 @@
         <v>14</v>
       </c>
       <c r="H158" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="I158" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="B159" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="C159" t="s">
         <v>19</v>
       </c>
       <c r="D159" t="s">
-        <v>649</v>
-      </c>
-      <c r="E159" t="s">
-        <v>37</v>
-      </c>
+        <v>353</v>
+      </c>
+      <c r="E159"/>
       <c r="F159" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="G159" t="s">
         <v>14</v>
       </c>
       <c r="H159" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="I159" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B160" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="C160" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D160" t="s">
-        <v>653</v>
+        <v>194</v>
       </c>
       <c r="E160" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F160" t="s">
-        <v>43</v>
+        <v>195</v>
       </c>
       <c r="G160" t="s">
         <v>14</v>
@@ -9153,17 +9226,15 @@
         <v>656</v>
       </c>
       <c r="B161" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="C161" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D161" t="s">
-        <v>657</v>
-      </c>
-      <c r="E161" t="s">
-        <v>28</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="E161"/>
       <c r="F161" t="s">
         <v>104</v>
       </c>
@@ -9171,10 +9242,97 @@
         <v>14</v>
       </c>
       <c r="H161" t="s">
+        <v>657</v>
+      </c>
+      <c r="I161" t="s">
         <v>658</v>
       </c>
-      <c r="I161" t="s">
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
         <v>659</v>
+      </c>
+      <c r="B162" t="s">
+        <v>660</v>
+      </c>
+      <c r="C162" t="s">
+        <v>19</v>
+      </c>
+      <c r="D162" t="s">
+        <v>661</v>
+      </c>
+      <c r="E162" t="s">
+        <v>37</v>
+      </c>
+      <c r="F162" t="s">
+        <v>43</v>
+      </c>
+      <c r="G162" t="s">
+        <v>14</v>
+      </c>
+      <c r="H162" t="s">
+        <v>662</v>
+      </c>
+      <c r="I162" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s">
+        <v>664</v>
+      </c>
+      <c r="B163" t="s">
+        <v>660</v>
+      </c>
+      <c r="C163" t="s">
+        <v>19</v>
+      </c>
+      <c r="D163" t="s">
+        <v>665</v>
+      </c>
+      <c r="E163" t="s">
+        <v>11</v>
+      </c>
+      <c r="F163" t="s">
+        <v>43</v>
+      </c>
+      <c r="G163" t="s">
+        <v>14</v>
+      </c>
+      <c r="H163" t="s">
+        <v>666</v>
+      </c>
+      <c r="I163" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s">
+        <v>668</v>
+      </c>
+      <c r="B164" t="s">
+        <v>660</v>
+      </c>
+      <c r="C164" t="s">
+        <v>19</v>
+      </c>
+      <c r="D164" t="s">
+        <v>669</v>
+      </c>
+      <c r="E164" t="s">
+        <v>28</v>
+      </c>
+      <c r="F164" t="s">
+        <v>104</v>
+      </c>
+      <c r="G164" t="s">
+        <v>14</v>
+      </c>
+      <c r="H164" t="s">
+        <v>670</v>
+      </c>
+      <c r="I164" t="s">
+        <v>671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>